<commit_message>
Updated the template with an additional test case
</commit_message>
<xml_diff>
--- a/AutoTester/Tests/System/System Testing Template.xlsx
+++ b/AutoTester/Tests/System/System Testing Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni Files\Y3Sem1\CS3201 &amp; CS3202\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni Files\Y3Sem1\CS3201 &amp; CS3202\SPA Project Folder\AutoTester\Tests\System\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26439" uniqueCount="458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26494" uniqueCount="460">
   <si>
     <t>such that</t>
   </si>
@@ -1399,6 +1399,12 @@
   <si>
     <t>Such That Pattern Validity Cases</t>
   </si>
+  <si>
+    <t>pl.prog_line#=2</t>
+  </si>
+  <si>
+    <t>ifs.prog_line#=10</t>
+  </si>
 </sst>
 </file>
 
@@ -1582,7 +1588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1617,25 +1623,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1647,28 +1638,34 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1985,10 +1982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1C4663-D304-44C8-B0BF-D228A95395FB}">
-  <dimension ref="B3:AY687"/>
+  <dimension ref="B3:AY688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A563" workbookViewId="0">
-      <selection activeCell="AA583" sqref="AA583"/>
+    <sheetView tabSelected="1" topLeftCell="C570" workbookViewId="0">
+      <selection activeCell="C590" sqref="C590"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -78704,7 +78701,7 @@
       <c r="B562" s="6">
         <v>558</v>
       </c>
-      <c r="C562" s="6" t="s">
+      <c r="C562" s="2" t="s">
         <v>115</v>
       </c>
       <c r="D562" s="7" t="s">
@@ -78722,13 +78719,13 @@
       <c r="H562" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I562" s="13" t="s">
+      <c r="I562" s="12" t="s">
         <v>447</v>
       </c>
       <c r="J562" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K562" s="29" t="s">
+      <c r="K562" s="13" t="s">
         <v>166</v>
       </c>
       <c r="L562" s="2" t="s">
@@ -78843,9 +78840,7 @@
       <c r="B563" s="6">
         <v>559</v>
       </c>
-      <c r="C563" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C563" s="2"/>
       <c r="D563" s="7" t="s">
         <v>44</v>
       </c>
@@ -78864,10 +78859,10 @@
       <c r="I563" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J563" s="13" t="s">
+      <c r="J563" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="K563" s="29"/>
+      <c r="K563" s="13"/>
       <c r="L563" s="2"/>
       <c r="M563" s="2"/>
       <c r="N563" s="7" t="s">
@@ -78976,9 +78971,7 @@
       <c r="B564" s="6">
         <v>560</v>
       </c>
-      <c r="C564" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C564" s="2"/>
       <c r="D564" s="7" t="s">
         <v>44</v>
       </c>
@@ -78997,10 +78990,10 @@
       <c r="I564" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="J564" s="13" t="s">
+      <c r="J564" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="K564" s="29"/>
+      <c r="K564" s="13"/>
       <c r="L564" s="2"/>
       <c r="M564" s="2"/>
       <c r="N564" s="7" t="s">
@@ -79109,9 +79102,7 @@
       <c r="B565" s="6">
         <v>561</v>
       </c>
-      <c r="C565" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C565" s="2"/>
       <c r="D565" s="7" t="s">
         <v>44</v>
       </c>
@@ -79130,10 +79121,10 @@
       <c r="I565" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J565" s="13" t="s">
+      <c r="J565" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="K565" s="29"/>
+      <c r="K565" s="13"/>
       <c r="L565" s="2"/>
       <c r="M565" s="2"/>
       <c r="N565" s="7" t="s">
@@ -79242,9 +79233,7 @@
       <c r="B566" s="6">
         <v>562</v>
       </c>
-      <c r="C566" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C566" s="2"/>
       <c r="D566" s="7" t="s">
         <v>44</v>
       </c>
@@ -79260,13 +79249,13 @@
       <c r="H566" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I566" s="13" t="s">
+      <c r="I566" s="12" t="s">
         <v>447</v>
       </c>
       <c r="J566" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K566" s="29"/>
+      <c r="K566" s="13"/>
       <c r="L566" s="2"/>
       <c r="M566" s="2"/>
       <c r="N566" s="7" t="s">
@@ -79375,9 +79364,7 @@
       <c r="B567" s="6">
         <v>563</v>
       </c>
-      <c r="C567" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C567" s="2"/>
       <c r="D567" s="7" t="s">
         <v>44</v>
       </c>
@@ -79396,13 +79383,13 @@
       <c r="I567" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="J567" s="19" t="s">
+      <c r="J567" s="14" t="s">
         <v>434</v>
       </c>
       <c r="K567" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L567" s="19" t="s">
+      <c r="L567" s="14" t="s">
         <v>436</v>
       </c>
       <c r="M567" s="2"/>
@@ -79512,9 +79499,7 @@
       <c r="B568" s="6">
         <v>564</v>
       </c>
-      <c r="C568" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C568" s="2"/>
       <c r="D568" s="7" t="s">
         <v>44</v>
       </c>
@@ -79533,10 +79518,10 @@
       <c r="I568" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J568" s="13" t="s">
+      <c r="J568" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="K568" s="29" t="s">
+      <c r="K568" s="13" t="s">
         <v>166</v>
       </c>
       <c r="L568" s="2" t="s">
@@ -79649,9 +79634,7 @@
       <c r="B569" s="6">
         <v>565</v>
       </c>
-      <c r="C569" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C569" s="2"/>
       <c r="D569" s="7" t="s">
         <v>44</v>
       </c>
@@ -79667,13 +79650,13 @@
       <c r="H569" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I569" s="13" t="s">
+      <c r="I569" s="12" t="s">
         <v>447</v>
       </c>
       <c r="J569" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K569" s="29"/>
+      <c r="K569" s="13"/>
       <c r="L569" s="2"/>
       <c r="M569" s="2"/>
       <c r="N569" s="7" t="s">
@@ -79782,9 +79765,7 @@
       <c r="B570" s="6">
         <v>566</v>
       </c>
-      <c r="C570" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C570" s="2"/>
       <c r="D570" s="7" t="s">
         <v>44</v>
       </c>
@@ -79800,13 +79781,13 @@
       <c r="H570" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I570" s="13" t="s">
+      <c r="I570" s="12" t="s">
         <v>447</v>
       </c>
       <c r="J570" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K570" s="29"/>
+      <c r="K570" s="13"/>
       <c r="L570" s="2"/>
       <c r="M570" s="2"/>
       <c r="N570" s="7" t="s">
@@ -79915,9 +79896,7 @@
       <c r="B571" s="6">
         <v>567</v>
       </c>
-      <c r="C571" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C571" s="2"/>
       <c r="D571" s="7" t="s">
         <v>44</v>
       </c>
@@ -79936,10 +79915,10 @@
       <c r="I571" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J571" s="13" t="s">
+      <c r="J571" s="12" t="s">
         <v>447</v>
       </c>
-      <c r="K571" s="29"/>
+      <c r="K571" s="13"/>
       <c r="L571" s="2"/>
       <c r="M571" s="2"/>
       <c r="N571" s="7" t="s">
@@ -80048,9 +80027,7 @@
       <c r="B572" s="6">
         <v>568</v>
       </c>
-      <c r="C572" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C572" s="2"/>
       <c r="D572" s="7" t="s">
         <v>44</v>
       </c>
@@ -80066,13 +80043,13 @@
       <c r="H572" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I572" s="20" t="s">
+      <c r="I572" s="15" t="s">
         <v>438</v>
       </c>
       <c r="J572" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K572" s="20" t="s">
+      <c r="K572" s="15" t="s">
         <v>167</v>
       </c>
       <c r="L572" s="2"/>
@@ -80185,9 +80162,7 @@
       <c r="B573" s="6">
         <v>569</v>
       </c>
-      <c r="C573" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C573" s="2"/>
       <c r="D573" s="7" t="s">
         <v>44</v>
       </c>
@@ -80206,10 +80181,10 @@
       <c r="I573" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J573" s="21" t="s">
+      <c r="J573" s="16" t="s">
         <v>437</v>
       </c>
-      <c r="K573" s="21" t="s">
+      <c r="K573" s="16" t="s">
         <v>168</v>
       </c>
       <c r="L573" s="2"/>
@@ -80320,9 +80295,7 @@
       <c r="B574" s="6">
         <v>570</v>
       </c>
-      <c r="C574" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C574" s="2"/>
       <c r="D574" s="7" t="s">
         <v>44</v>
       </c>
@@ -80338,7 +80311,7 @@
       <c r="H574" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I574" s="16" t="s">
+      <c r="I574" s="17" t="s">
         <v>432</v>
       </c>
       <c r="J574" s="6" t="s">
@@ -80459,9 +80432,7 @@
       <c r="B575" s="6">
         <v>571</v>
       </c>
-      <c r="C575" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C575" s="2"/>
       <c r="D575" s="7" t="s">
         <v>44</v>
       </c>
@@ -80480,7 +80451,7 @@
       <c r="I575" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J575" s="16" t="s">
+      <c r="J575" s="17" t="s">
         <v>432</v>
       </c>
       <c r="K575" s="7" t="s">
@@ -80596,9 +80567,7 @@
       <c r="B576" s="6">
         <v>572</v>
       </c>
-      <c r="C576" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C576" s="2"/>
       <c r="D576" s="7" t="s">
         <v>44</v>
       </c>
@@ -80629,7 +80598,7 @@
       <c r="M576" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N576" s="22" t="s">
+      <c r="N576" s="19" t="s">
         <v>445</v>
       </c>
       <c r="O576" s="7" t="s">
@@ -80735,9 +80704,7 @@
       <c r="B577" s="6">
         <v>573</v>
       </c>
-      <c r="C577" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C577" s="2"/>
       <c r="D577" s="7" t="s">
         <v>44</v>
       </c>
@@ -80756,9 +80723,7 @@
       <c r="I577" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J577" s="19" t="s">
-        <v>434</v>
-      </c>
+      <c r="J577" s="19"/>
       <c r="K577" s="7" t="s">
         <v>44</v>
       </c>
@@ -80768,7 +80733,7 @@
       <c r="M577" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N577" s="22"/>
+      <c r="N577" s="19"/>
       <c r="O577" s="7" t="s">
         <v>44</v>
       </c>
@@ -80872,9 +80837,7 @@
       <c r="B578" s="6">
         <v>574</v>
       </c>
-      <c r="C578" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C578" s="2"/>
       <c r="D578" s="7" t="s">
         <v>44</v>
       </c>
@@ -80890,7 +80853,7 @@
       <c r="H578" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I578" s="14" t="s">
+      <c r="I578" s="20" t="s">
         <v>433</v>
       </c>
       <c r="J578" s="6" t="s">
@@ -80905,7 +80868,7 @@
       <c r="M578" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N578" s="23" t="s">
+      <c r="N578" s="25" t="s">
         <v>424</v>
       </c>
       <c r="O578" s="7" t="s">
@@ -81011,9 +80974,7 @@
       <c r="B579" s="6">
         <v>575</v>
       </c>
-      <c r="C579" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C579" s="2"/>
       <c r="D579" s="7" t="s">
         <v>44</v>
       </c>
@@ -81032,7 +80993,7 @@
       <c r="I579" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J579" s="14" t="s">
+      <c r="J579" s="20" t="s">
         <v>433</v>
       </c>
       <c r="K579" s="7" t="s">
@@ -81044,7 +81005,7 @@
       <c r="M579" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N579" s="24"/>
+      <c r="N579" s="25"/>
       <c r="O579" s="7" t="s">
         <v>44</v>
       </c>
@@ -81148,9 +81109,7 @@
       <c r="B580" s="6">
         <v>576</v>
       </c>
-      <c r="C580" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C580" s="2"/>
       <c r="D580" s="7" t="s">
         <v>44</v>
       </c>
@@ -81166,7 +81125,7 @@
       <c r="H580" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I580" s="14" t="s">
+      <c r="I580" s="20" t="s">
         <v>433</v>
       </c>
       <c r="J580" s="6" t="s">
@@ -81181,7 +81140,7 @@
       <c r="M580" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N580" s="24"/>
+      <c r="N580" s="25"/>
       <c r="O580" s="7" t="s">
         <v>44</v>
       </c>
@@ -81285,9 +81244,7 @@
       <c r="B581" s="6">
         <v>577</v>
       </c>
-      <c r="C581" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C581" s="2"/>
       <c r="D581" s="7" t="s">
         <v>44</v>
       </c>
@@ -81306,7 +81263,7 @@
       <c r="I581" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J581" s="14" t="s">
+      <c r="J581" s="20" t="s">
         <v>433</v>
       </c>
       <c r="K581" s="7" t="s">
@@ -81422,9 +81379,7 @@
       <c r="B582" s="6">
         <v>578</v>
       </c>
-      <c r="C582" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C582" s="2"/>
       <c r="D582" s="7" t="s">
         <v>44</v>
       </c>
@@ -81440,7 +81395,7 @@
       <c r="H582" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I582" s="15" t="s">
+      <c r="I582" s="21" t="s">
         <v>431</v>
       </c>
       <c r="J582" s="6" t="s">
@@ -81561,9 +81516,7 @@
       <c r="B583" s="6">
         <v>579</v>
       </c>
-      <c r="C583" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C583" s="2"/>
       <c r="D583" s="7" t="s">
         <v>44</v>
       </c>
@@ -81582,7 +81535,7 @@
       <c r="I583" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J583" s="15" t="s">
+      <c r="J583" s="21" t="s">
         <v>431</v>
       </c>
       <c r="K583" s="7" t="s">
@@ -81594,7 +81547,7 @@
       <c r="M583" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N583" s="27"/>
+      <c r="N583" s="26"/>
       <c r="O583" s="7" t="s">
         <v>44</v>
       </c>
@@ -81698,9 +81651,7 @@
       <c r="B584" s="6">
         <v>580</v>
       </c>
-      <c r="C584" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C584" s="2"/>
       <c r="D584" s="7" t="s">
         <v>44</v>
       </c>
@@ -81716,7 +81667,7 @@
       <c r="H584" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I584" s="15" t="s">
+      <c r="I584" s="21" t="s">
         <v>431</v>
       </c>
       <c r="J584" s="6" t="s">
@@ -81731,7 +81682,7 @@
       <c r="M584" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N584" s="27"/>
+      <c r="N584" s="26"/>
       <c r="O584" s="7" t="s">
         <v>44</v>
       </c>
@@ -81835,9 +81786,7 @@
       <c r="B585" s="6">
         <v>581</v>
       </c>
-      <c r="C585" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C585" s="2"/>
       <c r="D585" s="7" t="s">
         <v>44</v>
       </c>
@@ -81856,7 +81805,7 @@
       <c r="I585" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J585" s="15" t="s">
+      <c r="J585" s="21" t="s">
         <v>431</v>
       </c>
       <c r="K585" s="7" t="s">
@@ -81868,7 +81817,7 @@
       <c r="M585" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N585" s="28"/>
+      <c r="N585" s="26"/>
       <c r="O585" s="7" t="s">
         <v>44</v>
       </c>
@@ -81972,9 +81921,7 @@
       <c r="B586" s="6">
         <v>582</v>
       </c>
-      <c r="C586" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C586" s="2"/>
       <c r="D586" s="7" t="s">
         <v>44</v>
       </c>
@@ -81999,13 +81946,13 @@
       <c r="K586" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L586" s="19" t="s">
+      <c r="L586" s="14" t="s">
         <v>434</v>
       </c>
       <c r="M586" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="N586" s="19" t="s">
+      <c r="N586" s="14" t="s">
         <v>445</v>
       </c>
       <c r="O586" s="7" t="s">
@@ -82111,9 +82058,7 @@
       <c r="B587" s="6">
         <v>583</v>
       </c>
-      <c r="C587" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C587" s="2"/>
       <c r="D587" s="7" t="s">
         <v>44</v>
       </c>
@@ -82135,16 +82080,16 @@
       <c r="J587" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K587" s="20" t="s">
+      <c r="K587" s="15" t="s">
         <v>438</v>
       </c>
-      <c r="L587" s="8" t="s">
+      <c r="L587" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M587" s="8" t="s">
+      <c r="M587" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N587" s="20" t="s">
+      <c r="N587" s="15" t="s">
         <v>393</v>
       </c>
       <c r="O587" s="7" t="s">
@@ -82250,9 +82195,7 @@
       <c r="B588" s="6">
         <v>584</v>
       </c>
-      <c r="C588" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="C588" s="2"/>
       <c r="D588" s="7" t="s">
         <v>44</v>
       </c>
@@ -82274,12 +82217,12 @@
       <c r="J588" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K588" s="21" t="s">
+      <c r="K588" s="16" t="s">
         <v>437</v>
       </c>
-      <c r="L588" s="11"/>
-      <c r="M588" s="11"/>
-      <c r="N588" s="21" t="s">
+      <c r="L588" s="2"/>
+      <c r="M588" s="2"/>
+      <c r="N588" s="16" t="s">
         <v>412</v>
       </c>
       <c r="O588" s="7" t="s">
@@ -82385,7 +82328,7 @@
       <c r="B589" s="6">
         <v>585</v>
       </c>
-      <c r="C589" s="13" t="s">
+      <c r="C589" s="12" t="s">
         <v>447</v>
       </c>
       <c r="D589" s="7" t="s">
@@ -82403,7 +82346,7 @@
       <c r="H589" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I589" s="13" t="s">
+      <c r="I589" s="12" t="s">
         <v>447</v>
       </c>
       <c r="J589" s="6" t="s">
@@ -82412,13 +82355,13 @@
       <c r="K589" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L589" s="19" t="s">
+      <c r="L589" s="14" t="s">
         <v>434</v>
       </c>
       <c r="M589" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="N589" s="19" t="s">
+      <c r="N589" s="14" t="s">
         <v>445</v>
       </c>
       <c r="O589" s="7" t="s">
@@ -82524,7 +82467,7 @@
       <c r="B590" s="6">
         <v>586</v>
       </c>
-      <c r="C590" s="20" t="s">
+      <c r="C590" s="15" t="s">
         <v>438</v>
       </c>
       <c r="D590" s="7" t="s">
@@ -82542,22 +82485,22 @@
       <c r="H590" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I590" s="6" t="s">
+      <c r="I590" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J590" s="14" t="s">
+      <c r="J590" s="20" t="s">
         <v>433</v>
       </c>
-      <c r="K590" s="20" t="s">
+      <c r="K590" s="15" t="s">
         <v>167</v>
       </c>
       <c r="L590" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M590" s="6" t="s">
+      <c r="M590" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N590" s="14" t="s">
+      <c r="N590" s="20" t="s">
         <v>448</v>
       </c>
       <c r="O590" s="7" t="s">
@@ -82663,7 +82606,7 @@
       <c r="B591" s="6">
         <v>587</v>
       </c>
-      <c r="C591" s="17" t="s">
+      <c r="C591" s="22" t="s">
         <v>444</v>
       </c>
       <c r="D591" s="7" t="s">
@@ -82681,22 +82624,18 @@
       <c r="H591" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I591" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J591" s="19" t="s">
+      <c r="I591" s="2"/>
+      <c r="J591" s="14" t="s">
         <v>434</v>
       </c>
       <c r="K591" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L591" s="19" t="s">
+      <c r="L591" s="14" t="s">
         <v>436</v>
       </c>
-      <c r="M591" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N591" s="17" t="s">
+      <c r="M591" s="2"/>
+      <c r="N591" s="22" t="s">
         <v>449</v>
       </c>
       <c r="O591" s="7" t="s">
@@ -82802,7 +82741,7 @@
       <c r="B592" s="6">
         <v>588</v>
       </c>
-      <c r="C592" s="21" t="s">
+      <c r="C592" s="16" t="s">
         <v>437</v>
       </c>
       <c r="D592" s="7" t="s">
@@ -82820,21 +82759,19 @@
       <c r="H592" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I592" s="21" t="s">
+      <c r="I592" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="J592" s="6" t="s">
+      <c r="J592" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K592" s="21" t="s">
+      <c r="K592" s="24" t="s">
         <v>168</v>
       </c>
-      <c r="L592" s="6" t="s">
+      <c r="L592" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="M592" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="M592" s="2"/>
       <c r="N592" s="6" t="s">
         <v>450</v>
       </c>
@@ -82938,11 +82875,9 @@
       <c r="AV592" s="6"/>
     </row>
     <row r="593" spans="2:48" x14ac:dyDescent="0.25">
-      <c r="B593" s="6">
-        <v>589</v>
-      </c>
-      <c r="C593" s="21" t="s">
-        <v>437</v>
+      <c r="B593" s="6"/>
+      <c r="C593" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="D593" s="7" t="s">
         <v>44</v>
@@ -82957,283 +82892,453 @@
         <v>44</v>
       </c>
       <c r="H593" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I593" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="J593" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K593" s="21" t="s">
-        <v>168</v>
-      </c>
-      <c r="L593" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M593" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N593" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I593" s="24"/>
+      <c r="J593" s="2"/>
+      <c r="K593" s="24"/>
+      <c r="L593" s="2"/>
+      <c r="M593" s="2"/>
+      <c r="N593" s="16" t="s">
         <v>451</v>
       </c>
-      <c r="O593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="P593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="R593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="S593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="T593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="U593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="V593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="W593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="X593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT593" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU593" s="11"/>
+      <c r="O593" s="7"/>
+      <c r="P593" s="7"/>
+      <c r="Q593" s="7"/>
+      <c r="R593" s="7"/>
+      <c r="S593" s="7"/>
+      <c r="T593" s="7"/>
+      <c r="U593" s="7"/>
+      <c r="V593" s="7"/>
+      <c r="W593" s="7"/>
+      <c r="X593" s="7"/>
+      <c r="Y593" s="7"/>
+      <c r="Z593" s="7"/>
+      <c r="AA593" s="7"/>
+      <c r="AB593" s="7"/>
+      <c r="AC593" s="7"/>
+      <c r="AD593" s="7"/>
+      <c r="AE593" s="7"/>
+      <c r="AF593" s="7"/>
+      <c r="AG593" s="7"/>
+      <c r="AH593" s="7"/>
+      <c r="AI593" s="7"/>
+      <c r="AJ593" s="7"/>
+      <c r="AK593" s="7"/>
+      <c r="AL593" s="7"/>
+      <c r="AM593" s="7"/>
+      <c r="AN593" s="7"/>
+      <c r="AO593" s="7"/>
+      <c r="AP593" s="7"/>
+      <c r="AQ593" s="7"/>
+      <c r="AR593" s="7"/>
+      <c r="AS593" s="7"/>
+      <c r="AT593" s="7"/>
+      <c r="AU593" s="9"/>
       <c r="AV593" s="6"/>
     </row>
     <row r="594" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B594" s="6">
-        <v>590</v>
-      </c>
-      <c r="C594" s="6"/>
-      <c r="D594" s="6"/>
-      <c r="E594" s="6"/>
-      <c r="F594" s="6"/>
-      <c r="G594" s="6"/>
-      <c r="H594" s="6"/>
-      <c r="I594" s="6"/>
-      <c r="J594" s="6"/>
-      <c r="K594" s="6"/>
-      <c r="L594" s="6"/>
-      <c r="M594" s="6"/>
-      <c r="N594" s="6"/>
-      <c r="O594" s="7"/>
-      <c r="P594" s="7"/>
-      <c r="Q594" s="7"/>
-      <c r="R594" s="7"/>
-      <c r="S594" s="7"/>
-      <c r="T594" s="7"/>
-      <c r="U594" s="7"/>
-      <c r="V594" s="7"/>
-      <c r="W594" s="7"/>
-      <c r="X594" s="7"/>
-      <c r="Y594" s="7"/>
-      <c r="Z594" s="7"/>
-      <c r="AA594" s="7"/>
-      <c r="AB594" s="7"/>
-      <c r="AC594" s="7"/>
-      <c r="AD594" s="7"/>
-      <c r="AE594" s="7"/>
-      <c r="AF594" s="7"/>
-      <c r="AG594" s="7"/>
-      <c r="AH594" s="7"/>
-      <c r="AI594" s="7"/>
-      <c r="AJ594" s="7"/>
-      <c r="AK594" s="7"/>
-      <c r="AL594" s="7"/>
-      <c r="AM594" s="7"/>
-      <c r="AN594" s="7"/>
-      <c r="AO594" s="7"/>
-      <c r="AP594" s="7"/>
-      <c r="AQ594" s="7"/>
-      <c r="AR594" s="7"/>
-      <c r="AS594" s="7"/>
-      <c r="AT594" s="7"/>
-      <c r="AU594" s="6" t="s">
-        <v>453</v>
-      </c>
+        <v>589</v>
+      </c>
+      <c r="C594" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="D594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H594" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I594" s="24"/>
+      <c r="J594" s="2"/>
+      <c r="K594" s="24"/>
+      <c r="L594" s="2"/>
+      <c r="M594" s="2"/>
+      <c r="N594" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="O594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="W594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT594" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU594" s="11"/>
       <c r="AV594" s="6"/>
     </row>
     <row r="595" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B595" s="6">
-        <v>591</v>
-      </c>
-      <c r="C595" s="6"/>
-      <c r="D595" s="6"/>
-      <c r="E595" s="6"/>
-      <c r="F595" s="6"/>
-      <c r="G595" s="6"/>
-      <c r="H595" s="6"/>
-      <c r="I595" s="6"/>
-      <c r="J595" s="6"/>
-      <c r="K595" s="6"/>
-      <c r="L595" s="6"/>
-      <c r="M595" s="6"/>
-      <c r="N595" s="6"/>
-      <c r="O595" s="6"/>
-      <c r="P595" s="6"/>
-      <c r="Q595" s="6"/>
-      <c r="R595" s="6"/>
-      <c r="S595" s="6"/>
-      <c r="T595" s="6"/>
-      <c r="U595" s="6"/>
-      <c r="V595" s="6"/>
-      <c r="W595" s="6"/>
-      <c r="X595" s="6"/>
-      <c r="Y595" s="6"/>
-      <c r="Z595" s="6"/>
-      <c r="AA595" s="6"/>
-      <c r="AB595" s="6"/>
-      <c r="AC595" s="6"/>
-      <c r="AD595" s="6"/>
-      <c r="AE595" s="6"/>
-      <c r="AF595" s="6"/>
-      <c r="AG595" s="6"/>
-      <c r="AH595" s="6"/>
-      <c r="AI595" s="6"/>
-      <c r="AJ595" s="6"/>
-      <c r="AK595" s="6"/>
-      <c r="AL595" s="6"/>
-      <c r="AM595" s="6"/>
-      <c r="AN595" s="6"/>
-      <c r="AO595" s="6"/>
-      <c r="AP595" s="6"/>
-      <c r="AQ595" s="6"/>
-      <c r="AR595" s="6"/>
-      <c r="AS595" s="6"/>
-      <c r="AT595" s="6"/>
-      <c r="AU595" s="6"/>
+        <v>590</v>
+      </c>
+      <c r="C595" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H595" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I595" s="16" t="s">
+        <v>437</v>
+      </c>
+      <c r="J595" s="19" t="s">
+        <v>434</v>
+      </c>
+      <c r="K595" s="24"/>
+      <c r="L595" s="19" t="s">
+        <v>436</v>
+      </c>
+      <c r="M595" s="2"/>
+      <c r="N595" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="O595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="W595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT595" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU595" s="8" t="s">
+        <v>453</v>
+      </c>
       <c r="AV595" s="6"/>
     </row>
     <row r="596" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B596" s="6">
-        <v>592</v>
-      </c>
-      <c r="C596" s="6"/>
-      <c r="D596" s="6"/>
-      <c r="E596" s="6"/>
-      <c r="F596" s="6"/>
-      <c r="G596" s="6"/>
-      <c r="H596" s="6"/>
-      <c r="I596" s="6"/>
-      <c r="J596" s="6"/>
-      <c r="K596" s="6"/>
-      <c r="L596" s="6"/>
-      <c r="M596" s="6"/>
-      <c r="N596" s="6"/>
-      <c r="O596" s="6"/>
-      <c r="P596" s="6"/>
-      <c r="Q596" s="6"/>
-      <c r="R596" s="6"/>
-      <c r="S596" s="6"/>
-      <c r="T596" s="6"/>
-      <c r="U596" s="6"/>
-      <c r="V596" s="6"/>
-      <c r="W596" s="6"/>
-      <c r="X596" s="6"/>
-      <c r="Y596" s="6"/>
-      <c r="Z596" s="6"/>
-      <c r="AA596" s="6"/>
-      <c r="AB596" s="6"/>
-      <c r="AC596" s="6"/>
-      <c r="AD596" s="6"/>
-      <c r="AE596" s="6"/>
-      <c r="AF596" s="6"/>
-      <c r="AG596" s="6"/>
-      <c r="AH596" s="6"/>
-      <c r="AI596" s="6"/>
-      <c r="AJ596" s="6"/>
-      <c r="AK596" s="6"/>
-      <c r="AL596" s="6"/>
-      <c r="AM596" s="6"/>
-      <c r="AN596" s="6"/>
-      <c r="AO596" s="6"/>
-      <c r="AP596" s="6"/>
-      <c r="AQ596" s="6"/>
-      <c r="AR596" s="6"/>
-      <c r="AS596" s="6"/>
-      <c r="AT596" s="6"/>
-      <c r="AU596" s="6"/>
+        <v>591</v>
+      </c>
+      <c r="C596" s="2"/>
+      <c r="D596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H596" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I596" s="12" t="s">
+        <v>447</v>
+      </c>
+      <c r="J596" s="19"/>
+      <c r="K596" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="L596" s="19"/>
+      <c r="M596" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N596" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="O596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="W596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT596" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU596" s="11"/>
       <c r="AV596" s="6"/>
     </row>
     <row r="597" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B597" s="6">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C597" s="6"/>
       <c r="D597" s="6"/>
@@ -83284,7 +83389,7 @@
     </row>
     <row r="598" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B598" s="6">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C598" s="6"/>
       <c r="D598" s="6"/>
@@ -83335,7 +83440,7 @@
     </row>
     <row r="599" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B599" s="6">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C599" s="6"/>
       <c r="D599" s="6"/>
@@ -83386,7 +83491,7 @@
     </row>
     <row r="600" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B600" s="6">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C600" s="6"/>
       <c r="D600" s="6"/>
@@ -83437,7 +83542,7 @@
     </row>
     <row r="601" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B601" s="6">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C601" s="6"/>
       <c r="D601" s="6"/>
@@ -83488,7 +83593,7 @@
     </row>
     <row r="602" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B602" s="6">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C602" s="6"/>
       <c r="D602" s="6"/>
@@ -83539,7 +83644,7 @@
     </row>
     <row r="603" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B603" s="6">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C603" s="6"/>
       <c r="D603" s="6"/>
@@ -83590,7 +83695,7 @@
     </row>
     <row r="604" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B604" s="6">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C604" s="6"/>
       <c r="D604" s="6"/>
@@ -83641,7 +83746,7 @@
     </row>
     <row r="605" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B605" s="6">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C605" s="6"/>
       <c r="D605" s="6"/>
@@ -83692,7 +83797,7 @@
     </row>
     <row r="606" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B606" s="6">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="C606" s="6"/>
       <c r="D606" s="6"/>
@@ -83743,7 +83848,7 @@
     </row>
     <row r="607" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B607" s="6">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="C607" s="6"/>
       <c r="D607" s="6"/>
@@ -83794,7 +83899,7 @@
     </row>
     <row r="608" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B608" s="6">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C608" s="6"/>
       <c r="D608" s="6"/>
@@ -83845,7 +83950,7 @@
     </row>
     <row r="609" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B609" s="6">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C609" s="6"/>
       <c r="D609" s="6"/>
@@ -83896,7 +84001,7 @@
     </row>
     <row r="610" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B610" s="6">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C610" s="6"/>
       <c r="D610" s="6"/>
@@ -83947,7 +84052,7 @@
     </row>
     <row r="611" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B611" s="6">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C611" s="6"/>
       <c r="D611" s="6"/>
@@ -83998,7 +84103,7 @@
     </row>
     <row r="612" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B612" s="6">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C612" s="6"/>
       <c r="D612" s="6"/>
@@ -84049,7 +84154,7 @@
     </row>
     <row r="613" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B613" s="6">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="C613" s="6"/>
       <c r="D613" s="6"/>
@@ -84100,7 +84205,7 @@
     </row>
     <row r="614" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B614" s="6">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C614" s="6"/>
       <c r="D614" s="6"/>
@@ -84151,7 +84256,7 @@
     </row>
     <row r="615" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B615" s="6">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="C615" s="6"/>
       <c r="D615" s="6"/>
@@ -84202,7 +84307,7 @@
     </row>
     <row r="616" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B616" s="6">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C616" s="6"/>
       <c r="D616" s="6"/>
@@ -84253,7 +84358,7 @@
     </row>
     <row r="617" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B617" s="6">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C617" s="6"/>
       <c r="D617" s="6"/>
@@ -84304,7 +84409,7 @@
     </row>
     <row r="618" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B618" s="6">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="C618" s="6"/>
       <c r="D618" s="6"/>
@@ -84355,7 +84460,7 @@
     </row>
     <row r="619" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B619" s="6">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="C619" s="6"/>
       <c r="D619" s="6"/>
@@ -84406,7 +84511,7 @@
     </row>
     <row r="620" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B620" s="6">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C620" s="6"/>
       <c r="D620" s="6"/>
@@ -84457,7 +84562,7 @@
     </row>
     <row r="621" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B621" s="6">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C621" s="6"/>
       <c r="D621" s="6"/>
@@ -84508,7 +84613,7 @@
     </row>
     <row r="622" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B622" s="6">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C622" s="6"/>
       <c r="D622" s="6"/>
@@ -84559,7 +84664,7 @@
     </row>
     <row r="623" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B623" s="6">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C623" s="6"/>
       <c r="D623" s="6"/>
@@ -84610,7 +84715,7 @@
     </row>
     <row r="624" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B624" s="6">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C624" s="6"/>
       <c r="D624" s="6"/>
@@ -84661,7 +84766,7 @@
     </row>
     <row r="625" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B625" s="6">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="C625" s="6"/>
       <c r="D625" s="6"/>
@@ -84712,7 +84817,7 @@
     </row>
     <row r="626" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B626" s="6">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C626" s="6"/>
       <c r="D626" s="6"/>
@@ -84763,7 +84868,7 @@
     </row>
     <row r="627" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B627" s="6">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="C627" s="6"/>
       <c r="D627" s="6"/>
@@ -84814,7 +84919,7 @@
     </row>
     <row r="628" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B628" s="6">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="C628" s="6"/>
       <c r="D628" s="6"/>
@@ -84865,7 +84970,7 @@
     </row>
     <row r="629" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B629" s="6">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C629" s="6"/>
       <c r="D629" s="6"/>
@@ -84916,7 +85021,7 @@
     </row>
     <row r="630" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B630" s="6">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C630" s="6"/>
       <c r="D630" s="6"/>
@@ -84967,7 +85072,7 @@
     </row>
     <row r="631" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B631" s="6">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C631" s="6"/>
       <c r="D631" s="6"/>
@@ -85018,7 +85123,7 @@
     </row>
     <row r="632" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B632" s="6">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C632" s="6"/>
       <c r="D632" s="6"/>
@@ -85069,7 +85174,7 @@
     </row>
     <row r="633" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B633" s="6">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C633" s="6"/>
       <c r="D633" s="6"/>
@@ -85120,7 +85225,7 @@
     </row>
     <row r="634" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B634" s="6">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="C634" s="6"/>
       <c r="D634" s="6"/>
@@ -85171,7 +85276,7 @@
     </row>
     <row r="635" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B635" s="6">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C635" s="6"/>
       <c r="D635" s="6"/>
@@ -85222,7 +85327,7 @@
     </row>
     <row r="636" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B636" s="6">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="C636" s="6"/>
       <c r="D636" s="6"/>
@@ -85273,7 +85378,7 @@
     </row>
     <row r="637" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B637" s="6">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="C637" s="6"/>
       <c r="D637" s="6"/>
@@ -85324,7 +85429,7 @@
     </row>
     <row r="638" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B638" s="6">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C638" s="6"/>
       <c r="D638" s="6"/>
@@ -85375,7 +85480,7 @@
     </row>
     <row r="639" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B639" s="6">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C639" s="6"/>
       <c r="D639" s="6"/>
@@ -85426,7 +85531,7 @@
     </row>
     <row r="640" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B640" s="6">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C640" s="6"/>
       <c r="D640" s="6"/>
@@ -85477,7 +85582,7 @@
     </row>
     <row r="641" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B641" s="6">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C641" s="6"/>
       <c r="D641" s="6"/>
@@ -85528,7 +85633,7 @@
     </row>
     <row r="642" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B642" s="6">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="C642" s="6"/>
       <c r="D642" s="6"/>
@@ -85579,7 +85684,7 @@
     </row>
     <row r="643" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B643" s="6">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C643" s="6"/>
       <c r="D643" s="6"/>
@@ -85630,7 +85735,7 @@
     </row>
     <row r="644" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B644" s="6">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C644" s="6"/>
       <c r="D644" s="6"/>
@@ -85677,11 +85782,11 @@
       <c r="AS644" s="6"/>
       <c r="AT644" s="6"/>
       <c r="AU644" s="6"/>
-      <c r="AV644" s="12"/>
+      <c r="AV644" s="6"/>
     </row>
     <row r="645" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B645" s="6">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C645" s="6"/>
       <c r="D645" s="6"/>
@@ -85728,11 +85833,11 @@
       <c r="AS645" s="6"/>
       <c r="AT645" s="6"/>
       <c r="AU645" s="6"/>
-      <c r="AV645" s="12"/>
+      <c r="AV645" s="23"/>
     </row>
     <row r="646" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B646" s="6">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C646" s="6"/>
       <c r="D646" s="6"/>
@@ -85779,11 +85884,11 @@
       <c r="AS646" s="6"/>
       <c r="AT646" s="6"/>
       <c r="AU646" s="6"/>
-      <c r="AV646" s="12"/>
+      <c r="AV646" s="23"/>
     </row>
     <row r="647" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B647" s="6">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C647" s="6"/>
       <c r="D647" s="6"/>
@@ -85830,11 +85935,11 @@
       <c r="AS647" s="6"/>
       <c r="AT647" s="6"/>
       <c r="AU647" s="6"/>
-      <c r="AV647" s="12"/>
+      <c r="AV647" s="23"/>
     </row>
     <row r="648" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B648" s="6">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="C648" s="6"/>
       <c r="D648" s="6"/>
@@ -85881,11 +85986,11 @@
       <c r="AS648" s="6"/>
       <c r="AT648" s="6"/>
       <c r="AU648" s="6"/>
-      <c r="AV648" s="12"/>
+      <c r="AV648" s="23"/>
     </row>
     <row r="649" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B649" s="6">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C649" s="6"/>
       <c r="D649" s="6"/>
@@ -85932,11 +86037,11 @@
       <c r="AS649" s="6"/>
       <c r="AT649" s="6"/>
       <c r="AU649" s="6"/>
-      <c r="AV649" s="12"/>
+      <c r="AV649" s="23"/>
     </row>
     <row r="650" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B650" s="6">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C650" s="6"/>
       <c r="D650" s="6"/>
@@ -85983,11 +86088,11 @@
       <c r="AS650" s="6"/>
       <c r="AT650" s="6"/>
       <c r="AU650" s="6"/>
-      <c r="AV650" s="12"/>
+      <c r="AV650" s="23"/>
     </row>
     <row r="651" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B651" s="6">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C651" s="6"/>
       <c r="D651" s="6"/>
@@ -86034,11 +86139,11 @@
       <c r="AS651" s="6"/>
       <c r="AT651" s="6"/>
       <c r="AU651" s="6"/>
-      <c r="AV651" s="12"/>
+      <c r="AV651" s="23"/>
     </row>
     <row r="652" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B652" s="6">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="C652" s="6"/>
       <c r="D652" s="6"/>
@@ -86085,11 +86190,11 @@
       <c r="AS652" s="6"/>
       <c r="AT652" s="6"/>
       <c r="AU652" s="6"/>
-      <c r="AV652" s="12"/>
+      <c r="AV652" s="23"/>
     </row>
     <row r="653" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B653" s="6">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C653" s="6"/>
       <c r="D653" s="6"/>
@@ -86136,11 +86241,11 @@
       <c r="AS653" s="6"/>
       <c r="AT653" s="6"/>
       <c r="AU653" s="6"/>
-      <c r="AV653" s="12"/>
+      <c r="AV653" s="23"/>
     </row>
     <row r="654" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B654" s="6">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C654" s="6"/>
       <c r="D654" s="6"/>
@@ -86187,154 +86292,66 @@
       <c r="AS654" s="6"/>
       <c r="AT654" s="6"/>
       <c r="AU654" s="6"/>
-      <c r="AV654" s="12"/>
+      <c r="AV654" s="23"/>
     </row>
     <row r="655" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B655" s="6">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C655" s="6"/>
-      <c r="D655" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H655" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I655" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J655" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K655" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L655" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M655" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="N655" s="2" t="s">
-        <v>338</v>
-      </c>
-      <c r="O655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="P655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="R655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="S655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="T655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="U655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="V655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="W655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="X655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT655" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU655" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="AV655" s="6"/>
+      <c r="D655" s="6"/>
+      <c r="E655" s="6"/>
+      <c r="F655" s="6"/>
+      <c r="G655" s="6"/>
+      <c r="H655" s="6"/>
+      <c r="I655" s="6"/>
+      <c r="J655" s="6"/>
+      <c r="K655" s="6"/>
+      <c r="L655" s="6"/>
+      <c r="M655" s="6"/>
+      <c r="N655" s="6"/>
+      <c r="O655" s="6"/>
+      <c r="P655" s="6"/>
+      <c r="Q655" s="6"/>
+      <c r="R655" s="6"/>
+      <c r="S655" s="6"/>
+      <c r="T655" s="6"/>
+      <c r="U655" s="6"/>
+      <c r="V655" s="6"/>
+      <c r="W655" s="6"/>
+      <c r="X655" s="6"/>
+      <c r="Y655" s="6"/>
+      <c r="Z655" s="6"/>
+      <c r="AA655" s="6"/>
+      <c r="AB655" s="6"/>
+      <c r="AC655" s="6"/>
+      <c r="AD655" s="6"/>
+      <c r="AE655" s="6"/>
+      <c r="AF655" s="6"/>
+      <c r="AG655" s="6"/>
+      <c r="AH655" s="6"/>
+      <c r="AI655" s="6"/>
+      <c r="AJ655" s="6"/>
+      <c r="AK655" s="6"/>
+      <c r="AL655" s="6"/>
+      <c r="AM655" s="6"/>
+      <c r="AN655" s="6"/>
+      <c r="AO655" s="6"/>
+      <c r="AP655" s="6"/>
+      <c r="AQ655" s="6"/>
+      <c r="AR655" s="6"/>
+      <c r="AS655" s="6"/>
+      <c r="AT655" s="6"/>
+      <c r="AU655" s="6"/>
+      <c r="AV655" s="23"/>
     </row>
     <row r="656" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B656" s="6">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C656" s="6"/>
       <c r="D656" s="6" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="E656" s="7" t="s">
         <v>44</v>
@@ -86345,13 +86362,27 @@
       <c r="G656" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H656" s="2"/>
-      <c r="I656" s="2"/>
-      <c r="J656" s="2"/>
-      <c r="K656" s="2"/>
-      <c r="L656" s="2"/>
-      <c r="M656" s="2"/>
-      <c r="N656" s="2"/>
+      <c r="H656" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I656" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J656" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K656" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="L656" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M656" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N656" s="2" t="s">
+        <v>338</v>
+      </c>
       <c r="O656" s="7" t="s">
         <v>44</v>
       </c>
@@ -86448,16 +86479,18 @@
       <c r="AT656" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU656" s="2"/>
+      <c r="AU656" s="2" t="s">
+        <v>430</v>
+      </c>
       <c r="AV656" s="6"/>
     </row>
     <row r="657" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B657" s="6">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C657" s="6"/>
       <c r="D657" s="6" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="E657" s="7" t="s">
         <v>44</v>
@@ -86576,11 +86609,11 @@
     </row>
     <row r="658" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B658" s="6">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C658" s="6"/>
       <c r="D658" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E658" s="7" t="s">
         <v>44</v>
@@ -86699,11 +86732,11 @@
     </row>
     <row r="659" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B659" s="6">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C659" s="6"/>
       <c r="D659" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E659" s="7" t="s">
         <v>44</v>
@@ -86822,11 +86855,11 @@
     </row>
     <row r="660" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B660" s="6">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C660" s="6"/>
       <c r="D660" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E660" s="7" t="s">
         <v>44</v>
@@ -86945,11 +86978,11 @@
     </row>
     <row r="661" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B661" s="6">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C661" s="6"/>
       <c r="D661" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E661" s="7" t="s">
         <v>44</v>
@@ -87068,11 +87101,11 @@
     </row>
     <row r="662" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B662" s="6">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C662" s="6"/>
       <c r="D662" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E662" s="7" t="s">
         <v>44</v>
@@ -87191,11 +87224,11 @@
     </row>
     <row r="663" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B663" s="6">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C663" s="6"/>
       <c r="D663" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E663" s="7" t="s">
         <v>44</v>
@@ -87314,11 +87347,11 @@
     </row>
     <row r="664" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B664" s="6">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C664" s="6"/>
       <c r="D664" s="6" t="s">
-        <v>228</v>
+        <v>43</v>
       </c>
       <c r="E664" s="7" t="s">
         <v>44</v>
@@ -87437,11 +87470,11 @@
     </row>
     <row r="665" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B665" s="6">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C665" s="6"/>
       <c r="D665" s="6" t="s">
-        <v>115</v>
+        <v>228</v>
       </c>
       <c r="E665" s="7" t="s">
         <v>44</v>
@@ -87560,11 +87593,11 @@
     </row>
     <row r="666" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B666" s="6">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C666" s="6"/>
       <c r="D666" s="6" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="E666" s="7" t="s">
         <v>44</v>
@@ -87575,15 +87608,11 @@
       <c r="G666" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H666" s="6" t="s">
-        <v>25</v>
-      </c>
+      <c r="H666" s="2"/>
       <c r="I666" s="2"/>
       <c r="J666" s="2"/>
       <c r="K666" s="2"/>
-      <c r="L666" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="L666" s="2"/>
       <c r="M666" s="2"/>
       <c r="N666" s="2"/>
       <c r="O666" s="7" t="s">
@@ -87687,11 +87716,11 @@
     </row>
     <row r="667" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B667" s="6">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C667" s="6"/>
       <c r="D667" s="6" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="E667" s="7" t="s">
         <v>44</v>
@@ -87703,13 +87732,13 @@
         <v>44</v>
       </c>
       <c r="H667" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I667" s="2"/>
       <c r="J667" s="2"/>
       <c r="K667" s="2"/>
       <c r="L667" s="6" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="M667" s="2"/>
       <c r="N667" s="2"/>
@@ -87814,11 +87843,11 @@
     </row>
     <row r="668" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B668" s="6">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C668" s="6"/>
       <c r="D668" s="6" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="E668" s="7" t="s">
         <v>44</v>
@@ -87830,13 +87859,13 @@
         <v>44</v>
       </c>
       <c r="H668" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I668" s="2"/>
       <c r="J668" s="2"/>
       <c r="K668" s="2"/>
       <c r="L668" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="M668" s="2"/>
       <c r="N668" s="2"/>
@@ -87941,11 +87970,11 @@
     </row>
     <row r="669" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B669" s="6">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C669" s="6"/>
       <c r="D669" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E669" s="7" t="s">
         <v>44</v>
@@ -87957,19 +87986,15 @@
         <v>44</v>
       </c>
       <c r="H669" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I669" s="2"/>
-      <c r="J669" s="2" t="s">
-        <v>42</v>
-      </c>
+      <c r="J669" s="2"/>
       <c r="K669" s="2"/>
-      <c r="L669" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M669" s="6" t="s">
-        <v>226</v>
-      </c>
+      <c r="L669" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M669" s="2"/>
       <c r="N669" s="2"/>
       <c r="O669" s="7" t="s">
         <v>44</v>
@@ -88072,11 +88097,11 @@
     </row>
     <row r="670" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B670" s="6">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C670" s="6"/>
       <c r="D670" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E670" s="7" t="s">
         <v>44</v>
@@ -88088,14 +88113,18 @@
         <v>44</v>
       </c>
       <c r="H670" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I670" s="2"/>
-      <c r="J670" s="2"/>
+      <c r="J670" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="K670" s="2"/>
-      <c r="L670" s="2"/>
+      <c r="L670" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="M670" s="6" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="N670" s="2"/>
       <c r="O670" s="7" t="s">
@@ -88199,11 +88228,11 @@
     </row>
     <row r="671" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B671" s="6">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C671" s="6"/>
       <c r="D671" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E671" s="7" t="s">
         <v>44</v>
@@ -88215,18 +88244,14 @@
         <v>44</v>
       </c>
       <c r="H671" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I671" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J671" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="I671" s="2"/>
+      <c r="J671" s="2"/>
       <c r="K671" s="2"/>
       <c r="L671" s="2"/>
-      <c r="M671" s="2" t="s">
-        <v>52</v>
+      <c r="M671" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="N671" s="2"/>
       <c r="O671" s="7" t="s">
@@ -88330,11 +88355,11 @@
     </row>
     <row r="672" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B672" s="6">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="C672" s="6"/>
       <c r="D672" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E672" s="7" t="s">
         <v>44</v>
@@ -88346,15 +88371,19 @@
         <v>44</v>
       </c>
       <c r="H672" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="I672" s="2"/>
-      <c r="J672" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="I672" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J672" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="K672" s="2"/>
-      <c r="L672" s="6" t="s">
+      <c r="L672" s="2"/>
+      <c r="M672" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="M672" s="2"/>
       <c r="N672" s="2"/>
       <c r="O672" s="7" t="s">
         <v>44</v>
@@ -88457,11 +88486,11 @@
     </row>
     <row r="673" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B673" s="6">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="C673" s="6"/>
       <c r="D673" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E673" s="7" t="s">
         <v>44</v>
@@ -88473,17 +88502,13 @@
         <v>44</v>
       </c>
       <c r="H673" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="I673" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="J673" s="2" t="s">
-        <v>43</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="I673" s="2"/>
+      <c r="J673" s="2"/>
       <c r="K673" s="2"/>
       <c r="L673" s="6" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="M673" s="2"/>
       <c r="N673" s="2"/>
@@ -88588,33 +88613,35 @@
     </row>
     <row r="674" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B674" s="6">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C674" s="6"/>
       <c r="D674" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E674" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F674" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G674" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H674" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I674" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E674" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F674" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G674" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H674" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I674" s="2"/>
-      <c r="J674" s="2"/>
+      <c r="J674" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="K674" s="2"/>
-      <c r="L674" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M674" s="6" t="s">
-        <v>226</v>
-      </c>
+      <c r="L674" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="M674" s="2"/>
       <c r="N674" s="2"/>
       <c r="O674" s="7" t="s">
         <v>44</v>
@@ -88717,11 +88744,11 @@
     </row>
     <row r="675" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B675" s="6">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C675" s="6"/>
       <c r="D675" s="6" t="s">
-        <v>228</v>
+        <v>43</v>
       </c>
       <c r="E675" s="7" t="s">
         <v>44</v>
@@ -88733,18 +88760,16 @@
         <v>44</v>
       </c>
       <c r="H675" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I675" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J675" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="I675" s="2"/>
+      <c r="J675" s="2"/>
       <c r="K675" s="2"/>
-      <c r="L675" s="2"/>
+      <c r="L675" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="M675" s="6" t="s">
-        <v>62</v>
+        <v>226</v>
       </c>
       <c r="N675" s="2"/>
       <c r="O675" s="7" t="s">
@@ -88848,11 +88873,11 @@
     </row>
     <row r="676" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B676" s="6">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C676" s="6"/>
       <c r="D676" s="6" t="s">
-        <v>115</v>
+        <v>228</v>
       </c>
       <c r="E676" s="7" t="s">
         <v>44</v>
@@ -88864,16 +88889,18 @@
         <v>44</v>
       </c>
       <c r="H676" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="I676" s="2"/>
-      <c r="J676" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="I676" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J676" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="K676" s="2"/>
-      <c r="L676" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="L676" s="2"/>
       <c r="M676" s="6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="N676" s="2"/>
       <c r="O676" s="7" t="s">
@@ -88977,11 +89004,11 @@
     </row>
     <row r="677" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B677" s="6">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C677" s="6"/>
       <c r="D677" s="6" t="s">
-        <v>36</v>
+        <v>115</v>
       </c>
       <c r="E677" s="7" t="s">
         <v>44</v>
@@ -88993,20 +89020,16 @@
         <v>44</v>
       </c>
       <c r="H677" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I677" s="2" t="s">
-        <v>37</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="I677" s="2"/>
       <c r="J677" s="2"/>
-      <c r="K677" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="L677" s="2" t="s">
+      <c r="K677" s="2"/>
+      <c r="L677" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M677" s="2" t="s">
-        <v>62</v>
+      <c r="M677" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="N677" s="2"/>
       <c r="O677" s="7" t="s">
@@ -89110,11 +89133,11 @@
     </row>
     <row r="678" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B678" s="6">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C678" s="6"/>
       <c r="D678" s="6" t="s">
-        <v>282</v>
+        <v>36</v>
       </c>
       <c r="E678" s="7" t="s">
         <v>44</v>
@@ -89126,15 +89149,21 @@
         <v>44</v>
       </c>
       <c r="H678" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I678" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="I678" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="J678" s="2"/>
       <c r="K678" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="L678" s="2"/>
-      <c r="M678" s="2"/>
+        <v>40</v>
+      </c>
+      <c r="L678" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M678" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="N678" s="2"/>
       <c r="O678" s="7" t="s">
         <v>44</v>
@@ -89237,11 +89266,11 @@
     </row>
     <row r="679" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B679" s="6">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C679" s="6"/>
       <c r="D679" s="6" t="s">
-        <v>37</v>
+        <v>282</v>
       </c>
       <c r="E679" s="7" t="s">
         <v>44</v>
@@ -89253,20 +89282,16 @@
         <v>44</v>
       </c>
       <c r="H679" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I679" s="2"/>
       <c r="J679" s="2"/>
       <c r="K679" s="6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="L679" s="2"/>
-      <c r="M679" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="N679" s="6" t="s">
-        <v>357</v>
-      </c>
+      <c r="M679" s="2"/>
+      <c r="N679" s="2"/>
       <c r="O679" s="7" t="s">
         <v>44</v>
       </c>
@@ -89368,37 +89393,35 @@
     </row>
     <row r="680" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B680" s="6">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C680" s="6"/>
       <c r="D680" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E680" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F680" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G680" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H680" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I680" s="2"/>
+      <c r="J680" s="2"/>
+      <c r="K680" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E680" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="F680" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="G680" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="H680" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I680" s="2"/>
-      <c r="J680" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="K680" s="6" t="s">
-        <v>40</v>
-      </c>
       <c r="L680" s="2"/>
-      <c r="M680" s="2" t="s">
-        <v>62</v>
+      <c r="M680" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="N680" s="6" t="s">
-        <v>377</v>
+        <v>357</v>
       </c>
       <c r="O680" s="7" t="s">
         <v>44</v>
@@ -89501,11 +89524,11 @@
     </row>
     <row r="681" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B681" s="6">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C681" s="6"/>
       <c r="D681" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E681" s="7" t="s">
         <v>44</v>
@@ -89517,17 +89540,21 @@
         <v>44</v>
       </c>
       <c r="H681" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I681" s="2"/>
-      <c r="J681" s="2"/>
+      <c r="J681" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="K681" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L681" s="2"/>
-      <c r="M681" s="2"/>
+      <c r="M681" s="2" t="s">
+        <v>62</v>
+      </c>
       <c r="N681" s="6" t="s">
-        <v>424</v>
+        <v>377</v>
       </c>
       <c r="O681" s="7" t="s">
         <v>44</v>
@@ -89630,11 +89657,11 @@
     </row>
     <row r="682" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B682" s="6">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C682" s="6"/>
       <c r="D682" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E682" s="7" t="s">
         <v>44</v>
@@ -89646,25 +89673,17 @@
         <v>44</v>
       </c>
       <c r="H682" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I682" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J682" s="6" t="s">
-        <v>36</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="I682" s="2"/>
+      <c r="J682" s="2"/>
       <c r="K682" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L682" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M682" s="6" t="s">
-        <v>52</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="L682" s="2"/>
+      <c r="M682" s="2"/>
       <c r="N682" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="O682" s="7" t="s">
         <v>44</v>
@@ -89767,58 +89786,144 @@
     </row>
     <row r="683" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B683" s="6">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C683" s="6"/>
-      <c r="D683" s="6"/>
-      <c r="E683" s="6"/>
-      <c r="F683" s="6"/>
-      <c r="G683" s="6"/>
-      <c r="H683" s="6"/>
-      <c r="I683" s="6"/>
-      <c r="J683" s="6"/>
-      <c r="K683" s="6"/>
-      <c r="L683" s="6"/>
-      <c r="M683" s="6"/>
-      <c r="N683" s="6"/>
-      <c r="O683" s="6"/>
-      <c r="P683" s="6"/>
-      <c r="Q683" s="6"/>
-      <c r="R683" s="6"/>
-      <c r="S683" s="6"/>
-      <c r="T683" s="6"/>
-      <c r="U683" s="6"/>
-      <c r="V683" s="6"/>
-      <c r="W683" s="6"/>
-      <c r="X683" s="6"/>
-      <c r="Y683" s="6"/>
-      <c r="Z683" s="6"/>
-      <c r="AA683" s="6"/>
-      <c r="AB683" s="6"/>
-      <c r="AC683" s="6"/>
-      <c r="AD683" s="6"/>
-      <c r="AE683" s="6"/>
-      <c r="AF683" s="6"/>
-      <c r="AG683" s="6"/>
-      <c r="AH683" s="6"/>
-      <c r="AI683" s="6"/>
-      <c r="AJ683" s="6"/>
-      <c r="AK683" s="6"/>
-      <c r="AL683" s="6"/>
-      <c r="AM683" s="6"/>
-      <c r="AN683" s="6"/>
-      <c r="AO683" s="6"/>
-      <c r="AP683" s="6"/>
-      <c r="AQ683" s="6"/>
-      <c r="AR683" s="6"/>
-      <c r="AS683" s="6"/>
-      <c r="AT683" s="6"/>
-      <c r="AU683" s="6"/>
+      <c r="D683" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H683" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I683" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J683" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K683" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L683" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="M683" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="N683" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="O683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="W683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT683" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU683" s="2"/>
       <c r="AV683" s="6"/>
     </row>
     <row r="684" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B684" s="6">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C684" s="6"/>
       <c r="D684" s="6"/>
@@ -89869,7 +89974,7 @@
     </row>
     <row r="685" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B685" s="6">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="C685" s="6"/>
       <c r="D685" s="6"/>
@@ -89920,7 +90025,7 @@
     </row>
     <row r="686" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B686" s="6">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C686" s="6"/>
       <c r="D686" s="6"/>
@@ -89970,7 +90075,9 @@
       <c r="AV686" s="6"/>
     </row>
     <row r="687" spans="2:48" x14ac:dyDescent="0.25">
-      <c r="B687" s="6"/>
+      <c r="B687" s="6">
+        <v>682</v>
+      </c>
       <c r="C687" s="6"/>
       <c r="D687" s="6"/>
       <c r="E687" s="6"/>
@@ -90018,48 +90125,214 @@
       <c r="AU687" s="6"/>
       <c r="AV687" s="6"/>
     </row>
+    <row r="688" spans="2:48" x14ac:dyDescent="0.25">
+      <c r="B688" s="6"/>
+      <c r="C688" s="6"/>
+      <c r="D688" s="6"/>
+      <c r="E688" s="6"/>
+      <c r="F688" s="6"/>
+      <c r="G688" s="6"/>
+      <c r="H688" s="6"/>
+      <c r="I688" s="6"/>
+      <c r="J688" s="6"/>
+      <c r="K688" s="6"/>
+      <c r="L688" s="6"/>
+      <c r="M688" s="6"/>
+      <c r="N688" s="6"/>
+      <c r="O688" s="6"/>
+      <c r="P688" s="6"/>
+      <c r="Q688" s="6"/>
+      <c r="R688" s="6"/>
+      <c r="S688" s="6"/>
+      <c r="T688" s="6"/>
+      <c r="U688" s="6"/>
+      <c r="V688" s="6"/>
+      <c r="W688" s="6"/>
+      <c r="X688" s="6"/>
+      <c r="Y688" s="6"/>
+      <c r="Z688" s="6"/>
+      <c r="AA688" s="6"/>
+      <c r="AB688" s="6"/>
+      <c r="AC688" s="6"/>
+      <c r="AD688" s="6"/>
+      <c r="AE688" s="6"/>
+      <c r="AF688" s="6"/>
+      <c r="AG688" s="6"/>
+      <c r="AH688" s="6"/>
+      <c r="AI688" s="6"/>
+      <c r="AJ688" s="6"/>
+      <c r="AK688" s="6"/>
+      <c r="AL688" s="6"/>
+      <c r="AM688" s="6"/>
+      <c r="AN688" s="6"/>
+      <c r="AO688" s="6"/>
+      <c r="AP688" s="6"/>
+      <c r="AQ688" s="6"/>
+      <c r="AR688" s="6"/>
+      <c r="AS688" s="6"/>
+      <c r="AT688" s="6"/>
+      <c r="AU688" s="6"/>
+      <c r="AV688" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="217">
-    <mergeCell ref="AU542:AU593"/>
-    <mergeCell ref="AU655:AU682"/>
-    <mergeCell ref="M671:M673"/>
-    <mergeCell ref="L674:L675"/>
-    <mergeCell ref="I677:I681"/>
-    <mergeCell ref="J680:J681"/>
-    <mergeCell ref="L677:L681"/>
-    <mergeCell ref="M677:M678"/>
-    <mergeCell ref="M680:M681"/>
-    <mergeCell ref="N655:N678"/>
-    <mergeCell ref="J669:J670"/>
-    <mergeCell ref="I671:I672"/>
-    <mergeCell ref="J671:J672"/>
-    <mergeCell ref="J673:J674"/>
-    <mergeCell ref="I673:I674"/>
-    <mergeCell ref="I675:I676"/>
-    <mergeCell ref="I536:I541"/>
-    <mergeCell ref="J536:J539"/>
-    <mergeCell ref="J540:J541"/>
-    <mergeCell ref="N524:N537"/>
-    <mergeCell ref="L536:L540"/>
-    <mergeCell ref="M536:M537"/>
-    <mergeCell ref="M539:M540"/>
-    <mergeCell ref="AU524:AU541"/>
-    <mergeCell ref="H655:H665"/>
-    <mergeCell ref="L655:L665"/>
-    <mergeCell ref="I534:I535"/>
-    <mergeCell ref="J534:J535"/>
-    <mergeCell ref="K524:K535"/>
-    <mergeCell ref="M524:M526"/>
-    <mergeCell ref="L527:L528"/>
-    <mergeCell ref="M529:M531"/>
-    <mergeCell ref="L532:L533"/>
-    <mergeCell ref="M534:M535"/>
-    <mergeCell ref="K655:K676"/>
-    <mergeCell ref="I655:I670"/>
-    <mergeCell ref="J655:J668"/>
-    <mergeCell ref="M655:M668"/>
-    <mergeCell ref="L669:L671"/>
-    <mergeCell ref="J675:J679"/>
+  <mergeCells count="229">
+    <mergeCell ref="AU595:AU596"/>
+    <mergeCell ref="J576:J577"/>
+    <mergeCell ref="I592:I594"/>
+    <mergeCell ref="J595:J596"/>
+    <mergeCell ref="I590:I591"/>
+    <mergeCell ref="J592:J594"/>
+    <mergeCell ref="L592:L594"/>
+    <mergeCell ref="C562:C588"/>
+    <mergeCell ref="C595:C596"/>
+    <mergeCell ref="L568:L573"/>
+    <mergeCell ref="K562:K566"/>
+    <mergeCell ref="K568:K571"/>
+    <mergeCell ref="N574:N575"/>
+    <mergeCell ref="N576:N577"/>
+    <mergeCell ref="L587:L588"/>
+    <mergeCell ref="M590:M595"/>
+    <mergeCell ref="K592:K595"/>
+    <mergeCell ref="L595:L596"/>
+    <mergeCell ref="M405:M407"/>
+    <mergeCell ref="H16:H49"/>
+    <mergeCell ref="J37:J41"/>
+    <mergeCell ref="H50:H83"/>
+    <mergeCell ref="I296:I300"/>
+    <mergeCell ref="J301:J305"/>
+    <mergeCell ref="I342:I349"/>
+    <mergeCell ref="J350:J357"/>
+    <mergeCell ref="AU428:AU429"/>
+    <mergeCell ref="AU382:AU384"/>
+    <mergeCell ref="K382:K404"/>
+    <mergeCell ref="M419:M427"/>
+    <mergeCell ref="K405:K427"/>
+    <mergeCell ref="AU405:AU407"/>
+    <mergeCell ref="L408:L418"/>
+    <mergeCell ref="K358:K381"/>
+    <mergeCell ref="M382:M384"/>
+    <mergeCell ref="L385:L395"/>
+    <mergeCell ref="M396:M404"/>
+    <mergeCell ref="M358:M360"/>
+    <mergeCell ref="L361:L362"/>
+    <mergeCell ref="AU358:AU362"/>
+    <mergeCell ref="M363:M371"/>
+    <mergeCell ref="L372:L381"/>
+    <mergeCell ref="H116:H147"/>
+    <mergeCell ref="H148:H172"/>
+    <mergeCell ref="H173:H197"/>
+    <mergeCell ref="J173:J181"/>
+    <mergeCell ref="I182:I183"/>
+    <mergeCell ref="AU173:AU183"/>
+    <mergeCell ref="AU116:AU128"/>
+    <mergeCell ref="AU148:AU158"/>
+    <mergeCell ref="I332:I336"/>
+    <mergeCell ref="I316:I323"/>
+    <mergeCell ref="AU226:AU230"/>
+    <mergeCell ref="J226:J228"/>
+    <mergeCell ref="I229:I230"/>
+    <mergeCell ref="AU198:AU202"/>
+    <mergeCell ref="I201:I202"/>
+    <mergeCell ref="J198:J200"/>
+    <mergeCell ref="I203:I212"/>
+    <mergeCell ref="J213:J222"/>
+    <mergeCell ref="I254:I261"/>
+    <mergeCell ref="H84:H115"/>
+    <mergeCell ref="I66:I70"/>
+    <mergeCell ref="J71:J75"/>
+    <mergeCell ref="J130:J136"/>
+    <mergeCell ref="I137:I141"/>
+    <mergeCell ref="J184:J187"/>
+    <mergeCell ref="I188:I197"/>
+    <mergeCell ref="J98:J104"/>
+    <mergeCell ref="I105:I109"/>
+    <mergeCell ref="J148:J156"/>
+    <mergeCell ref="J116:J121"/>
+    <mergeCell ref="I122:I128"/>
+    <mergeCell ref="I157:I158"/>
+    <mergeCell ref="I163:I172"/>
+    <mergeCell ref="J159:J162"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="AU5:AU15"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AA3:AC3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="AU16:AU30"/>
+    <mergeCell ref="AU50:AU64"/>
+    <mergeCell ref="AU84:AU96"/>
+    <mergeCell ref="J16:J23"/>
+    <mergeCell ref="I24:I30"/>
+    <mergeCell ref="I58:I64"/>
+    <mergeCell ref="J84:J89"/>
+    <mergeCell ref="I90:I96"/>
+    <mergeCell ref="J50:J57"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="AU458:AU463"/>
+    <mergeCell ref="AU467:AU472"/>
+    <mergeCell ref="AU476:AU486"/>
+    <mergeCell ref="H198:H225"/>
+    <mergeCell ref="H226:H253"/>
+    <mergeCell ref="I231:I240"/>
+    <mergeCell ref="J241:J250"/>
+    <mergeCell ref="H254:H279"/>
+    <mergeCell ref="H280:H305"/>
+    <mergeCell ref="J337:J340"/>
+    <mergeCell ref="AU332:AU340"/>
+    <mergeCell ref="J324:J331"/>
+    <mergeCell ref="H306:H331"/>
+    <mergeCell ref="H332:H357"/>
+    <mergeCell ref="I270:I274"/>
+    <mergeCell ref="J275:J279"/>
+    <mergeCell ref="AU254:AU268"/>
+    <mergeCell ref="AU280:AU294"/>
+    <mergeCell ref="J288:J294"/>
+    <mergeCell ref="I280:I287"/>
+    <mergeCell ref="J262:J268"/>
+    <mergeCell ref="I306:I310"/>
+    <mergeCell ref="J311:J314"/>
+    <mergeCell ref="AU306:AU314"/>
+    <mergeCell ref="J499:J500"/>
+    <mergeCell ref="AU487:AU500"/>
+    <mergeCell ref="I501:I506"/>
+    <mergeCell ref="J501:J504"/>
+    <mergeCell ref="J505:J506"/>
+    <mergeCell ref="I507:I508"/>
+    <mergeCell ref="J507:J508"/>
+    <mergeCell ref="I509:I510"/>
+    <mergeCell ref="J509:J510"/>
+    <mergeCell ref="K487:K498"/>
+    <mergeCell ref="M487:M489"/>
+    <mergeCell ref="L490:L491"/>
+    <mergeCell ref="M492:M494"/>
+    <mergeCell ref="L495:L496"/>
+    <mergeCell ref="M497:M498"/>
+    <mergeCell ref="J487:J490"/>
+    <mergeCell ref="I487:I492"/>
+    <mergeCell ref="J491:J492"/>
+    <mergeCell ref="J493:J494"/>
+    <mergeCell ref="I493:I494"/>
+    <mergeCell ref="I495:I496"/>
+    <mergeCell ref="J495:J496"/>
+    <mergeCell ref="J497:J498"/>
+    <mergeCell ref="I497:I498"/>
     <mergeCell ref="AV3:AV4"/>
     <mergeCell ref="AV5:AV475"/>
     <mergeCell ref="AV476:AV523"/>
@@ -90084,159 +90357,54 @@
     <mergeCell ref="M521:M522"/>
     <mergeCell ref="AU517:AU523"/>
     <mergeCell ref="I499:I500"/>
-    <mergeCell ref="J499:J500"/>
-    <mergeCell ref="AU487:AU500"/>
-    <mergeCell ref="I501:I506"/>
-    <mergeCell ref="J501:J504"/>
-    <mergeCell ref="J505:J506"/>
-    <mergeCell ref="I507:I508"/>
-    <mergeCell ref="J507:J508"/>
-    <mergeCell ref="I509:I510"/>
-    <mergeCell ref="J509:J510"/>
-    <mergeCell ref="K487:K498"/>
-    <mergeCell ref="M487:M489"/>
-    <mergeCell ref="L490:L491"/>
-    <mergeCell ref="M492:M494"/>
-    <mergeCell ref="L495:L496"/>
-    <mergeCell ref="M497:M498"/>
-    <mergeCell ref="J487:J490"/>
-    <mergeCell ref="I487:I492"/>
-    <mergeCell ref="J491:J492"/>
-    <mergeCell ref="J493:J494"/>
-    <mergeCell ref="I493:I494"/>
-    <mergeCell ref="I495:I496"/>
-    <mergeCell ref="J495:J496"/>
-    <mergeCell ref="J497:J498"/>
-    <mergeCell ref="I497:I498"/>
-    <mergeCell ref="AU458:AU463"/>
-    <mergeCell ref="AU467:AU472"/>
-    <mergeCell ref="AU476:AU486"/>
-    <mergeCell ref="H198:H225"/>
-    <mergeCell ref="H226:H253"/>
-    <mergeCell ref="I231:I240"/>
-    <mergeCell ref="J241:J250"/>
-    <mergeCell ref="H254:H279"/>
-    <mergeCell ref="H280:H305"/>
-    <mergeCell ref="J337:J340"/>
-    <mergeCell ref="AU332:AU340"/>
-    <mergeCell ref="J324:J331"/>
-    <mergeCell ref="H306:H331"/>
-    <mergeCell ref="H332:H357"/>
-    <mergeCell ref="I270:I274"/>
-    <mergeCell ref="J275:J279"/>
-    <mergeCell ref="AU254:AU268"/>
-    <mergeCell ref="AU280:AU294"/>
-    <mergeCell ref="J288:J294"/>
-    <mergeCell ref="I280:I287"/>
-    <mergeCell ref="J262:J268"/>
-    <mergeCell ref="I306:I310"/>
-    <mergeCell ref="J311:J314"/>
-    <mergeCell ref="AU306:AU314"/>
-    <mergeCell ref="AU16:AU30"/>
-    <mergeCell ref="AU50:AU64"/>
-    <mergeCell ref="AU84:AU96"/>
-    <mergeCell ref="J16:J23"/>
-    <mergeCell ref="I24:I30"/>
-    <mergeCell ref="I58:I64"/>
-    <mergeCell ref="J84:J89"/>
-    <mergeCell ref="I90:I96"/>
-    <mergeCell ref="J50:J57"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="AU5:AU15"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="H84:H115"/>
-    <mergeCell ref="I66:I70"/>
-    <mergeCell ref="J71:J75"/>
-    <mergeCell ref="J130:J136"/>
-    <mergeCell ref="I137:I141"/>
-    <mergeCell ref="J184:J187"/>
-    <mergeCell ref="I188:I197"/>
-    <mergeCell ref="J98:J104"/>
-    <mergeCell ref="I105:I109"/>
-    <mergeCell ref="J148:J156"/>
-    <mergeCell ref="J116:J121"/>
-    <mergeCell ref="I122:I128"/>
-    <mergeCell ref="I157:I158"/>
-    <mergeCell ref="I163:I172"/>
-    <mergeCell ref="J159:J162"/>
-    <mergeCell ref="M358:M360"/>
-    <mergeCell ref="L361:L362"/>
-    <mergeCell ref="AU358:AU362"/>
-    <mergeCell ref="M363:M371"/>
-    <mergeCell ref="L372:L381"/>
-    <mergeCell ref="H116:H147"/>
-    <mergeCell ref="H148:H172"/>
-    <mergeCell ref="H173:H197"/>
-    <mergeCell ref="J173:J181"/>
-    <mergeCell ref="I182:I183"/>
-    <mergeCell ref="AU173:AU183"/>
-    <mergeCell ref="AU116:AU128"/>
-    <mergeCell ref="AU148:AU158"/>
-    <mergeCell ref="I332:I336"/>
-    <mergeCell ref="I316:I323"/>
-    <mergeCell ref="AU226:AU230"/>
-    <mergeCell ref="J226:J228"/>
-    <mergeCell ref="I229:I230"/>
-    <mergeCell ref="AU198:AU202"/>
-    <mergeCell ref="I201:I202"/>
-    <mergeCell ref="J198:J200"/>
-    <mergeCell ref="I203:I212"/>
-    <mergeCell ref="J213:J222"/>
-    <mergeCell ref="I254:I261"/>
+    <mergeCell ref="I536:I541"/>
+    <mergeCell ref="J536:J539"/>
+    <mergeCell ref="J540:J541"/>
+    <mergeCell ref="N524:N537"/>
+    <mergeCell ref="L536:L540"/>
+    <mergeCell ref="M536:M537"/>
+    <mergeCell ref="M539:M540"/>
+    <mergeCell ref="AU524:AU541"/>
+    <mergeCell ref="H656:H666"/>
+    <mergeCell ref="L656:L666"/>
+    <mergeCell ref="I534:I535"/>
+    <mergeCell ref="J534:J535"/>
+    <mergeCell ref="K524:K535"/>
+    <mergeCell ref="M524:M526"/>
+    <mergeCell ref="L527:L528"/>
+    <mergeCell ref="M529:M531"/>
+    <mergeCell ref="L532:L533"/>
+    <mergeCell ref="M534:M535"/>
+    <mergeCell ref="K656:K677"/>
+    <mergeCell ref="I656:I671"/>
+    <mergeCell ref="J656:J669"/>
+    <mergeCell ref="M656:M669"/>
+    <mergeCell ref="L670:L672"/>
+    <mergeCell ref="J676:J680"/>
+    <mergeCell ref="AU542:AU594"/>
+    <mergeCell ref="AU656:AU683"/>
+    <mergeCell ref="M672:M674"/>
+    <mergeCell ref="L675:L676"/>
+    <mergeCell ref="I678:I682"/>
+    <mergeCell ref="J681:J682"/>
+    <mergeCell ref="L678:L682"/>
+    <mergeCell ref="M678:M679"/>
+    <mergeCell ref="M681:M682"/>
+    <mergeCell ref="N656:N679"/>
+    <mergeCell ref="J670:J671"/>
+    <mergeCell ref="I672:I673"/>
+    <mergeCell ref="J672:J673"/>
+    <mergeCell ref="J674:J675"/>
+    <mergeCell ref="I674:I675"/>
+    <mergeCell ref="I676:I677"/>
     <mergeCell ref="L554:L556"/>
     <mergeCell ref="M555:M556"/>
     <mergeCell ref="M562:M571"/>
     <mergeCell ref="M572:M573"/>
-    <mergeCell ref="M405:M407"/>
-    <mergeCell ref="H16:H49"/>
-    <mergeCell ref="J37:J41"/>
-    <mergeCell ref="H50:H83"/>
-    <mergeCell ref="I296:I300"/>
-    <mergeCell ref="J301:J305"/>
-    <mergeCell ref="I342:I349"/>
-    <mergeCell ref="J350:J357"/>
-    <mergeCell ref="AU428:AU429"/>
-    <mergeCell ref="AU382:AU384"/>
-    <mergeCell ref="K382:K404"/>
-    <mergeCell ref="M419:M427"/>
-    <mergeCell ref="K405:K427"/>
-    <mergeCell ref="AU405:AU407"/>
-    <mergeCell ref="L408:L418"/>
-    <mergeCell ref="K358:K381"/>
-    <mergeCell ref="M382:M384"/>
-    <mergeCell ref="L385:L395"/>
-    <mergeCell ref="M396:M404"/>
     <mergeCell ref="N578:N581"/>
     <mergeCell ref="N582:N585"/>
     <mergeCell ref="M587:M588"/>
     <mergeCell ref="L562:L566"/>
-    <mergeCell ref="L568:L573"/>
-    <mergeCell ref="K562:K566"/>
-    <mergeCell ref="K568:K571"/>
-    <mergeCell ref="N574:N575"/>
-    <mergeCell ref="N576:N577"/>
-    <mergeCell ref="L587:L588"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Minor Fixes to template; Started on common synonym tests
</commit_message>
<xml_diff>
--- a/AutoTester/Tests/System/System Testing Template.xlsx
+++ b/AutoTester/Tests/System/System Testing Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26494" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26492" uniqueCount="458">
   <si>
     <t>such that</t>
   </si>
@@ -1331,9 +1331,6 @@
     <t>var (v)</t>
   </si>
   <si>
-    <t>c</t>
-  </si>
-  <si>
     <t>v</t>
   </si>
   <si>
@@ -1353,9 +1350,6 @@
   </si>
   <si>
     <t>assign(a)</t>
-  </si>
-  <si>
-    <t>procedure (p)</t>
   </si>
   <si>
     <t>constant (co)</t>
@@ -1455,7 +1449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1507,6 +1501,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFA5CEF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1588,7 +1588,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1662,10 +1662,22 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1674,6 +1686,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFA5CEF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1984,8 +2001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1C4663-D304-44C8-B0BF-D228A95395FB}">
   <dimension ref="B3:AY688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C570" workbookViewId="0">
-      <selection activeCell="C590" sqref="C590"/>
+    <sheetView tabSelected="1" topLeftCell="A566" workbookViewId="0">
+      <selection activeCell="M548" sqref="M548"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64386,7 +64403,7 @@
         <v>44</v>
       </c>
       <c r="N457" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="O457" s="7" t="s">
         <v>44</v>
@@ -64485,7 +64502,7 @@
         <v>44</v>
       </c>
       <c r="AU457" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="AV457" s="9"/>
     </row>
@@ -68677,7 +68694,7 @@
         <v>44</v>
       </c>
       <c r="AU487" s="8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="AV487" s="9"/>
     </row>
@@ -70555,7 +70572,7 @@
         <v>44</v>
       </c>
       <c r="AU501" s="8" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="AV501" s="9"/>
     </row>
@@ -72721,7 +72738,7 @@
         <v>44</v>
       </c>
       <c r="AU517" s="8" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="AV517" s="9"/>
     </row>
@@ -73676,7 +73693,7 @@
         <v>44</v>
       </c>
       <c r="AU524" s="8" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="AV524" s="6"/>
     </row>
@@ -75925,7 +75942,7 @@
       <c r="B542" s="6">
         <v>538</v>
       </c>
-      <c r="C542" s="6" t="s">
+      <c r="C542" s="20" t="s">
         <v>433</v>
       </c>
       <c r="D542" s="7" t="s">
@@ -75943,7 +75960,7 @@
       <c r="H542" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I542" s="6" t="s">
+      <c r="I542" s="20" t="s">
         <v>165</v>
       </c>
       <c r="J542" s="6" t="s">
@@ -76058,7 +76075,7 @@
         <v>44</v>
       </c>
       <c r="AU542" s="8" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="AV542" s="6"/>
     </row>
@@ -76066,7 +76083,7 @@
       <c r="B543" s="6">
         <v>539</v>
       </c>
-      <c r="C543" s="6" t="s">
+      <c r="C543" s="21" t="s">
         <v>431</v>
       </c>
       <c r="D543" s="7" t="s">
@@ -76087,7 +76104,7 @@
       <c r="I543" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J543" s="6" t="s">
+      <c r="J543" s="21" t="s">
         <v>169</v>
       </c>
       <c r="K543" s="7" t="s">
@@ -76205,8 +76222,8 @@
       <c r="B544" s="6">
         <v>540</v>
       </c>
-      <c r="C544" s="6" t="s">
-        <v>437</v>
+      <c r="C544" s="16" t="s">
+        <v>436</v>
       </c>
       <c r="D544" s="7" t="s">
         <v>44</v>
@@ -76223,7 +76240,7 @@
       <c r="H544" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I544" s="6" t="s">
+      <c r="I544" s="16" t="s">
         <v>168</v>
       </c>
       <c r="J544" s="6" t="s">
@@ -76344,8 +76361,8 @@
       <c r="B545" s="6">
         <v>541</v>
       </c>
-      <c r="C545" s="6" t="s">
-        <v>438</v>
+      <c r="C545" s="15" t="s">
+        <v>437</v>
       </c>
       <c r="D545" s="7" t="s">
         <v>44</v>
@@ -76365,7 +76382,7 @@
       <c r="I545" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J545" s="6" t="s">
+      <c r="J545" s="15" t="s">
         <v>167</v>
       </c>
       <c r="K545" s="7" t="s">
@@ -76483,8 +76500,8 @@
       <c r="B546" s="6">
         <v>542</v>
       </c>
-      <c r="C546" s="6" t="s">
-        <v>439</v>
+      <c r="C546" s="30" t="s">
+        <v>438</v>
       </c>
       <c r="D546" s="7" t="s">
         <v>44</v>
@@ -76501,8 +76518,8 @@
       <c r="H546" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I546" s="6" t="s">
-        <v>435</v>
+      <c r="I546" s="30" t="s">
+        <v>245</v>
       </c>
       <c r="J546" s="6" t="s">
         <v>42</v>
@@ -76622,7 +76639,7 @@
       <c r="B547" s="6">
         <v>543</v>
       </c>
-      <c r="C547" s="6" t="s">
+      <c r="C547" s="14" t="s">
         <v>434</v>
       </c>
       <c r="D547" s="7" t="s">
@@ -76643,8 +76660,8 @@
       <c r="I547" s="6">
         <v>1</v>
       </c>
-      <c r="J547" s="6" t="s">
-        <v>436</v>
+      <c r="J547" s="14" t="s">
+        <v>435</v>
       </c>
       <c r="K547" s="7" t="s">
         <v>44</v>
@@ -76761,7 +76778,7 @@
       <c r="B548" s="6">
         <v>544</v>
       </c>
-      <c r="C548" s="6" t="s">
+      <c r="C548" s="17" t="s">
         <v>432</v>
       </c>
       <c r="D548" s="7" t="s">
@@ -76779,7 +76796,7 @@
       <c r="H548" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I548" s="6" t="s">
+      <c r="I548" s="17" t="s">
         <v>199</v>
       </c>
       <c r="J548" s="6" t="s">
@@ -76900,7 +76917,7 @@
       <c r="B549" s="6">
         <v>545</v>
       </c>
-      <c r="C549" s="6" t="s">
+      <c r="C549" s="17" t="s">
         <v>432</v>
       </c>
       <c r="D549" s="7" t="s">
@@ -76921,7 +76938,7 @@
       <c r="I549" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J549" s="6" t="s">
+      <c r="J549" s="17" t="s">
         <v>199</v>
       </c>
       <c r="K549" s="7" t="s">
@@ -77039,7 +77056,7 @@
       <c r="B550" s="6">
         <v>546</v>
       </c>
-      <c r="C550" s="6" t="s">
+      <c r="C550" s="21" t="s">
         <v>431</v>
       </c>
       <c r="D550" s="7" t="s">
@@ -77057,7 +77074,7 @@
       <c r="H550" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I550" s="6" t="s">
+      <c r="I550" s="21" t="s">
         <v>169</v>
       </c>
       <c r="J550" s="6" t="s">
@@ -77178,7 +77195,7 @@
       <c r="B551" s="6">
         <v>547</v>
       </c>
-      <c r="C551" s="6" t="s">
+      <c r="C551" s="20" t="s">
         <v>433</v>
       </c>
       <c r="D551" s="7" t="s">
@@ -77199,7 +77216,7 @@
       <c r="I551" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J551" s="6" t="s">
+      <c r="J551" s="20" t="s">
         <v>165</v>
       </c>
       <c r="K551" s="7" t="s">
@@ -77317,7 +77334,7 @@
       <c r="B552" s="6">
         <v>548</v>
       </c>
-      <c r="C552" s="6" t="s">
+      <c r="C552" s="20" t="s">
         <v>433</v>
       </c>
       <c r="D552" s="7" t="s">
@@ -77335,7 +77352,7 @@
       <c r="H552" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I552" s="6" t="s">
+      <c r="I552" s="20" t="s">
         <v>165</v>
       </c>
       <c r="J552" s="6" t="s">
@@ -77456,8 +77473,8 @@
       <c r="B553" s="6">
         <v>549</v>
       </c>
-      <c r="C553" s="6" t="s">
-        <v>442</v>
+      <c r="C553" s="12" t="s">
+        <v>441</v>
       </c>
       <c r="D553" s="7" t="s">
         <v>44</v>
@@ -77477,7 +77494,7 @@
       <c r="I553" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J553" s="6" t="s">
+      <c r="J553" s="12" t="s">
         <v>166</v>
       </c>
       <c r="K553" s="7" t="s">
@@ -77595,7 +77612,7 @@
       <c r="B554" s="6">
         <v>550</v>
       </c>
-      <c r="C554" s="6" t="s">
+      <c r="C554" s="25" t="s">
         <v>434</v>
       </c>
       <c r="D554" s="7" t="s">
@@ -77622,8 +77639,8 @@
       <c r="K554" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L554" s="8" t="s">
-        <v>436</v>
+      <c r="L554" s="25" t="s">
+        <v>435</v>
       </c>
       <c r="M554" s="6" t="s">
         <v>52</v>
@@ -77734,9 +77751,7 @@
       <c r="B555" s="6">
         <v>551</v>
       </c>
-      <c r="C555" s="6" t="s">
-        <v>434</v>
-      </c>
+      <c r="C555" s="29"/>
       <c r="D555" s="7" t="s">
         <v>44</v>
       </c>
@@ -77761,7 +77776,7 @@
       <c r="K555" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L555" s="9"/>
+      <c r="L555" s="29"/>
       <c r="M555" s="8" t="s">
         <v>62</v>
       </c>
@@ -77871,9 +77886,7 @@
       <c r="B556" s="6">
         <v>552</v>
       </c>
-      <c r="C556" s="6" t="s">
-        <v>434</v>
-      </c>
+      <c r="C556" s="26"/>
       <c r="D556" s="7" t="s">
         <v>44</v>
       </c>
@@ -77898,7 +77911,7 @@
       <c r="K556" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L556" s="11"/>
+      <c r="L556" s="26"/>
       <c r="M556" s="11"/>
       <c r="N556" s="7" t="s">
         <v>44</v>
@@ -78006,8 +78019,8 @@
       <c r="B557" s="6">
         <v>553</v>
       </c>
-      <c r="C557" s="6" t="s">
-        <v>443</v>
+      <c r="C557" s="17" t="s">
+        <v>432</v>
       </c>
       <c r="D557" s="7" t="s">
         <v>44</v>
@@ -78039,7 +78052,7 @@
       <c r="M557" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N557" s="6" t="s">
+      <c r="N557" s="17" t="s">
         <v>338</v>
       </c>
       <c r="O557" s="7" t="s">
@@ -78145,7 +78158,7 @@
       <c r="B558" s="6">
         <v>554</v>
       </c>
-      <c r="C558" s="6" t="s">
+      <c r="C558" s="14" t="s">
         <v>434</v>
       </c>
       <c r="D558" s="7" t="s">
@@ -78178,8 +78191,8 @@
       <c r="M558" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N558" s="6" t="s">
-        <v>445</v>
+      <c r="N558" s="14" t="s">
+        <v>443</v>
       </c>
       <c r="O558" s="7" t="s">
         <v>44</v>
@@ -78284,8 +78297,8 @@
       <c r="B559" s="6">
         <v>555</v>
       </c>
-      <c r="C559" s="6" t="s">
-        <v>444</v>
+      <c r="C559" s="22" t="s">
+        <v>442</v>
       </c>
       <c r="D559" s="7" t="s">
         <v>44</v>
@@ -78317,7 +78330,7 @@
       <c r="M559" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N559" s="6" t="s">
+      <c r="N559" s="22" t="s">
         <v>377</v>
       </c>
       <c r="O559" s="7" t="s">
@@ -78423,7 +78436,7 @@
       <c r="B560" s="6">
         <v>556</v>
       </c>
-      <c r="C560" s="6" t="s">
+      <c r="C560" s="20" t="s">
         <v>433</v>
       </c>
       <c r="D560" s="7" t="s">
@@ -78456,7 +78469,7 @@
       <c r="M560" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N560" s="6" t="s">
+      <c r="N560" s="20" t="s">
         <v>424</v>
       </c>
       <c r="O560" s="7" t="s">
@@ -78562,7 +78575,7 @@
       <c r="B561" s="6">
         <v>557</v>
       </c>
-      <c r="C561" s="6" t="s">
+      <c r="C561" s="21" t="s">
         <v>431</v>
       </c>
       <c r="D561" s="7" t="s">
@@ -78595,8 +78608,8 @@
       <c r="M561" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N561" s="6" t="s">
-        <v>446</v>
+      <c r="N561" s="21" t="s">
+        <v>444</v>
       </c>
       <c r="O561" s="7" t="s">
         <v>44</v>
@@ -78720,7 +78733,7 @@
         <v>24</v>
       </c>
       <c r="I562" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J562" s="6" t="s">
         <v>37</v>
@@ -78860,7 +78873,7 @@
         <v>37</v>
       </c>
       <c r="J563" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K563" s="13"/>
       <c r="L563" s="2"/>
@@ -78991,7 +79004,7 @@
         <v>168</v>
       </c>
       <c r="J564" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K564" s="13"/>
       <c r="L564" s="2"/>
@@ -79122,7 +79135,7 @@
         <v>40</v>
       </c>
       <c r="J565" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K565" s="13"/>
       <c r="L565" s="2"/>
@@ -79250,7 +79263,7 @@
         <v>28</v>
       </c>
       <c r="I566" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J566" s="6" t="s">
         <v>42</v>
@@ -79390,7 +79403,7 @@
         <v>38</v>
       </c>
       <c r="L567" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M567" s="2"/>
       <c r="N567" s="7" t="s">
@@ -79519,7 +79532,7 @@
         <v>43</v>
       </c>
       <c r="J568" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K568" s="13" t="s">
         <v>166</v>
@@ -79651,7 +79664,7 @@
         <v>33</v>
       </c>
       <c r="I569" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J569" s="6" t="s">
         <v>43</v>
@@ -79782,7 +79795,7 @@
         <v>34</v>
       </c>
       <c r="I570" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J570" s="6" t="s">
         <v>37</v>
@@ -79916,7 +79929,7 @@
         <v>37</v>
       </c>
       <c r="J571" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K571" s="13"/>
       <c r="L571" s="2"/>
@@ -80044,7 +80057,7 @@
         <v>24</v>
       </c>
       <c r="I572" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J572" s="6" t="s">
         <v>37</v>
@@ -80182,7 +80195,7 @@
         <v>37</v>
       </c>
       <c r="J573" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="K573" s="16" t="s">
         <v>168</v>
@@ -80599,7 +80612,7 @@
         <v>44</v>
       </c>
       <c r="N576" s="19" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="O576" s="7" t="s">
         <v>44</v>
@@ -80868,7 +80881,7 @@
       <c r="M578" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N578" s="25" t="s">
+      <c r="N578" s="27" t="s">
         <v>424</v>
       </c>
       <c r="O578" s="7" t="s">
@@ -81005,7 +81018,7 @@
       <c r="M579" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N579" s="25"/>
+      <c r="N579" s="27"/>
       <c r="O579" s="7" t="s">
         <v>44</v>
       </c>
@@ -81140,7 +81153,7 @@
       <c r="M580" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N580" s="25"/>
+      <c r="N580" s="27"/>
       <c r="O580" s="7" t="s">
         <v>44</v>
       </c>
@@ -81275,7 +81288,7 @@
       <c r="M581" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N581" s="25"/>
+      <c r="N581" s="27"/>
       <c r="O581" s="7" t="s">
         <v>44</v>
       </c>
@@ -81410,8 +81423,8 @@
       <c r="M582" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N582" s="26" t="s">
-        <v>446</v>
+      <c r="N582" s="28" t="s">
+        <v>444</v>
       </c>
       <c r="O582" s="7" t="s">
         <v>44</v>
@@ -81547,7 +81560,7 @@
       <c r="M583" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N583" s="26"/>
+      <c r="N583" s="28"/>
       <c r="O583" s="7" t="s">
         <v>44</v>
       </c>
@@ -81682,7 +81695,7 @@
       <c r="M584" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N584" s="26"/>
+      <c r="N584" s="28"/>
       <c r="O584" s="7" t="s">
         <v>44</v>
       </c>
@@ -81817,7 +81830,7 @@
       <c r="M585" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N585" s="26"/>
+      <c r="N585" s="28"/>
       <c r="O585" s="7" t="s">
         <v>44</v>
       </c>
@@ -81953,7 +81966,7 @@
         <v>52</v>
       </c>
       <c r="N586" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="O586" s="7" t="s">
         <v>44</v>
@@ -82081,7 +82094,7 @@
         <v>44</v>
       </c>
       <c r="K587" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="L587" s="2" t="s">
         <v>42</v>
@@ -82218,7 +82231,7 @@
         <v>44</v>
       </c>
       <c r="K588" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="L588" s="2"/>
       <c r="M588" s="2"/>
@@ -82329,7 +82342,7 @@
         <v>585</v>
       </c>
       <c r="C589" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D589" s="7" t="s">
         <v>44</v>
@@ -82347,7 +82360,7 @@
         <v>24</v>
       </c>
       <c r="I589" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J589" s="6" t="s">
         <v>37</v>
@@ -82362,7 +82375,7 @@
         <v>52</v>
       </c>
       <c r="N589" s="14" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="O589" s="7" t="s">
         <v>44</v>
@@ -82468,7 +82481,7 @@
         <v>586</v>
       </c>
       <c r="C590" s="15" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D590" s="7" t="s">
         <v>44</v>
@@ -82501,7 +82514,7 @@
         <v>62</v>
       </c>
       <c r="N590" s="20" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="O590" s="7" t="s">
         <v>44</v>
@@ -82607,7 +82620,7 @@
         <v>587</v>
       </c>
       <c r="C591" s="22" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D591" s="7" t="s">
         <v>44</v>
@@ -82632,11 +82645,11 @@
         <v>41</v>
       </c>
       <c r="L591" s="14" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M591" s="2"/>
       <c r="N591" s="22" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="O591" s="7" t="s">
         <v>44</v>
@@ -82742,7 +82755,7 @@
         <v>588</v>
       </c>
       <c r="C592" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D592" s="7" t="s">
         <v>44</v>
@@ -82773,7 +82786,7 @@
       </c>
       <c r="M592" s="2"/>
       <c r="N592" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="O592" s="7" t="s">
         <v>44</v>
@@ -82900,7 +82913,7 @@
       <c r="L593" s="2"/>
       <c r="M593" s="2"/>
       <c r="N593" s="16" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="O593" s="7"/>
       <c r="P593" s="7"/>
@@ -82942,7 +82955,7 @@
         <v>589</v>
       </c>
       <c r="C594" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D594" s="7" t="s">
         <v>44</v>
@@ -82965,7 +82978,7 @@
       <c r="L594" s="2"/>
       <c r="M594" s="2"/>
       <c r="N594" s="16" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="O594" s="7" t="s">
         <v>44</v>
@@ -83089,14 +83102,14 @@
         <v>28</v>
       </c>
       <c r="I595" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J595" s="19" t="s">
         <v>434</v>
       </c>
       <c r="K595" s="24"/>
       <c r="L595" s="19" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="M595" s="2"/>
       <c r="N595" s="6" t="s">
@@ -83199,7 +83212,7 @@
         <v>44</v>
       </c>
       <c r="AU595" s="8" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="AV595" s="6"/>
     </row>
@@ -83224,7 +83237,7 @@
         <v>29</v>
       </c>
       <c r="I596" s="12" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J596" s="19"/>
       <c r="K596" s="12" t="s">
@@ -83235,7 +83248,7 @@
         <v>52</v>
       </c>
       <c r="N596" s="6" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="O596" s="7" t="s">
         <v>44</v>
@@ -90175,8 +90188,9 @@
       <c r="AV688" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="229">
+  <mergeCells count="230">
     <mergeCell ref="AU595:AU596"/>
+    <mergeCell ref="C554:C556"/>
     <mergeCell ref="J576:J577"/>
     <mergeCell ref="I592:I594"/>
     <mergeCell ref="J595:J596"/>

</xml_diff>

<commit_message>
Finished With Test Cases 1
</commit_message>
<xml_diff>
--- a/AutoTester/Tests/System/System Testing Template.xlsx
+++ b/AutoTester/Tests/System/System Testing Template.xlsx
@@ -1451,9 +1451,6 @@
     <t>1=s.stmt#</t>
   </si>
   <si>
-    <t>2=co.value#</t>
-  </si>
-  <si>
     <t>With String-Attribute Test Cases</t>
   </si>
   <si>
@@ -1515,6 +1512,9 @@
   </si>
   <si>
     <t>1=1</t>
+  </si>
+  <si>
+    <t>2=co.value</t>
   </si>
 </sst>
 </file>
@@ -1758,7 +1758,19 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1785,21 +1797,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1807,6 +1804,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2130,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1C4663-D304-44C8-B0BF-D228A95395FB}">
   <dimension ref="B3:AY688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A414" workbookViewId="0">
-      <selection activeCell="C414" sqref="C414"/>
+    <sheetView tabSelected="1" topLeftCell="K465" workbookViewId="0">
+      <selection activeCell="N487" sqref="N487"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68261,7 +68261,7 @@
         <v>44</v>
       </c>
       <c r="AU483" s="8" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AV483" s="2"/>
     </row>
@@ -68541,7 +68541,7 @@
         <v>44</v>
       </c>
       <c r="AU485" s="8" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AV485" s="2"/>
     </row>
@@ -68583,7 +68583,7 @@
         <v>44</v>
       </c>
       <c r="N486" s="6" t="s">
-        <v>475</v>
+        <v>496</v>
       </c>
       <c r="O486" s="7" t="s">
         <v>44</v>
@@ -68722,7 +68722,7 @@
         <v>44</v>
       </c>
       <c r="N487" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="O487" s="7" t="s">
         <v>44</v>
@@ -68821,7 +68821,7 @@
         <v>44</v>
       </c>
       <c r="AU487" s="8" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AV487" s="2"/>
     </row>
@@ -68863,7 +68863,7 @@
         <v>44</v>
       </c>
       <c r="N488" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="O488" s="7" t="s">
         <v>44</v>
@@ -69002,106 +69002,106 @@
         <v>44</v>
       </c>
       <c r="N489" s="6" t="s">
+        <v>480</v>
+      </c>
+      <c r="O489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="W489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT489" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU489" s="6" t="s">
         <v>481</v>
-      </c>
-      <c r="O489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="P489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="R489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="S489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="T489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="U489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="V489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="W489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="X489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT489" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU489" s="6" t="s">
-        <v>482</v>
       </c>
       <c r="AV489" s="2"/>
     </row>
@@ -69143,7 +69143,7 @@
         <v>44</v>
       </c>
       <c r="N490" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="O490" s="7" t="s">
         <v>44</v>
@@ -69242,7 +69242,7 @@
         <v>44</v>
       </c>
       <c r="AU490" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="AV490" s="2"/>
     </row>
@@ -69284,7 +69284,7 @@
         <v>44</v>
       </c>
       <c r="N491" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="O491" s="7" t="s">
         <v>44</v>
@@ -69383,7 +69383,7 @@
         <v>44</v>
       </c>
       <c r="AU491" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="AV491" s="2"/>
     </row>
@@ -69425,7 +69425,7 @@
         <v>44</v>
       </c>
       <c r="N492" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="O492" s="7" t="s">
         <v>44</v>
@@ -69524,7 +69524,7 @@
         <v>44</v>
       </c>
       <c r="AU492" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="AV492" s="2"/>
     </row>
@@ -69566,106 +69566,106 @@
         <v>44</v>
       </c>
       <c r="N493" s="6" t="s">
+        <v>488</v>
+      </c>
+      <c r="O493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="P493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="R493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="S493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="T493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="U493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="V493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="W493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="X493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AL493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AM493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AO493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AR493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AS493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT493" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AU493" s="6" t="s">
         <v>489</v>
-      </c>
-      <c r="O493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="P493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="R493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="S493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="T493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="U493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="V493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="W493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="X493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AA493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AB493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AE493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AJ493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AK493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AS493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT493" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="AU493" s="6" t="s">
-        <v>490</v>
       </c>
       <c r="AV493" s="2"/>
     </row>
@@ -69707,7 +69707,7 @@
         <v>44</v>
       </c>
       <c r="N494" s="6" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="O494" s="7" t="s">
         <v>44</v>
@@ -69806,7 +69806,7 @@
         <v>44</v>
       </c>
       <c r="AU494" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="AV494" s="2"/>
     </row>
@@ -69848,7 +69848,7 @@
         <v>44</v>
       </c>
       <c r="N495" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="O495" s="7" t="s">
         <v>44</v>
@@ -69947,7 +69947,7 @@
         <v>44</v>
       </c>
       <c r="AU495" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="AV495" s="2"/>
     </row>
@@ -69989,7 +69989,7 @@
         <v>44</v>
       </c>
       <c r="N496" s="6" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="O496" s="7" t="s">
         <v>44</v>
@@ -70088,7 +70088,7 @@
         <v>44</v>
       </c>
       <c r="AU496" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="AV496" s="2"/>
     </row>
@@ -80827,7 +80827,7 @@
       <c r="B582" s="6">
         <v>578</v>
       </c>
-      <c r="C582" s="28" t="s">
+      <c r="C582" s="18" t="s">
         <v>420</v>
       </c>
       <c r="D582" s="7" t="s">
@@ -80845,7 +80845,7 @@
       <c r="H582" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I582" s="18" t="s">
+      <c r="I582" s="19" t="s">
         <v>199</v>
       </c>
       <c r="J582" s="6" t="s">
@@ -80966,7 +80966,7 @@
       <c r="B583" s="6">
         <v>579</v>
       </c>
-      <c r="C583" s="29"/>
+      <c r="C583" s="20"/>
       <c r="D583" s="7" t="s">
         <v>44</v>
       </c>
@@ -80985,7 +80985,7 @@
       <c r="I583" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J583" s="18" t="s">
+      <c r="J583" s="19" t="s">
         <v>199</v>
       </c>
       <c r="K583" s="7" t="s">
@@ -81242,7 +81242,7 @@
       <c r="B585" s="6">
         <v>581</v>
       </c>
-      <c r="C585" s="30" t="s">
+      <c r="C585" s="21" t="s">
         <v>421</v>
       </c>
       <c r="D585" s="7" t="s">
@@ -81381,7 +81381,7 @@
       <c r="B586" s="6">
         <v>582</v>
       </c>
-      <c r="C586" s="31"/>
+      <c r="C586" s="22"/>
       <c r="D586" s="7" t="s">
         <v>44</v>
       </c>
@@ -81518,7 +81518,7 @@
       <c r="B587" s="6">
         <v>583</v>
       </c>
-      <c r="C587" s="19" t="s">
+      <c r="C587" s="23" t="s">
         <v>429</v>
       </c>
       <c r="D587" s="7" t="s">
@@ -81539,7 +81539,7 @@
       <c r="I587" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J587" s="19" t="s">
+      <c r="J587" s="23" t="s">
         <v>166</v>
       </c>
       <c r="K587" s="7" t="s">
@@ -81657,7 +81657,7 @@
       <c r="B588" s="6">
         <v>584</v>
       </c>
-      <c r="C588" s="20" t="s">
+      <c r="C588" s="24" t="s">
         <v>422</v>
       </c>
       <c r="D588" s="7" t="s">
@@ -81684,7 +81684,7 @@
       <c r="K588" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L588" s="20" t="s">
+      <c r="L588" s="24" t="s">
         <v>423</v>
       </c>
       <c r="M588" s="6" t="s">
@@ -81796,7 +81796,7 @@
       <c r="B589" s="6">
         <v>585</v>
       </c>
-      <c r="C589" s="21"/>
+      <c r="C589" s="25"/>
       <c r="D589" s="7" t="s">
         <v>44</v>
       </c>
@@ -81821,7 +81821,7 @@
       <c r="K589" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L589" s="21"/>
+      <c r="L589" s="25"/>
       <c r="M589" s="6" t="s">
         <v>62</v>
       </c>
@@ -81931,7 +81931,7 @@
       <c r="B590" s="6">
         <v>586</v>
       </c>
-      <c r="C590" s="22"/>
+      <c r="C590" s="26"/>
       <c r="D590" s="7" t="s">
         <v>44</v>
       </c>
@@ -81956,7 +81956,7 @@
       <c r="K590" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L590" s="22"/>
+      <c r="L590" s="26"/>
       <c r="M590" s="6"/>
       <c r="N590" s="7" t="s">
         <v>44</v>
@@ -82064,7 +82064,7 @@
       <c r="B591" s="6">
         <v>587</v>
       </c>
-      <c r="C591" s="18" t="s">
+      <c r="C591" s="19" t="s">
         <v>420</v>
       </c>
       <c r="D591" s="7" t="s">
@@ -82097,7 +82097,7 @@
       <c r="M591" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N591" s="18" t="s">
+      <c r="N591" s="19" t="s">
         <v>338</v>
       </c>
       <c r="O591" s="7" t="s">
@@ -82340,7 +82340,7 @@
     </row>
     <row r="593" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B593" s="6"/>
-      <c r="C593" s="23" t="s">
+      <c r="C593" s="27" t="s">
         <v>430</v>
       </c>
       <c r="D593" s="7" t="s">
@@ -82373,7 +82373,7 @@
       <c r="M593" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N593" s="23" t="s">
+      <c r="N593" s="27" t="s">
         <v>377</v>
       </c>
       <c r="O593" s="7" t="s">
@@ -82775,13 +82775,13 @@
       <c r="H596" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I596" s="19" t="s">
+      <c r="I596" s="23" t="s">
         <v>433</v>
       </c>
       <c r="J596" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K596" s="24" t="s">
+      <c r="K596" s="28" t="s">
         <v>166</v>
       </c>
       <c r="L596" s="8" t="s">
@@ -82915,10 +82915,10 @@
       <c r="I597" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J597" s="24" t="s">
+      <c r="J597" s="28" t="s">
         <v>433</v>
       </c>
-      <c r="K597" s="25"/>
+      <c r="K597" s="29"/>
       <c r="L597" s="9"/>
       <c r="M597" s="9"/>
       <c r="N597" s="7" t="s">
@@ -83046,8 +83046,8 @@
       <c r="I598" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="J598" s="25"/>
-      <c r="K598" s="25"/>
+      <c r="J598" s="29"/>
+      <c r="K598" s="29"/>
       <c r="L598" s="9"/>
       <c r="M598" s="9"/>
       <c r="N598" s="7" t="s">
@@ -83175,8 +83175,8 @@
       <c r="I599" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="J599" s="26"/>
-      <c r="K599" s="25"/>
+      <c r="J599" s="30"/>
+      <c r="K599" s="29"/>
       <c r="L599" s="9"/>
       <c r="M599" s="9"/>
       <c r="N599" s="7" t="s">
@@ -83301,13 +83301,13 @@
       <c r="H600" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I600" s="19" t="s">
+      <c r="I600" s="23" t="s">
         <v>433</v>
       </c>
       <c r="J600" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K600" s="26"/>
+      <c r="K600" s="30"/>
       <c r="L600" s="11"/>
       <c r="M600" s="9"/>
       <c r="N600" s="7" t="s">
@@ -83570,10 +83570,10 @@
       <c r="I602" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J602" s="19" t="s">
+      <c r="J602" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="K602" s="24" t="s">
+      <c r="K602" s="28" t="s">
         <v>166</v>
       </c>
       <c r="L602" s="8" t="s">
@@ -83702,13 +83702,13 @@
       <c r="H603" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I603" s="24" t="s">
+      <c r="I603" s="28" t="s">
         <v>433</v>
       </c>
       <c r="J603" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="K603" s="25"/>
+      <c r="K603" s="29"/>
       <c r="L603" s="9"/>
       <c r="M603" s="9"/>
       <c r="N603" s="7" t="s">
@@ -83833,11 +83833,11 @@
       <c r="H604" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I604" s="26"/>
+      <c r="I604" s="30"/>
       <c r="J604" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K604" s="25"/>
+      <c r="K604" s="29"/>
       <c r="L604" s="9"/>
       <c r="M604" s="9"/>
       <c r="N604" s="7" t="s">
@@ -83965,10 +83965,10 @@
       <c r="I605" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J605" s="19" t="s">
+      <c r="J605" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="K605" s="26"/>
+      <c r="K605" s="30"/>
       <c r="L605" s="9"/>
       <c r="M605" s="11"/>
       <c r="N605" s="7" t="s">
@@ -84361,7 +84361,7 @@
       <c r="H608" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I608" s="18" t="s">
+      <c r="I608" s="19" t="s">
         <v>420</v>
       </c>
       <c r="J608" s="6" t="s">
@@ -84376,7 +84376,7 @@
       <c r="M608" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N608" s="18" t="s">
+      <c r="N608" s="19" t="s">
         <v>338</v>
       </c>
       <c r="O608" s="7" t="s">
@@ -84501,7 +84501,7 @@
       <c r="I609" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J609" s="18" t="s">
+      <c r="J609" s="19" t="s">
         <v>420</v>
       </c>
       <c r="K609" s="7" t="s">
@@ -84513,7 +84513,7 @@
       <c r="M609" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N609" s="18"/>
+      <c r="N609" s="19"/>
       <c r="O609" s="7" t="s">
         <v>44</v>
       </c>
@@ -84634,7 +84634,7 @@
         <v>28</v>
       </c>
       <c r="I610" s="9"/>
-      <c r="J610" s="20" t="s">
+      <c r="J610" s="24" t="s">
         <v>422</v>
       </c>
       <c r="K610" s="7" t="s">
@@ -84769,7 +84769,7 @@
         <v>29</v>
       </c>
       <c r="I611" s="11"/>
-      <c r="J611" s="22"/>
+      <c r="J611" s="26"/>
       <c r="K611" s="7" t="s">
         <v>44</v>
       </c>
@@ -86374,7 +86374,7 @@
       <c r="B623" s="6">
         <v>618</v>
       </c>
-      <c r="C623" s="19" t="s">
+      <c r="C623" s="23" t="s">
         <v>433</v>
       </c>
       <c r="D623" s="7" t="s">
@@ -86392,7 +86392,7 @@
       <c r="H623" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I623" s="19" t="s">
+      <c r="I623" s="23" t="s">
         <v>433</v>
       </c>
       <c r="J623" s="6" t="s">
@@ -86654,7 +86654,7 @@
       <c r="B625" s="6">
         <v>620</v>
       </c>
-      <c r="C625" s="23" t="s">
+      <c r="C625" s="27" t="s">
         <v>430</v>
       </c>
       <c r="D625" s="7" t="s">
@@ -86683,7 +86683,7 @@
         <v>423</v>
       </c>
       <c r="M625" s="9"/>
-      <c r="N625" s="23" t="s">
+      <c r="N625" s="27" t="s">
         <v>435</v>
       </c>
       <c r="O625" s="7" t="s">
@@ -86807,13 +86807,13 @@
       <c r="H626" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I626" s="32" t="s">
+      <c r="I626" s="31" t="s">
         <v>168</v>
       </c>
       <c r="J626" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K626" s="32" t="s">
+      <c r="K626" s="31" t="s">
         <v>168</v>
       </c>
       <c r="L626" s="8" t="s">
@@ -86944,9 +86944,9 @@
       <c r="H627" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I627" s="33"/>
+      <c r="I627" s="32"/>
       <c r="J627" s="9"/>
-      <c r="K627" s="33"/>
+      <c r="K627" s="32"/>
       <c r="L627" s="9"/>
       <c r="M627" s="9"/>
       <c r="N627" s="14" t="s">
@@ -87073,9 +87073,9 @@
       <c r="H628" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I628" s="34"/>
+      <c r="I628" s="33"/>
       <c r="J628" s="11"/>
-      <c r="K628" s="33"/>
+      <c r="K628" s="32"/>
       <c r="L628" s="11"/>
       <c r="M628" s="9"/>
       <c r="N628" s="14" t="s">
@@ -87205,11 +87205,11 @@
       <c r="I629" s="14" t="s">
         <v>424</v>
       </c>
-      <c r="J629" s="20" t="s">
+      <c r="J629" s="24" t="s">
         <v>422</v>
       </c>
-      <c r="K629" s="34"/>
-      <c r="L629" s="20" t="s">
+      <c r="K629" s="33"/>
+      <c r="L629" s="24" t="s">
         <v>423</v>
       </c>
       <c r="M629" s="11"/>
@@ -87337,14 +87337,14 @@
       <c r="H630" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I630" s="19" t="s">
+      <c r="I630" s="23" t="s">
         <v>433</v>
       </c>
-      <c r="J630" s="22"/>
-      <c r="K630" s="19" t="s">
+      <c r="J630" s="26"/>
+      <c r="K630" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="L630" s="22"/>
+      <c r="L630" s="26"/>
       <c r="M630" s="6" t="s">
         <v>52</v>
       </c>
@@ -88213,7 +88213,7 @@
       <c r="AS645" s="6"/>
       <c r="AT645" s="6"/>
       <c r="AU645" s="6"/>
-      <c r="AV645" s="27"/>
+      <c r="AV645" s="34"/>
     </row>
     <row r="646" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B646" s="6">
@@ -88264,7 +88264,7 @@
       <c r="AS646" s="6"/>
       <c r="AT646" s="6"/>
       <c r="AU646" s="6"/>
-      <c r="AV646" s="27"/>
+      <c r="AV646" s="34"/>
     </row>
     <row r="647" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B647" s="6">
@@ -88315,7 +88315,7 @@
       <c r="AS647" s="6"/>
       <c r="AT647" s="6"/>
       <c r="AU647" s="6"/>
-      <c r="AV647" s="27"/>
+      <c r="AV647" s="34"/>
     </row>
     <row r="648" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B648" s="6">
@@ -88366,7 +88366,7 @@
       <c r="AS648" s="6"/>
       <c r="AT648" s="6"/>
       <c r="AU648" s="6"/>
-      <c r="AV648" s="27"/>
+      <c r="AV648" s="34"/>
     </row>
     <row r="649" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B649" s="6">
@@ -88417,7 +88417,7 @@
       <c r="AS649" s="6"/>
       <c r="AT649" s="6"/>
       <c r="AU649" s="6"/>
-      <c r="AV649" s="27"/>
+      <c r="AV649" s="34"/>
     </row>
     <row r="650" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B650" s="6">
@@ -88468,7 +88468,7 @@
       <c r="AS650" s="6"/>
       <c r="AT650" s="6"/>
       <c r="AU650" s="6"/>
-      <c r="AV650" s="27"/>
+      <c r="AV650" s="34"/>
     </row>
     <row r="651" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B651" s="6">
@@ -88519,7 +88519,7 @@
       <c r="AS651" s="6"/>
       <c r="AT651" s="6"/>
       <c r="AU651" s="6"/>
-      <c r="AV651" s="27"/>
+      <c r="AV651" s="34"/>
     </row>
     <row r="652" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B652" s="6">
@@ -88570,7 +88570,7 @@
       <c r="AS652" s="6"/>
       <c r="AT652" s="6"/>
       <c r="AU652" s="6"/>
-      <c r="AV652" s="27"/>
+      <c r="AV652" s="34"/>
     </row>
     <row r="653" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B653" s="6">
@@ -88621,7 +88621,7 @@
       <c r="AS653" s="6"/>
       <c r="AT653" s="6"/>
       <c r="AU653" s="6"/>
-      <c r="AV653" s="27"/>
+      <c r="AV653" s="34"/>
     </row>
     <row r="654" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B654" s="6">
@@ -88672,7 +88672,7 @@
       <c r="AS654" s="6"/>
       <c r="AT654" s="6"/>
       <c r="AU654" s="6"/>
-      <c r="AV654" s="27"/>
+      <c r="AV654" s="34"/>
     </row>
     <row r="655" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B655" s="6">
@@ -88723,7 +88723,7 @@
       <c r="AS655" s="6"/>
       <c r="AT655" s="6"/>
       <c r="AU655" s="6"/>
-      <c r="AV655" s="27"/>
+      <c r="AV655" s="34"/>
     </row>
     <row r="656" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B656" s="6">
@@ -92556,33 +92556,124 @@
     </row>
   </sheetData>
   <mergeCells count="169">
-    <mergeCell ref="K626:K629"/>
-    <mergeCell ref="J626:J628"/>
-    <mergeCell ref="J629:J630"/>
-    <mergeCell ref="I626:I628"/>
-    <mergeCell ref="I624:I625"/>
-    <mergeCell ref="C596:C622"/>
-    <mergeCell ref="L596:L600"/>
-    <mergeCell ref="M596:M605"/>
-    <mergeCell ref="L602:L607"/>
-    <mergeCell ref="M606:M607"/>
-    <mergeCell ref="K602:K605"/>
-    <mergeCell ref="I603:I604"/>
-    <mergeCell ref="J597:J599"/>
-    <mergeCell ref="K596:K600"/>
-    <mergeCell ref="J610:J611"/>
-    <mergeCell ref="I609:I611"/>
-    <mergeCell ref="AU467:AU478"/>
-    <mergeCell ref="AU479:AU482"/>
-    <mergeCell ref="AU485:AU486"/>
-    <mergeCell ref="AU483:AU484"/>
-    <mergeCell ref="AU487:AU488"/>
-    <mergeCell ref="M624:M629"/>
-    <mergeCell ref="M621:M622"/>
-    <mergeCell ref="L621:L622"/>
-    <mergeCell ref="L626:L628"/>
-    <mergeCell ref="L629:L630"/>
-    <mergeCell ref="L588:L590"/>
+    <mergeCell ref="M405:M407"/>
+    <mergeCell ref="H16:H49"/>
+    <mergeCell ref="J37:J41"/>
+    <mergeCell ref="H50:H83"/>
+    <mergeCell ref="I296:I300"/>
+    <mergeCell ref="J301:J305"/>
+    <mergeCell ref="I342:I349"/>
+    <mergeCell ref="J350:J357"/>
+    <mergeCell ref="AU428:AU429"/>
+    <mergeCell ref="AU382:AU384"/>
+    <mergeCell ref="K382:K404"/>
+    <mergeCell ref="M419:M427"/>
+    <mergeCell ref="K405:K427"/>
+    <mergeCell ref="AU405:AU407"/>
+    <mergeCell ref="L408:L418"/>
+    <mergeCell ref="K358:K381"/>
+    <mergeCell ref="M382:M384"/>
+    <mergeCell ref="L385:L395"/>
+    <mergeCell ref="M396:M404"/>
+    <mergeCell ref="M358:M360"/>
+    <mergeCell ref="L361:L362"/>
+    <mergeCell ref="AU358:AU362"/>
+    <mergeCell ref="M363:M371"/>
+    <mergeCell ref="L372:L381"/>
+    <mergeCell ref="I332:I336"/>
+    <mergeCell ref="I316:I323"/>
+    <mergeCell ref="AU226:AU230"/>
+    <mergeCell ref="J226:J228"/>
+    <mergeCell ref="I229:I230"/>
+    <mergeCell ref="AU198:AU202"/>
+    <mergeCell ref="I201:I202"/>
+    <mergeCell ref="J198:J200"/>
+    <mergeCell ref="I203:I212"/>
+    <mergeCell ref="J213:J222"/>
+    <mergeCell ref="I254:I261"/>
+    <mergeCell ref="H84:H115"/>
+    <mergeCell ref="I66:I70"/>
+    <mergeCell ref="J71:J75"/>
+    <mergeCell ref="J130:J136"/>
+    <mergeCell ref="I137:I141"/>
+    <mergeCell ref="J184:J187"/>
+    <mergeCell ref="I188:I197"/>
+    <mergeCell ref="J98:J104"/>
+    <mergeCell ref="I105:I109"/>
+    <mergeCell ref="J148:J156"/>
+    <mergeCell ref="J116:J121"/>
+    <mergeCell ref="I122:I128"/>
+    <mergeCell ref="I157:I158"/>
+    <mergeCell ref="I163:I172"/>
+    <mergeCell ref="J159:J162"/>
+    <mergeCell ref="H116:H147"/>
+    <mergeCell ref="H148:H172"/>
+    <mergeCell ref="H173:H197"/>
+    <mergeCell ref="J173:J181"/>
+    <mergeCell ref="I182:I183"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="H3:J3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="AU5:AU15"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="AQ3:AS3"/>
+    <mergeCell ref="AN3:AP3"/>
+    <mergeCell ref="AI3:AK3"/>
+    <mergeCell ref="AF3:AH3"/>
+    <mergeCell ref="AA3:AC3"/>
+    <mergeCell ref="X3:Z3"/>
+    <mergeCell ref="S3:U3"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="W3:W4"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="N3:N4"/>
+    <mergeCell ref="V3:V4"/>
+    <mergeCell ref="AD3:AD4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="I306:I310"/>
+    <mergeCell ref="J311:J314"/>
+    <mergeCell ref="AU306:AU314"/>
+    <mergeCell ref="AU16:AU30"/>
+    <mergeCell ref="AU50:AU64"/>
+    <mergeCell ref="AU84:AU96"/>
+    <mergeCell ref="J16:J23"/>
+    <mergeCell ref="I24:I30"/>
+    <mergeCell ref="I58:I64"/>
+    <mergeCell ref="J84:J89"/>
+    <mergeCell ref="I90:I96"/>
+    <mergeCell ref="J50:J57"/>
+    <mergeCell ref="I32:I36"/>
+    <mergeCell ref="AU173:AU183"/>
+    <mergeCell ref="AU116:AU128"/>
+    <mergeCell ref="AU148:AU158"/>
+    <mergeCell ref="L670:L672"/>
+    <mergeCell ref="J676:J680"/>
+    <mergeCell ref="AV3:AV4"/>
+    <mergeCell ref="AV5:AV475"/>
+    <mergeCell ref="AV476:AV523"/>
+    <mergeCell ref="AU458:AU463"/>
+    <mergeCell ref="H198:H225"/>
+    <mergeCell ref="H226:H253"/>
+    <mergeCell ref="I231:I240"/>
+    <mergeCell ref="J241:J250"/>
+    <mergeCell ref="H254:H279"/>
+    <mergeCell ref="H280:H305"/>
+    <mergeCell ref="J337:J340"/>
+    <mergeCell ref="AU332:AU340"/>
+    <mergeCell ref="J324:J331"/>
+    <mergeCell ref="H306:H331"/>
+    <mergeCell ref="H332:H357"/>
+    <mergeCell ref="I270:I274"/>
+    <mergeCell ref="J275:J279"/>
+    <mergeCell ref="AU254:AU268"/>
+    <mergeCell ref="AU280:AU294"/>
+    <mergeCell ref="J288:J294"/>
+    <mergeCell ref="I280:I287"/>
+    <mergeCell ref="J262:J268"/>
     <mergeCell ref="C588:C590"/>
     <mergeCell ref="C585:C586"/>
     <mergeCell ref="C582:C583"/>
@@ -92607,124 +92698,33 @@
     <mergeCell ref="I656:I671"/>
     <mergeCell ref="J656:J669"/>
     <mergeCell ref="M656:M669"/>
-    <mergeCell ref="L670:L672"/>
-    <mergeCell ref="J676:J680"/>
-    <mergeCell ref="AV3:AV4"/>
-    <mergeCell ref="AV5:AV475"/>
-    <mergeCell ref="AV476:AV523"/>
-    <mergeCell ref="AU458:AU463"/>
-    <mergeCell ref="H198:H225"/>
-    <mergeCell ref="H226:H253"/>
-    <mergeCell ref="I231:I240"/>
-    <mergeCell ref="J241:J250"/>
-    <mergeCell ref="H254:H279"/>
-    <mergeCell ref="H280:H305"/>
-    <mergeCell ref="J337:J340"/>
-    <mergeCell ref="AU332:AU340"/>
-    <mergeCell ref="J324:J331"/>
-    <mergeCell ref="H306:H331"/>
-    <mergeCell ref="H332:H357"/>
-    <mergeCell ref="I270:I274"/>
-    <mergeCell ref="J275:J279"/>
-    <mergeCell ref="AU254:AU268"/>
-    <mergeCell ref="AU280:AU294"/>
-    <mergeCell ref="J288:J294"/>
-    <mergeCell ref="I280:I287"/>
-    <mergeCell ref="J262:J268"/>
-    <mergeCell ref="I306:I310"/>
-    <mergeCell ref="J311:J314"/>
-    <mergeCell ref="AU306:AU314"/>
-    <mergeCell ref="AU16:AU30"/>
-    <mergeCell ref="AU50:AU64"/>
-    <mergeCell ref="AU84:AU96"/>
-    <mergeCell ref="J16:J23"/>
-    <mergeCell ref="I24:I30"/>
-    <mergeCell ref="I58:I64"/>
-    <mergeCell ref="J84:J89"/>
-    <mergeCell ref="I90:I96"/>
-    <mergeCell ref="J50:J57"/>
-    <mergeCell ref="I32:I36"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="H3:J3"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="AU5:AU15"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="AQ3:AS3"/>
-    <mergeCell ref="AN3:AP3"/>
-    <mergeCell ref="AI3:AK3"/>
-    <mergeCell ref="AF3:AH3"/>
-    <mergeCell ref="AA3:AC3"/>
-    <mergeCell ref="X3:Z3"/>
-    <mergeCell ref="S3:U3"/>
-    <mergeCell ref="P3:R3"/>
-    <mergeCell ref="W3:W4"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="N3:N4"/>
-    <mergeCell ref="V3:V4"/>
-    <mergeCell ref="AD3:AD4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="H84:H115"/>
-    <mergeCell ref="I66:I70"/>
-    <mergeCell ref="J71:J75"/>
-    <mergeCell ref="J130:J136"/>
-    <mergeCell ref="I137:I141"/>
-    <mergeCell ref="J184:J187"/>
-    <mergeCell ref="I188:I197"/>
-    <mergeCell ref="J98:J104"/>
-    <mergeCell ref="I105:I109"/>
-    <mergeCell ref="J148:J156"/>
-    <mergeCell ref="J116:J121"/>
-    <mergeCell ref="I122:I128"/>
-    <mergeCell ref="I157:I158"/>
-    <mergeCell ref="I163:I172"/>
-    <mergeCell ref="J159:J162"/>
-    <mergeCell ref="H116:H147"/>
-    <mergeCell ref="H148:H172"/>
-    <mergeCell ref="H173:H197"/>
-    <mergeCell ref="J173:J181"/>
-    <mergeCell ref="I182:I183"/>
-    <mergeCell ref="AU173:AU183"/>
-    <mergeCell ref="AU116:AU128"/>
-    <mergeCell ref="AU148:AU158"/>
-    <mergeCell ref="I332:I336"/>
-    <mergeCell ref="I316:I323"/>
-    <mergeCell ref="AU226:AU230"/>
-    <mergeCell ref="J226:J228"/>
-    <mergeCell ref="I229:I230"/>
-    <mergeCell ref="AU198:AU202"/>
-    <mergeCell ref="I201:I202"/>
-    <mergeCell ref="J198:J200"/>
-    <mergeCell ref="I203:I212"/>
-    <mergeCell ref="J213:J222"/>
-    <mergeCell ref="I254:I261"/>
-    <mergeCell ref="M405:M407"/>
-    <mergeCell ref="H16:H49"/>
-    <mergeCell ref="J37:J41"/>
-    <mergeCell ref="H50:H83"/>
-    <mergeCell ref="I296:I300"/>
-    <mergeCell ref="J301:J305"/>
-    <mergeCell ref="I342:I349"/>
-    <mergeCell ref="J350:J357"/>
-    <mergeCell ref="AU428:AU429"/>
-    <mergeCell ref="AU382:AU384"/>
-    <mergeCell ref="K382:K404"/>
-    <mergeCell ref="M419:M427"/>
-    <mergeCell ref="K405:K427"/>
-    <mergeCell ref="AU405:AU407"/>
-    <mergeCell ref="L408:L418"/>
-    <mergeCell ref="K358:K381"/>
-    <mergeCell ref="M382:M384"/>
-    <mergeCell ref="L385:L395"/>
-    <mergeCell ref="M396:M404"/>
-    <mergeCell ref="M358:M360"/>
-    <mergeCell ref="L361:L362"/>
-    <mergeCell ref="AU358:AU362"/>
-    <mergeCell ref="M363:M371"/>
-    <mergeCell ref="L372:L381"/>
+    <mergeCell ref="AU467:AU478"/>
+    <mergeCell ref="AU479:AU482"/>
+    <mergeCell ref="AU485:AU486"/>
+    <mergeCell ref="AU483:AU484"/>
+    <mergeCell ref="AU487:AU488"/>
+    <mergeCell ref="M624:M629"/>
+    <mergeCell ref="M621:M622"/>
+    <mergeCell ref="L621:L622"/>
+    <mergeCell ref="L626:L628"/>
+    <mergeCell ref="L629:L630"/>
+    <mergeCell ref="L588:L590"/>
+    <mergeCell ref="K626:K629"/>
+    <mergeCell ref="J626:J628"/>
+    <mergeCell ref="J629:J630"/>
+    <mergeCell ref="I626:I628"/>
+    <mergeCell ref="I624:I625"/>
+    <mergeCell ref="C596:C622"/>
+    <mergeCell ref="L596:L600"/>
+    <mergeCell ref="M596:M605"/>
+    <mergeCell ref="L602:L607"/>
+    <mergeCell ref="M606:M607"/>
+    <mergeCell ref="K602:K605"/>
+    <mergeCell ref="I603:I604"/>
+    <mergeCell ref="J597:J599"/>
+    <mergeCell ref="K596:K600"/>
+    <mergeCell ref="J610:J611"/>
+    <mergeCell ref="I609:I611"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed Template; Continued work on 1 Common Synonym
</commit_message>
<xml_diff>
--- a/AutoTester/Tests/System/System Testing Template.xlsx
+++ b/AutoTester/Tests/System/System Testing Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27609" uniqueCount="497">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27586" uniqueCount="506">
   <si>
     <t>such that</t>
   </si>
@@ -1516,6 +1516,33 @@
   <si>
     <t>2=co.value</t>
   </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 5</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 6</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 7</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 8</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 9</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 10</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 11</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 12</t>
+  </si>
+  <si>
+    <t>Multiple Clause Invalid Test Case 13</t>
+  </si>
 </sst>
 </file>
 
@@ -2130,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1C4663-D304-44C8-B0BF-D228A95395FB}">
   <dimension ref="B3:AY688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K465" workbookViewId="0">
-      <selection activeCell="N487" sqref="N487"/>
+    <sheetView tabSelected="1" topLeftCell="A532" workbookViewId="0">
+      <selection activeCell="I569" sqref="I569"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -70228,7 +70255,7 @@
       <c r="AT497" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU497" s="6" t="s">
+      <c r="AU497" s="8" t="s">
         <v>417</v>
       </c>
       <c r="AV497" s="2"/>
@@ -70369,7 +70396,7 @@
       <c r="AT498" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU498" s="6"/>
+      <c r="AU498" s="9"/>
       <c r="AV498" s="2"/>
     </row>
     <row r="499" spans="2:48" x14ac:dyDescent="0.25">
@@ -70508,7 +70535,7 @@
       <c r="AT499" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU499" s="6"/>
+      <c r="AU499" s="9"/>
       <c r="AV499" s="2"/>
     </row>
     <row r="500" spans="2:48" x14ac:dyDescent="0.25">
@@ -70647,7 +70674,7 @@
       <c r="AT500" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU500" s="6"/>
+      <c r="AU500" s="9"/>
       <c r="AV500" s="2"/>
     </row>
     <row r="501" spans="2:48" x14ac:dyDescent="0.25">
@@ -70786,7 +70813,7 @@
       <c r="AT501" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU501" s="6"/>
+      <c r="AU501" s="9"/>
       <c r="AV501" s="2"/>
     </row>
     <row r="502" spans="2:48" x14ac:dyDescent="0.25">
@@ -70925,7 +70952,7 @@
       <c r="AT502" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU502" s="6"/>
+      <c r="AU502" s="9"/>
       <c r="AV502" s="2"/>
     </row>
     <row r="503" spans="2:48" x14ac:dyDescent="0.25">
@@ -71064,7 +71091,7 @@
       <c r="AT503" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU503" s="6"/>
+      <c r="AU503" s="9"/>
       <c r="AV503" s="2"/>
     </row>
     <row r="504" spans="2:48" x14ac:dyDescent="0.25">
@@ -71203,7 +71230,7 @@
       <c r="AT504" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU504" s="6"/>
+      <c r="AU504" s="9"/>
       <c r="AV504" s="2"/>
     </row>
     <row r="505" spans="2:48" x14ac:dyDescent="0.25">
@@ -71342,7 +71369,7 @@
       <c r="AT505" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU505" s="6"/>
+      <c r="AU505" s="9"/>
       <c r="AV505" s="2"/>
     </row>
     <row r="506" spans="2:48" x14ac:dyDescent="0.25">
@@ -71481,7 +71508,7 @@
       <c r="AT506" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU506" s="6"/>
+      <c r="AU506" s="9"/>
       <c r="AV506" s="2"/>
     </row>
     <row r="507" spans="2:48" x14ac:dyDescent="0.25">
@@ -71620,7 +71647,7 @@
       <c r="AT507" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU507" s="6"/>
+      <c r="AU507" s="11"/>
       <c r="AV507" s="2"/>
     </row>
     <row r="508" spans="2:48" x14ac:dyDescent="0.25">
@@ -71645,19 +71672,19 @@
       <c r="H508" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I508" s="6" t="s">
+      <c r="I508" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J508" s="6" t="s">
+      <c r="J508" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K508" s="6" t="s">
+      <c r="K508" s="8" t="s">
         <v>38</v>
       </c>
       <c r="L508" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M508" s="6" t="s">
+      <c r="M508" s="8" t="s">
         <v>52</v>
       </c>
       <c r="N508" s="7" t="s">
@@ -71759,7 +71786,7 @@
       <c r="AT508" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU508" s="6" t="s">
+      <c r="AU508" s="8" t="s">
         <v>442</v>
       </c>
       <c r="AV508" s="2"/>
@@ -71786,13 +71813,13 @@
       <c r="H509" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I509" s="6"/>
-      <c r="J509" s="6"/>
-      <c r="K509" s="6"/>
+      <c r="I509" s="9"/>
+      <c r="J509" s="9"/>
+      <c r="K509" s="9"/>
       <c r="L509" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M509" s="6"/>
+      <c r="M509" s="9"/>
       <c r="N509" s="7" t="s">
         <v>44</v>
       </c>
@@ -71892,7 +71919,7 @@
       <c r="AT509" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU509" s="6"/>
+      <c r="AU509" s="9"/>
       <c r="AV509" s="2"/>
     </row>
     <row r="510" spans="2:48" x14ac:dyDescent="0.25">
@@ -71917,13 +71944,13 @@
       <c r="H510" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I510" s="6"/>
-      <c r="J510" s="6"/>
-      <c r="K510" s="6"/>
+      <c r="I510" s="9"/>
+      <c r="J510" s="9"/>
+      <c r="K510" s="9"/>
       <c r="L510" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M510" s="6"/>
+      <c r="M510" s="11"/>
       <c r="N510" s="7" t="s">
         <v>44</v>
       </c>
@@ -72023,7 +72050,7 @@
       <c r="AT510" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU510" s="6"/>
+      <c r="AU510" s="9"/>
       <c r="AV510" s="2"/>
     </row>
     <row r="511" spans="2:48" x14ac:dyDescent="0.25">
@@ -72048,10 +72075,10 @@
       <c r="H511" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I511" s="6"/>
-      <c r="J511" s="6"/>
-      <c r="K511" s="6"/>
-      <c r="L511" s="6" t="s">
+      <c r="I511" s="9"/>
+      <c r="J511" s="11"/>
+      <c r="K511" s="9"/>
+      <c r="L511" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M511" s="6" t="s">
@@ -72156,7 +72183,7 @@
       <c r="AT511" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU511" s="6"/>
+      <c r="AU511" s="9"/>
       <c r="AV511" s="2"/>
     </row>
     <row r="512" spans="2:48" x14ac:dyDescent="0.25">
@@ -72181,12 +72208,12 @@
       <c r="H512" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I512" s="6"/>
-      <c r="J512" s="6" t="s">
+      <c r="I512" s="9"/>
+      <c r="J512" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="K512" s="6"/>
-      <c r="L512" s="6"/>
+      <c r="K512" s="9"/>
+      <c r="L512" s="11"/>
       <c r="M512" s="6" t="s">
         <v>62</v>
       </c>
@@ -72289,7 +72316,7 @@
       <c r="AT512" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU512" s="6"/>
+      <c r="AU512" s="9"/>
       <c r="AV512" s="2"/>
     </row>
     <row r="513" spans="2:48" x14ac:dyDescent="0.25">
@@ -72314,13 +72341,13 @@
       <c r="H513" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I513" s="6"/>
-      <c r="J513" s="6"/>
-      <c r="K513" s="6"/>
+      <c r="I513" s="11"/>
+      <c r="J513" s="11"/>
+      <c r="K513" s="9"/>
       <c r="L513" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M513" s="6" t="s">
+      <c r="M513" s="8" t="s">
         <v>52</v>
       </c>
       <c r="N513" s="7" t="s">
@@ -72422,7 +72449,7 @@
       <c r="AT513" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU513" s="6"/>
+      <c r="AU513" s="9"/>
       <c r="AV513" s="2"/>
     </row>
     <row r="514" spans="2:48" x14ac:dyDescent="0.25">
@@ -72447,17 +72474,17 @@
       <c r="H514" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I514" s="6" t="s">
+      <c r="I514" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J514" s="6" t="s">
+      <c r="J514" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K514" s="6"/>
+      <c r="K514" s="9"/>
       <c r="L514" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M514" s="6"/>
+      <c r="M514" s="9"/>
       <c r="N514" s="7" t="s">
         <v>44</v>
       </c>
@@ -72557,7 +72584,7 @@
       <c r="AT514" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU514" s="6"/>
+      <c r="AU514" s="9"/>
       <c r="AV514" s="2"/>
     </row>
     <row r="515" spans="2:48" x14ac:dyDescent="0.25">
@@ -72582,13 +72609,13 @@
       <c r="H515" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I515" s="6"/>
-      <c r="J515" s="6"/>
-      <c r="K515" s="6"/>
+      <c r="I515" s="11"/>
+      <c r="J515" s="11"/>
+      <c r="K515" s="9"/>
       <c r="L515" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M515" s="6"/>
+      <c r="M515" s="11"/>
       <c r="N515" s="7" t="s">
         <v>44</v>
       </c>
@@ -72688,7 +72715,7 @@
       <c r="AT515" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU515" s="6"/>
+      <c r="AU515" s="9"/>
       <c r="AV515" s="2"/>
     </row>
     <row r="516" spans="2:48" x14ac:dyDescent="0.25">
@@ -72713,14 +72740,14 @@
       <c r="H516" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I516" s="6" t="s">
+      <c r="I516" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J516" s="6" t="s">
+      <c r="J516" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K516" s="6"/>
-      <c r="L516" s="6" t="s">
+      <c r="K516" s="9"/>
+      <c r="L516" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M516" s="6" t="s">
@@ -72825,7 +72852,7 @@
       <c r="AT516" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU516" s="6"/>
+      <c r="AU516" s="9"/>
       <c r="AV516" s="2"/>
     </row>
     <row r="517" spans="2:48" x14ac:dyDescent="0.25">
@@ -72850,10 +72877,10 @@
       <c r="H517" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I517" s="6"/>
-      <c r="J517" s="6"/>
-      <c r="K517" s="6"/>
-      <c r="L517" s="6"/>
+      <c r="I517" s="11"/>
+      <c r="J517" s="11"/>
+      <c r="K517" s="9"/>
+      <c r="L517" s="9"/>
       <c r="M517" s="6" t="s">
         <v>62</v>
       </c>
@@ -72956,7 +72983,7 @@
       <c r="AT517" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU517" s="6"/>
+      <c r="AU517" s="9"/>
       <c r="AV517" s="2"/>
     </row>
     <row r="518" spans="2:48" x14ac:dyDescent="0.25">
@@ -72981,17 +73008,15 @@
       <c r="H518" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I518" s="6" t="s">
+      <c r="I518" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J518" s="6" t="s">
+      <c r="J518" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K518" s="6"/>
-      <c r="L518" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M518" s="6" t="s">
+      <c r="K518" s="9"/>
+      <c r="L518" s="11"/>
+      <c r="M518" s="8" t="s">
         <v>52</v>
       </c>
       <c r="N518" s="7" t="s">
@@ -73093,7 +73118,7 @@
       <c r="AT518" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU518" s="6"/>
+      <c r="AU518" s="9"/>
       <c r="AV518" s="2"/>
     </row>
     <row r="519" spans="2:48" x14ac:dyDescent="0.25">
@@ -73118,13 +73143,13 @@
       <c r="H519" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I519" s="6"/>
-      <c r="J519" s="6"/>
-      <c r="K519" s="6"/>
+      <c r="I519" s="11"/>
+      <c r="J519" s="11"/>
+      <c r="K519" s="11"/>
       <c r="L519" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M519" s="6"/>
+      <c r="M519" s="11"/>
       <c r="N519" s="7" t="s">
         <v>44</v>
       </c>
@@ -73224,7 +73249,7 @@
       <c r="AT519" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU519" s="6"/>
+      <c r="AU519" s="9"/>
       <c r="AV519" s="2"/>
     </row>
     <row r="520" spans="2:48" x14ac:dyDescent="0.25">
@@ -73249,16 +73274,16 @@
       <c r="H520" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I520" s="6" t="s">
+      <c r="I520" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J520" s="6" t="s">
+      <c r="J520" s="8" t="s">
         <v>37</v>
       </c>
       <c r="K520" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L520" s="6" t="s">
+      <c r="L520" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M520" s="6" t="s">
@@ -73363,7 +73388,7 @@
       <c r="AT520" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU520" s="6"/>
+      <c r="AU520" s="9"/>
       <c r="AV520" s="2"/>
     </row>
     <row r="521" spans="2:48" x14ac:dyDescent="0.25">
@@ -73388,14 +73413,12 @@
       <c r="H521" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I521" s="6"/>
-      <c r="J521" s="6"/>
+      <c r="I521" s="11"/>
+      <c r="J521" s="11"/>
       <c r="K521" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L521" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="L521" s="11"/>
       <c r="M521" s="6" t="s">
         <v>62</v>
       </c>
@@ -73498,7 +73521,7 @@
       <c r="AT521" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU521" s="6"/>
+      <c r="AU521" s="11"/>
       <c r="AV521" s="2"/>
     </row>
     <row r="522" spans="2:48" x14ac:dyDescent="0.25">
@@ -73523,10 +73546,10 @@
       <c r="H522" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I522" s="6" t="s">
+      <c r="I522" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J522" s="6" t="s">
+      <c r="J522" s="8" t="s">
         <v>37</v>
       </c>
       <c r="K522" s="7" t="s">
@@ -73538,7 +73561,7 @@
       <c r="M522" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N522" s="6" t="s">
+      <c r="N522" s="8" t="s">
         <v>338</v>
       </c>
       <c r="O522" s="7" t="s">
@@ -73637,7 +73660,7 @@
       <c r="AT522" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU522" s="6" t="s">
+      <c r="AU522" s="8" t="s">
         <v>441</v>
       </c>
       <c r="AV522" s="2"/>
@@ -73664,8 +73687,8 @@
       <c r="H523" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I523" s="6"/>
-      <c r="J523" s="6"/>
+      <c r="I523" s="9"/>
+      <c r="J523" s="9"/>
       <c r="K523" s="7" t="s">
         <v>44</v>
       </c>
@@ -73675,7 +73698,7 @@
       <c r="M523" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N523" s="6"/>
+      <c r="N523" s="9"/>
       <c r="O523" s="7" t="s">
         <v>44</v>
       </c>
@@ -73772,7 +73795,7 @@
       <c r="AT523" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU523" s="6"/>
+      <c r="AU523" s="9"/>
       <c r="AV523" s="2"/>
     </row>
     <row r="524" spans="2:48" x14ac:dyDescent="0.25">
@@ -73797,8 +73820,8 @@
       <c r="H524" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I524" s="6"/>
-      <c r="J524" s="6"/>
+      <c r="I524" s="9"/>
+      <c r="J524" s="9"/>
       <c r="K524" s="7" t="s">
         <v>44</v>
       </c>
@@ -73808,7 +73831,7 @@
       <c r="M524" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N524" s="6"/>
+      <c r="N524" s="9"/>
       <c r="O524" s="7" t="s">
         <v>44</v>
       </c>
@@ -73905,7 +73928,7 @@
       <c r="AT524" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU524" s="6"/>
+      <c r="AU524" s="9"/>
       <c r="AV524" s="6"/>
     </row>
     <row r="525" spans="2:48" x14ac:dyDescent="0.25">
@@ -73930,8 +73953,8 @@
       <c r="H525" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I525" s="6"/>
-      <c r="J525" s="6"/>
+      <c r="I525" s="9"/>
+      <c r="J525" s="11"/>
       <c r="K525" s="7" t="s">
         <v>44</v>
       </c>
@@ -73941,7 +73964,7 @@
       <c r="M525" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N525" s="6"/>
+      <c r="N525" s="9"/>
       <c r="O525" s="7" t="s">
         <v>44</v>
       </c>
@@ -74038,7 +74061,7 @@
       <c r="AT525" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU525" s="6"/>
+      <c r="AU525" s="9"/>
       <c r="AV525" s="6"/>
     </row>
     <row r="526" spans="2:48" x14ac:dyDescent="0.25">
@@ -74063,8 +74086,8 @@
       <c r="H526" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I526" s="6"/>
-      <c r="J526" s="6" t="s">
+      <c r="I526" s="9"/>
+      <c r="J526" s="8" t="s">
         <v>42</v>
       </c>
       <c r="K526" s="7" t="s">
@@ -74076,7 +74099,7 @@
       <c r="M526" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N526" s="6"/>
+      <c r="N526" s="9"/>
       <c r="O526" s="7" t="s">
         <v>44</v>
       </c>
@@ -74173,7 +74196,7 @@
       <c r="AT526" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU526" s="6"/>
+      <c r="AU526" s="9"/>
       <c r="AV526" s="6"/>
     </row>
     <row r="527" spans="2:48" x14ac:dyDescent="0.25">
@@ -74198,8 +74221,8 @@
       <c r="H527" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I527" s="6"/>
-      <c r="J527" s="6"/>
+      <c r="I527" s="11"/>
+      <c r="J527" s="11"/>
       <c r="K527" s="7" t="s">
         <v>44</v>
       </c>
@@ -74209,7 +74232,7 @@
       <c r="M527" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N527" s="6"/>
+      <c r="N527" s="9"/>
       <c r="O527" s="7" t="s">
         <v>44</v>
       </c>
@@ -74306,7 +74329,7 @@
       <c r="AT527" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU527" s="6"/>
+      <c r="AU527" s="9"/>
       <c r="AV527" s="6"/>
     </row>
     <row r="528" spans="2:48" x14ac:dyDescent="0.25">
@@ -74331,10 +74354,10 @@
       <c r="H528" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I528" s="6" t="s">
+      <c r="I528" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J528" s="6" t="s">
+      <c r="J528" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K528" s="7" t="s">
@@ -74346,7 +74369,7 @@
       <c r="M528" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N528" s="6"/>
+      <c r="N528" s="9"/>
       <c r="O528" s="7" t="s">
         <v>44</v>
       </c>
@@ -74443,7 +74466,7 @@
       <c r="AT528" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU528" s="6"/>
+      <c r="AU528" s="9"/>
       <c r="AV528" s="6"/>
     </row>
     <row r="529" spans="2:48" x14ac:dyDescent="0.25">
@@ -74468,8 +74491,8 @@
       <c r="H529" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I529" s="6"/>
-      <c r="J529" s="6"/>
+      <c r="I529" s="11"/>
+      <c r="J529" s="11"/>
       <c r="K529" s="7" t="s">
         <v>44</v>
       </c>
@@ -74479,7 +74502,7 @@
       <c r="M529" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N529" s="6"/>
+      <c r="N529" s="9"/>
       <c r="O529" s="7" t="s">
         <v>44</v>
       </c>
@@ -74576,7 +74599,7 @@
       <c r="AT529" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU529" s="6"/>
+      <c r="AU529" s="9"/>
       <c r="AV529" s="6"/>
     </row>
     <row r="530" spans="2:48" x14ac:dyDescent="0.25">
@@ -74601,10 +74624,10 @@
       <c r="H530" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I530" s="6" t="s">
+      <c r="I530" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J530" s="6" t="s">
+      <c r="J530" s="8" t="s">
         <v>43</v>
       </c>
       <c r="K530" s="7" t="s">
@@ -74616,7 +74639,7 @@
       <c r="M530" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N530" s="6"/>
+      <c r="N530" s="9"/>
       <c r="O530" s="7" t="s">
         <v>44</v>
       </c>
@@ -74713,7 +74736,7 @@
       <c r="AT530" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU530" s="6"/>
+      <c r="AU530" s="9"/>
       <c r="AV530" s="6"/>
     </row>
     <row r="531" spans="2:48" x14ac:dyDescent="0.25">
@@ -74738,8 +74761,8 @@
       <c r="H531" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I531" s="6"/>
-      <c r="J531" s="6"/>
+      <c r="I531" s="11"/>
+      <c r="J531" s="11"/>
       <c r="K531" s="7" t="s">
         <v>44</v>
       </c>
@@ -74749,7 +74772,7 @@
       <c r="M531" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N531" s="6"/>
+      <c r="N531" s="9"/>
       <c r="O531" s="7" t="s">
         <v>44</v>
       </c>
@@ -74846,7 +74869,7 @@
       <c r="AT531" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU531" s="6"/>
+      <c r="AU531" s="9"/>
       <c r="AV531" s="6"/>
     </row>
     <row r="532" spans="2:48" x14ac:dyDescent="0.25">
@@ -74871,10 +74894,10 @@
       <c r="H532" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I532" s="6" t="s">
+      <c r="I532" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J532" s="6" t="s">
+      <c r="J532" s="8" t="s">
         <v>37</v>
       </c>
       <c r="K532" s="7" t="s">
@@ -74886,7 +74909,7 @@
       <c r="M532" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N532" s="6"/>
+      <c r="N532" s="9"/>
       <c r="O532" s="7" t="s">
         <v>44</v>
       </c>
@@ -74983,7 +75006,7 @@
       <c r="AT532" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU532" s="6"/>
+      <c r="AU532" s="9"/>
       <c r="AV532" s="6"/>
     </row>
     <row r="533" spans="2:48" x14ac:dyDescent="0.25">
@@ -75008,8 +75031,8 @@
       <c r="H533" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I533" s="6"/>
-      <c r="J533" s="6"/>
+      <c r="I533" s="11"/>
+      <c r="J533" s="11"/>
       <c r="K533" s="7" t="s">
         <v>44</v>
       </c>
@@ -75019,7 +75042,7 @@
       <c r="M533" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N533" s="6"/>
+      <c r="N533" s="11"/>
       <c r="O533" s="7" t="s">
         <v>44</v>
       </c>
@@ -75116,7 +75139,7 @@
       <c r="AT533" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU533" s="6"/>
+      <c r="AU533" s="9"/>
       <c r="AV533" s="6"/>
     </row>
     <row r="534" spans="2:48" x14ac:dyDescent="0.25">
@@ -75141,10 +75164,10 @@
       <c r="H534" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I534" s="6" t="s">
+      <c r="I534" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J534" s="6" t="s">
+      <c r="J534" s="8" t="s">
         <v>37</v>
       </c>
       <c r="K534" s="7" t="s">
@@ -75255,7 +75278,7 @@
       <c r="AT534" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU534" s="6"/>
+      <c r="AU534" s="9"/>
       <c r="AV534" s="6"/>
     </row>
     <row r="535" spans="2:48" x14ac:dyDescent="0.25">
@@ -75280,8 +75303,8 @@
       <c r="H535" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I535" s="6"/>
-      <c r="J535" s="6"/>
+      <c r="I535" s="11"/>
+      <c r="J535" s="11"/>
       <c r="K535" s="7" t="s">
         <v>44</v>
       </c>
@@ -75390,7 +75413,7 @@
       <c r="AT535" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU535" s="6"/>
+      <c r="AU535" s="9"/>
       <c r="AV535" s="6"/>
     </row>
     <row r="536" spans="2:48" x14ac:dyDescent="0.25">
@@ -75415,10 +75438,10 @@
       <c r="H536" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I536" s="6" t="s">
+      <c r="I536" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J536" s="6" t="s">
+      <c r="J536" s="8" t="s">
         <v>37</v>
       </c>
       <c r="K536" s="7" t="s">
@@ -75529,7 +75552,7 @@
       <c r="AT536" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU536" s="6"/>
+      <c r="AU536" s="9"/>
       <c r="AV536" s="6"/>
     </row>
     <row r="537" spans="2:48" x14ac:dyDescent="0.25">
@@ -75554,8 +75577,8 @@
       <c r="H537" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I537" s="6"/>
-      <c r="J537" s="6"/>
+      <c r="I537" s="11"/>
+      <c r="J537" s="11"/>
       <c r="K537" s="7" t="s">
         <v>44</v>
       </c>
@@ -75664,7 +75687,7 @@
       <c r="AT537" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU537" s="6"/>
+      <c r="AU537" s="11"/>
       <c r="AV537" s="6"/>
     </row>
     <row r="538" spans="2:48" x14ac:dyDescent="0.25">
@@ -75698,13 +75721,13 @@
       <c r="K538" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L538" s="6" t="s">
+      <c r="L538" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M538" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="N538" s="6" t="s">
+      <c r="N538" s="8" t="s">
         <v>338</v>
       </c>
       <c r="O538" s="7" t="s">
@@ -75803,7 +75826,7 @@
       <c r="AT538" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU538" s="6" t="s">
+      <c r="AU538" s="8" t="s">
         <v>440</v>
       </c>
       <c r="AV538" s="6"/>
@@ -75839,11 +75862,11 @@
       <c r="K539" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L539" s="6"/>
-      <c r="M539" s="6" t="s">
+      <c r="L539" s="9"/>
+      <c r="M539" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N539" s="6"/>
+      <c r="N539" s="9"/>
       <c r="O539" s="7" t="s">
         <v>44</v>
       </c>
@@ -75940,7 +75963,7 @@
       <c r="AT539" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU539" s="6"/>
+      <c r="AU539" s="9"/>
       <c r="AV539" s="6"/>
     </row>
     <row r="540" spans="2:48" x14ac:dyDescent="0.25">
@@ -75974,9 +75997,9 @@
       <c r="K540" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L540" s="6"/>
-      <c r="M540" s="6"/>
-      <c r="N540" s="6"/>
+      <c r="L540" s="9"/>
+      <c r="M540" s="11"/>
+      <c r="N540" s="11"/>
       <c r="O540" s="7" t="s">
         <v>44</v>
       </c>
@@ -76073,7 +76096,7 @@
       <c r="AT540" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU540" s="6"/>
+      <c r="AU540" s="9"/>
       <c r="AV540" s="6"/>
     </row>
     <row r="541" spans="2:48" x14ac:dyDescent="0.25">
@@ -76107,7 +76130,7 @@
       <c r="K541" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L541" s="6"/>
+      <c r="L541" s="9"/>
       <c r="M541" s="6" t="s">
         <v>52</v>
       </c>
@@ -76210,7 +76233,7 @@
       <c r="AT541" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU541" s="6"/>
+      <c r="AU541" s="9"/>
       <c r="AV541" s="6"/>
     </row>
     <row r="542" spans="2:48" x14ac:dyDescent="0.25">
@@ -76244,8 +76267,8 @@
       <c r="K542" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L542" s="6"/>
-      <c r="M542" s="6" t="s">
+      <c r="L542" s="9"/>
+      <c r="M542" s="8" t="s">
         <v>62</v>
       </c>
       <c r="N542" s="6" t="s">
@@ -76347,7 +76370,7 @@
       <c r="AT542" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU542" s="6"/>
+      <c r="AU542" s="9"/>
       <c r="AV542" s="6"/>
     </row>
     <row r="543" spans="2:48" x14ac:dyDescent="0.25">
@@ -76381,8 +76404,8 @@
       <c r="K543" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L543" s="6"/>
-      <c r="M543" s="6"/>
+      <c r="L543" s="9"/>
+      <c r="M543" s="11"/>
       <c r="N543" s="6" t="s">
         <v>412</v>
       </c>
@@ -76482,7 +76505,7 @@
       <c r="AT543" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU543" s="6"/>
+      <c r="AU543" s="9"/>
       <c r="AV543" s="6"/>
     </row>
     <row r="544" spans="2:48" x14ac:dyDescent="0.25">
@@ -76516,7 +76539,7 @@
       <c r="K544" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L544" s="6"/>
+      <c r="L544" s="11"/>
       <c r="M544" s="6" t="s">
         <v>52</v>
       </c>
@@ -76619,7 +76642,7 @@
       <c r="AT544" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU544" s="6"/>
+      <c r="AU544" s="11"/>
       <c r="AV544" s="6"/>
     </row>
     <row r="545" spans="2:48" x14ac:dyDescent="0.25">
@@ -76644,22 +76667,22 @@
       <c r="H545" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I545" s="6" t="s">
+      <c r="I545" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J545" s="6" t="s">
+      <c r="J545" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K545" s="6" t="s">
+      <c r="K545" s="8" t="s">
         <v>38</v>
       </c>
       <c r="L545" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M545" s="6" t="s">
+      <c r="M545" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="N545" s="6" t="s">
+      <c r="N545" s="8" t="s">
         <v>338</v>
       </c>
       <c r="O545" s="7" t="s">
@@ -76758,7 +76781,7 @@
       <c r="AT545" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU545" s="6" t="s">
+      <c r="AU545" s="8" t="s">
         <v>439</v>
       </c>
       <c r="AV545" s="6"/>
@@ -76785,14 +76808,14 @@
       <c r="H546" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I546" s="6"/>
-      <c r="J546" s="6"/>
-      <c r="K546" s="6"/>
+      <c r="I546" s="9"/>
+      <c r="J546" s="9"/>
+      <c r="K546" s="9"/>
       <c r="L546" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M546" s="6"/>
-      <c r="N546" s="6"/>
+      <c r="M546" s="9"/>
+      <c r="N546" s="9"/>
       <c r="O546" s="7" t="s">
         <v>44</v>
       </c>
@@ -76889,7 +76912,7 @@
       <c r="AT546" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU546" s="6"/>
+      <c r="AU546" s="9"/>
       <c r="AV546" s="6"/>
     </row>
     <row r="547" spans="2:48" x14ac:dyDescent="0.25">
@@ -76914,14 +76937,14 @@
       <c r="H547" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I547" s="6"/>
-      <c r="J547" s="6"/>
-      <c r="K547" s="6"/>
+      <c r="I547" s="9"/>
+      <c r="J547" s="9"/>
+      <c r="K547" s="9"/>
       <c r="L547" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M547" s="6"/>
-      <c r="N547" s="6"/>
+      <c r="M547" s="11"/>
+      <c r="N547" s="9"/>
       <c r="O547" s="7" t="s">
         <v>44</v>
       </c>
@@ -77018,7 +77041,7 @@
       <c r="AT547" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU547" s="6"/>
+      <c r="AU547" s="9"/>
       <c r="AV547" s="6"/>
     </row>
     <row r="548" spans="2:48" x14ac:dyDescent="0.25">
@@ -77043,16 +77066,16 @@
       <c r="H548" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I548" s="6"/>
-      <c r="J548" s="6"/>
-      <c r="K548" s="6"/>
-      <c r="L548" s="6" t="s">
+      <c r="I548" s="9"/>
+      <c r="J548" s="11"/>
+      <c r="K548" s="9"/>
+      <c r="L548" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M548" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="N548" s="6"/>
+      <c r="N548" s="9"/>
       <c r="O548" s="7" t="s">
         <v>44</v>
       </c>
@@ -77149,7 +77172,7 @@
       <c r="AT548" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU548" s="6"/>
+      <c r="AU548" s="9"/>
       <c r="AV548" s="6"/>
     </row>
     <row r="549" spans="2:48" x14ac:dyDescent="0.25">
@@ -77174,16 +77197,16 @@
       <c r="H549" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I549" s="6"/>
-      <c r="J549" s="6" t="s">
+      <c r="I549" s="9"/>
+      <c r="J549" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="K549" s="6"/>
-      <c r="L549" s="6"/>
+      <c r="K549" s="9"/>
+      <c r="L549" s="9"/>
       <c r="M549" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N549" s="6"/>
+      <c r="N549" s="9"/>
       <c r="O549" s="7" t="s">
         <v>44</v>
       </c>
@@ -77280,7 +77303,7 @@
       <c r="AT549" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU549" s="6"/>
+      <c r="AU549" s="9"/>
       <c r="AV549" s="6"/>
     </row>
     <row r="550" spans="2:48" x14ac:dyDescent="0.25">
@@ -77305,16 +77328,14 @@
       <c r="H550" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I550" s="6"/>
-      <c r="J550" s="6"/>
-      <c r="K550" s="6"/>
-      <c r="L550" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="M550" s="6" t="s">
+      <c r="I550" s="11"/>
+      <c r="J550" s="11"/>
+      <c r="K550" s="9"/>
+      <c r="L550" s="11"/>
+      <c r="M550" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="N550" s="6"/>
+      <c r="N550" s="9"/>
       <c r="O550" s="7" t="s">
         <v>44</v>
       </c>
@@ -77411,7 +77432,7 @@
       <c r="AT550" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU550" s="6"/>
+      <c r="AU550" s="9"/>
       <c r="AV550" s="6"/>
     </row>
     <row r="551" spans="2:48" x14ac:dyDescent="0.25">
@@ -77436,18 +77457,18 @@
       <c r="H551" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I551" s="6" t="s">
+      <c r="I551" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="J551" s="6" t="s">
+      <c r="J551" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="K551" s="6"/>
+      <c r="K551" s="9"/>
       <c r="L551" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M551" s="6"/>
-      <c r="N551" s="6"/>
+      <c r="M551" s="9"/>
+      <c r="N551" s="9"/>
       <c r="O551" s="7" t="s">
         <v>44</v>
       </c>
@@ -77544,7 +77565,7 @@
       <c r="AT551" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU551" s="6"/>
+      <c r="AU551" s="9"/>
       <c r="AV551" s="6"/>
     </row>
     <row r="552" spans="2:48" x14ac:dyDescent="0.25">
@@ -77569,14 +77590,14 @@
       <c r="H552" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="I552" s="6"/>
-      <c r="J552" s="6"/>
-      <c r="K552" s="6"/>
+      <c r="I552" s="11"/>
+      <c r="J552" s="11"/>
+      <c r="K552" s="9"/>
       <c r="L552" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="M552" s="6"/>
-      <c r="N552" s="6"/>
+      <c r="M552" s="11"/>
+      <c r="N552" s="9"/>
       <c r="O552" s="7" t="s">
         <v>44</v>
       </c>
@@ -77673,7 +77694,7 @@
       <c r="AT552" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU552" s="6"/>
+      <c r="AU552" s="9"/>
       <c r="AV552" s="6"/>
     </row>
     <row r="553" spans="2:48" x14ac:dyDescent="0.25">
@@ -77698,20 +77719,20 @@
       <c r="H553" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I553" s="6" t="s">
+      <c r="I553" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J553" s="6" t="s">
+      <c r="J553" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K553" s="6"/>
-      <c r="L553" s="6" t="s">
+      <c r="K553" s="9"/>
+      <c r="L553" s="8" t="s">
         <v>42</v>
       </c>
       <c r="M553" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="N553" s="6"/>
+      <c r="N553" s="9"/>
       <c r="O553" s="7" t="s">
         <v>44</v>
       </c>
@@ -77808,7 +77829,7 @@
       <c r="AT553" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU553" s="6"/>
+      <c r="AU553" s="9"/>
       <c r="AV553" s="6"/>
     </row>
     <row r="554" spans="2:48" x14ac:dyDescent="0.25">
@@ -77833,14 +77854,14 @@
       <c r="H554" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I554" s="6"/>
-      <c r="J554" s="6"/>
-      <c r="K554" s="6"/>
-      <c r="L554" s="6"/>
+      <c r="I554" s="11"/>
+      <c r="J554" s="11"/>
+      <c r="K554" s="9"/>
+      <c r="L554" s="11"/>
       <c r="M554" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="N554" s="6"/>
+      <c r="N554" s="9"/>
       <c r="O554" s="7" t="s">
         <v>44</v>
       </c>
@@ -77937,7 +77958,7 @@
       <c r="AT554" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU554" s="6"/>
+      <c r="AU554" s="9"/>
       <c r="AV554" s="6"/>
     </row>
     <row r="555" spans="2:48" x14ac:dyDescent="0.25">
@@ -77962,20 +77983,20 @@
       <c r="H555" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="I555" s="6" t="s">
+      <c r="I555" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J555" s="6" t="s">
+      <c r="J555" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K555" s="6"/>
+      <c r="K555" s="9"/>
       <c r="L555" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="M555" s="6" t="s">
+      <c r="M555" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="N555" s="6"/>
+      <c r="N555" s="9"/>
       <c r="O555" s="7" t="s">
         <v>44</v>
       </c>
@@ -78072,7 +78093,7 @@
       <c r="AT555" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU555" s="6"/>
+      <c r="AU555" s="9"/>
       <c r="AV555" s="6"/>
     </row>
     <row r="556" spans="2:48" x14ac:dyDescent="0.25">
@@ -78097,14 +78118,14 @@
       <c r="H556" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I556" s="6"/>
-      <c r="J556" s="6"/>
-      <c r="K556" s="6"/>
+      <c r="I556" s="11"/>
+      <c r="J556" s="11"/>
+      <c r="K556" s="11"/>
       <c r="L556" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="M556" s="6"/>
-      <c r="N556" s="6"/>
+      <c r="M556" s="11"/>
+      <c r="N556" s="9"/>
       <c r="O556" s="7" t="s">
         <v>44</v>
       </c>
@@ -78201,7 +78222,7 @@
       <c r="AT556" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU556" s="6"/>
+      <c r="AU556" s="9"/>
       <c r="AV556" s="6"/>
     </row>
     <row r="557" spans="2:48" x14ac:dyDescent="0.25">
@@ -78226,22 +78247,22 @@
       <c r="H557" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="I557" s="6" t="s">
+      <c r="I557" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="J557" s="6" t="s">
+      <c r="J557" s="8" t="s">
         <v>37</v>
       </c>
       <c r="K557" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L557" s="6" t="s">
+      <c r="L557" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="M557" s="6" t="s">
+      <c r="M557" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N557" s="6"/>
+      <c r="N557" s="9"/>
       <c r="O557" s="7" t="s">
         <v>44</v>
       </c>
@@ -78338,7 +78359,7 @@
       <c r="AT557" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU557" s="6"/>
+      <c r="AU557" s="9"/>
       <c r="AV557" s="6"/>
     </row>
     <row r="558" spans="2:48" x14ac:dyDescent="0.25">
@@ -78363,14 +78384,14 @@
       <c r="H558" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I558" s="6"/>
-      <c r="J558" s="6"/>
+      <c r="I558" s="9"/>
+      <c r="J558" s="9"/>
       <c r="K558" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L558" s="6"/>
-      <c r="M558" s="6"/>
-      <c r="N558" s="6"/>
+      <c r="L558" s="9"/>
+      <c r="M558" s="11"/>
+      <c r="N558" s="11"/>
       <c r="O558" s="7" t="s">
         <v>44</v>
       </c>
@@ -78467,7 +78488,7 @@
       <c r="AT558" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU558" s="6"/>
+      <c r="AU558" s="9"/>
       <c r="AV558" s="6"/>
     </row>
     <row r="559" spans="2:48" x14ac:dyDescent="0.25">
@@ -78492,12 +78513,12 @@
       <c r="H559" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I559" s="6"/>
-      <c r="J559" s="6"/>
+      <c r="I559" s="9"/>
+      <c r="J559" s="9"/>
       <c r="K559" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L559" s="6"/>
+      <c r="L559" s="9"/>
       <c r="M559" s="6" t="s">
         <v>52</v>
       </c>
@@ -78600,7 +78621,7 @@
       <c r="AT559" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU559" s="6"/>
+      <c r="AU559" s="9"/>
       <c r="AV559" s="6"/>
     </row>
     <row r="560" spans="2:48" x14ac:dyDescent="0.25">
@@ -78625,13 +78646,13 @@
       <c r="H560" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I560" s="6"/>
-      <c r="J560" s="6"/>
+      <c r="I560" s="9"/>
+      <c r="J560" s="11"/>
       <c r="K560" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L560" s="6"/>
-      <c r="M560" s="6" t="s">
+      <c r="L560" s="9"/>
+      <c r="M560" s="8" t="s">
         <v>62</v>
       </c>
       <c r="N560" s="6" t="s">
@@ -78733,7 +78754,7 @@
       <c r="AT560" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU560" s="6"/>
+      <c r="AU560" s="9"/>
       <c r="AV560" s="6"/>
     </row>
     <row r="561" spans="2:48" x14ac:dyDescent="0.25">
@@ -78758,15 +78779,15 @@
       <c r="H561" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I561" s="6"/>
-      <c r="J561" s="6" t="s">
+      <c r="I561" s="9"/>
+      <c r="J561" s="8" t="s">
         <v>42</v>
       </c>
       <c r="K561" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="L561" s="6"/>
-      <c r="M561" s="6"/>
+      <c r="L561" s="11"/>
+      <c r="M561" s="11"/>
       <c r="N561" s="6" t="s">
         <v>412</v>
       </c>
@@ -78866,7 +78887,7 @@
       <c r="AT561" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU561" s="6"/>
+      <c r="AU561" s="9"/>
       <c r="AV561" s="6"/>
     </row>
     <row r="562" spans="2:48" x14ac:dyDescent="0.25">
@@ -78891,15 +78912,15 @@
       <c r="H562" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I562" s="6"/>
-      <c r="J562" s="6"/>
-      <c r="K562" s="6" t="s">
+      <c r="I562" s="11"/>
+      <c r="J562" s="11"/>
+      <c r="K562" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="L562" s="6" t="s">
+      <c r="L562" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="M562" s="6" t="s">
+      <c r="M562" s="8" t="s">
         <v>52</v>
       </c>
       <c r="N562" s="6" t="s">
@@ -79001,7 +79022,7 @@
       <c r="AT562" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU562" s="6"/>
+      <c r="AU562" s="11"/>
       <c r="AV562" s="6"/>
     </row>
     <row r="563" spans="2:48" x14ac:dyDescent="0.25">
@@ -79032,15 +79053,9 @@
       <c r="J563" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K563" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L563" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M563" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="K563" s="11"/>
+      <c r="L563" s="11"/>
+      <c r="M563" s="11"/>
       <c r="N563" s="7" t="s">
         <v>44</v>
       </c>
@@ -79109,13 +79124,13 @@
       <c r="J564" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K564" s="6" t="s">
+      <c r="K564" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="L564" s="6" t="s">
+      <c r="L564" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="M564" s="6" t="s">
+      <c r="M564" s="8" t="s">
         <v>36</v>
       </c>
       <c r="N564" s="7" t="s">
@@ -79186,15 +79201,9 @@
       <c r="J565" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="K565" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="L565" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="M565" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="K565" s="11"/>
+      <c r="L565" s="11"/>
+      <c r="M565" s="11"/>
       <c r="N565" s="7" t="s">
         <v>44</v>
       </c>
@@ -79331,13 +79340,13 @@
       <c r="G567" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H567" s="6" t="s">
+      <c r="H567" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="I567" s="6" t="s">
+      <c r="I567" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J567" s="6" t="s">
+      <c r="J567" s="8" t="s">
         <v>36</v>
       </c>
       <c r="K567" s="7" t="s">
@@ -79384,7 +79393,9 @@
       <c r="AR567" s="6"/>
       <c r="AS567" s="6"/>
       <c r="AT567" s="6"/>
-      <c r="AU567" s="6"/>
+      <c r="AU567" s="6" t="s">
+        <v>497</v>
+      </c>
       <c r="AV567" s="6"/>
     </row>
     <row r="568" spans="2:48" x14ac:dyDescent="0.25">
@@ -79406,15 +79417,9 @@
       <c r="G568" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H568" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I568" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J568" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="H568" s="11"/>
+      <c r="I568" s="11"/>
+      <c r="J568" s="11"/>
       <c r="K568" s="7" t="s">
         <v>44</v>
       </c>
@@ -79459,7 +79464,9 @@
       <c r="AR568" s="6"/>
       <c r="AS568" s="6"/>
       <c r="AT568" s="6"/>
-      <c r="AU568" s="6"/>
+      <c r="AU568" s="6" t="s">
+        <v>498</v>
+      </c>
       <c r="AV568" s="6"/>
     </row>
     <row r="569" spans="2:48" x14ac:dyDescent="0.25">
@@ -79490,10 +79497,10 @@
       <c r="J569" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K569" s="6" t="s">
+      <c r="K569" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="L569" s="6" t="s">
+      <c r="L569" s="8" t="s">
         <v>52</v>
       </c>
       <c r="M569" s="6" t="s">
@@ -79534,7 +79541,9 @@
       <c r="AR569" s="6"/>
       <c r="AS569" s="6"/>
       <c r="AT569" s="6"/>
-      <c r="AU569" s="6"/>
+      <c r="AU569" s="6" t="s">
+        <v>499</v>
+      </c>
       <c r="AV569" s="6"/>
     </row>
     <row r="570" spans="2:48" x14ac:dyDescent="0.25">
@@ -79565,13 +79574,9 @@
       <c r="J570" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K570" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L570" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M570" s="6" t="s">
+      <c r="K570" s="9"/>
+      <c r="L570" s="9"/>
+      <c r="M570" s="8" t="s">
         <v>36</v>
       </c>
       <c r="N570" s="6" t="s">
@@ -79609,7 +79614,9 @@
       <c r="AR570" s="6"/>
       <c r="AS570" s="6"/>
       <c r="AT570" s="6"/>
-      <c r="AU570" s="6"/>
+      <c r="AU570" s="6" t="s">
+        <v>500</v>
+      </c>
       <c r="AV570" s="6"/>
     </row>
     <row r="571" spans="2:48" x14ac:dyDescent="0.25">
@@ -79640,15 +79647,9 @@
       <c r="J571" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K571" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L571" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M571" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="K571" s="9"/>
+      <c r="L571" s="9"/>
+      <c r="M571" s="11"/>
       <c r="N571" s="6" t="s">
         <v>344</v>
       </c>
@@ -79684,7 +79685,9 @@
       <c r="AR571" s="6"/>
       <c r="AS571" s="6"/>
       <c r="AT571" s="6"/>
-      <c r="AU571" s="6"/>
+      <c r="AU571" s="6" t="s">
+        <v>501</v>
+      </c>
       <c r="AV571" s="6"/>
     </row>
     <row r="572" spans="2:48" x14ac:dyDescent="0.25">
@@ -79706,21 +79709,17 @@
       <c r="G572" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H572" s="6" t="s">
+      <c r="H572" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="I572" s="6" t="s">
+      <c r="I572" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="J572" s="6" t="s">
+      <c r="J572" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K572" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L572" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="K572" s="9"/>
+      <c r="L572" s="9"/>
       <c r="M572" s="6" t="s">
         <v>42</v>
       </c>
@@ -79759,7 +79758,9 @@
       <c r="AR572" s="6"/>
       <c r="AS572" s="6"/>
       <c r="AT572" s="6"/>
-      <c r="AU572" s="6"/>
+      <c r="AU572" s="6" t="s">
+        <v>502</v>
+      </c>
       <c r="AV572" s="6"/>
     </row>
     <row r="573" spans="2:48" x14ac:dyDescent="0.25">
@@ -79781,25 +79782,15 @@
       <c r="G573" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H573" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I573" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="J573" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K573" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L573" s="6" t="s">
-        <v>52</v>
-      </c>
+      <c r="H573" s="11"/>
+      <c r="I573" s="11"/>
+      <c r="J573" s="9"/>
+      <c r="K573" s="9"/>
+      <c r="L573" s="9"/>
       <c r="M573" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="N573" s="6" t="s">
+      <c r="N573" s="8" t="s">
         <v>344</v>
       </c>
       <c r="O573" s="6"/>
@@ -79834,7 +79825,9 @@
       <c r="AR573" s="6"/>
       <c r="AS573" s="6"/>
       <c r="AT573" s="6"/>
-      <c r="AU573" s="6"/>
+      <c r="AU573" s="6" t="s">
+        <v>503</v>
+      </c>
       <c r="AV573" s="6"/>
     </row>
     <row r="574" spans="2:48" x14ac:dyDescent="0.25">
@@ -79862,21 +79855,13 @@
       <c r="I574" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="J574" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K574" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L574" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M574" s="6" t="s">
+      <c r="J574" s="9"/>
+      <c r="K574" s="9"/>
+      <c r="L574" s="9"/>
+      <c r="M574" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N574" s="6" t="s">
-        <v>344</v>
-      </c>
+      <c r="N574" s="11"/>
       <c r="O574" s="6"/>
       <c r="P574" s="6"/>
       <c r="Q574" s="6"/>
@@ -79909,7 +79894,9 @@
       <c r="AR574" s="6"/>
       <c r="AS574" s="6"/>
       <c r="AT574" s="6"/>
-      <c r="AU574" s="6"/>
+      <c r="AU574" s="6" t="s">
+        <v>504</v>
+      </c>
       <c r="AV574" s="6"/>
     </row>
     <row r="575" spans="2:48" x14ac:dyDescent="0.25">
@@ -79937,18 +79924,10 @@
       <c r="I575" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="J575" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K575" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L575" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="M575" s="6" t="s">
-        <v>36</v>
-      </c>
+      <c r="J575" s="11"/>
+      <c r="K575" s="11"/>
+      <c r="L575" s="11"/>
+      <c r="M575" s="11"/>
       <c r="N575" s="6" t="s">
         <v>453</v>
       </c>
@@ -79984,7 +79963,9 @@
       <c r="AR575" s="6"/>
       <c r="AS575" s="6"/>
       <c r="AT575" s="6"/>
-      <c r="AU575" s="6"/>
+      <c r="AU575" s="6" t="s">
+        <v>505</v>
+      </c>
       <c r="AV575" s="6"/>
     </row>
     <row r="576" spans="2:48" x14ac:dyDescent="0.25">
@@ -80123,7 +80104,7 @@
       <c r="AT576" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU576" s="6" t="s">
+      <c r="AU576" s="8" t="s">
         <v>445</v>
       </c>
       <c r="AV576" s="6"/>
@@ -80264,7 +80245,7 @@
       <c r="AT577" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU577" s="6"/>
+      <c r="AU577" s="9"/>
       <c r="AV577" s="6"/>
     </row>
     <row r="578" spans="2:48" x14ac:dyDescent="0.25">
@@ -80403,7 +80384,7 @@
       <c r="AT578" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU578" s="6"/>
+      <c r="AU578" s="9"/>
       <c r="AV578" s="6"/>
     </row>
     <row r="579" spans="2:48" x14ac:dyDescent="0.25">
@@ -80542,7 +80523,7 @@
       <c r="AT579" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU579" s="6"/>
+      <c r="AU579" s="9"/>
       <c r="AV579" s="6"/>
     </row>
     <row r="580" spans="2:48" x14ac:dyDescent="0.25">
@@ -80681,7 +80662,7 @@
       <c r="AT580" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU580" s="6"/>
+      <c r="AU580" s="9"/>
       <c r="AV580" s="6"/>
     </row>
     <row r="581" spans="2:48" x14ac:dyDescent="0.25">
@@ -80820,7 +80801,7 @@
       <c r="AT581" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU581" s="6"/>
+      <c r="AU581" s="9"/>
       <c r="AV581" s="6"/>
     </row>
     <row r="582" spans="2:48" x14ac:dyDescent="0.25">
@@ -80959,7 +80940,7 @@
       <c r="AT582" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU582" s="6"/>
+      <c r="AU582" s="9"/>
       <c r="AV582" s="6"/>
     </row>
     <row r="583" spans="2:48" x14ac:dyDescent="0.25">
@@ -81096,7 +81077,7 @@
       <c r="AT583" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU583" s="6"/>
+      <c r="AU583" s="9"/>
       <c r="AV583" s="6"/>
     </row>
     <row r="584" spans="2:48" x14ac:dyDescent="0.25">
@@ -81235,7 +81216,7 @@
       <c r="AT584" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU584" s="6"/>
+      <c r="AU584" s="9"/>
       <c r="AV584" s="6"/>
     </row>
     <row r="585" spans="2:48" x14ac:dyDescent="0.25">
@@ -81374,7 +81355,7 @@
       <c r="AT585" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU585" s="6"/>
+      <c r="AU585" s="9"/>
       <c r="AV585" s="6"/>
     </row>
     <row r="586" spans="2:48" x14ac:dyDescent="0.25">
@@ -81511,7 +81492,7 @@
       <c r="AT586" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU586" s="6"/>
+      <c r="AU586" s="9"/>
       <c r="AV586" s="6"/>
     </row>
     <row r="587" spans="2:48" x14ac:dyDescent="0.25">
@@ -81650,7 +81631,7 @@
       <c r="AT587" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU587" s="6"/>
+      <c r="AU587" s="9"/>
       <c r="AV587" s="6"/>
     </row>
     <row r="588" spans="2:48" x14ac:dyDescent="0.25">
@@ -81789,7 +81770,7 @@
       <c r="AT588" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU588" s="6"/>
+      <c r="AU588" s="9"/>
       <c r="AV588" s="6"/>
     </row>
     <row r="589" spans="2:48" x14ac:dyDescent="0.25">
@@ -81924,7 +81905,7 @@
       <c r="AT589" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU589" s="6"/>
+      <c r="AU589" s="9"/>
       <c r="AV589" s="6"/>
     </row>
     <row r="590" spans="2:48" x14ac:dyDescent="0.25">
@@ -82057,7 +82038,7 @@
       <c r="AT590" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU590" s="6"/>
+      <c r="AU590" s="9"/>
       <c r="AV590" s="6"/>
     </row>
     <row r="591" spans="2:48" x14ac:dyDescent="0.25">
@@ -82196,7 +82177,7 @@
       <c r="AT591" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU591" s="6"/>
+      <c r="AU591" s="9"/>
       <c r="AV591" s="6"/>
     </row>
     <row r="592" spans="2:48" x14ac:dyDescent="0.25">
@@ -82335,7 +82316,7 @@
       <c r="AT592" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU592" s="6"/>
+      <c r="AU592" s="9"/>
       <c r="AV592" s="6"/>
     </row>
     <row r="593" spans="2:48" x14ac:dyDescent="0.25">
@@ -82472,7 +82453,7 @@
       <c r="AT593" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU593" s="6"/>
+      <c r="AU593" s="9"/>
       <c r="AV593" s="6"/>
     </row>
     <row r="594" spans="2:48" x14ac:dyDescent="0.25">
@@ -82611,7 +82592,7 @@
       <c r="AT594" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU594" s="6"/>
+      <c r="AU594" s="9"/>
       <c r="AV594" s="6"/>
     </row>
     <row r="595" spans="2:48" x14ac:dyDescent="0.25">
@@ -82750,7 +82731,7 @@
       <c r="AT595" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU595" s="6"/>
+      <c r="AU595" s="9"/>
       <c r="AV595" s="6"/>
     </row>
     <row r="596" spans="2:48" x14ac:dyDescent="0.25">
@@ -82889,7 +82870,7 @@
       <c r="AT596" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU596" s="6"/>
+      <c r="AU596" s="9"/>
       <c r="AV596" s="6"/>
     </row>
     <row r="597" spans="2:48" x14ac:dyDescent="0.25">
@@ -83020,7 +83001,7 @@
       <c r="AT597" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU597" s="6"/>
+      <c r="AU597" s="9"/>
       <c r="AV597" s="6"/>
     </row>
     <row r="598" spans="2:48" x14ac:dyDescent="0.25">
@@ -83149,7 +83130,7 @@
       <c r="AT598" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU598" s="6"/>
+      <c r="AU598" s="9"/>
       <c r="AV598" s="6"/>
     </row>
     <row r="599" spans="2:48" x14ac:dyDescent="0.25">
@@ -83278,7 +83259,7 @@
       <c r="AT599" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU599" s="6"/>
+      <c r="AU599" s="9"/>
       <c r="AV599" s="6"/>
     </row>
     <row r="600" spans="2:48" x14ac:dyDescent="0.25">
@@ -83409,7 +83390,7 @@
       <c r="AT600" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU600" s="6"/>
+      <c r="AU600" s="9"/>
       <c r="AV600" s="6"/>
     </row>
     <row r="601" spans="2:48" x14ac:dyDescent="0.25">
@@ -83544,7 +83525,7 @@
       <c r="AT601" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU601" s="6"/>
+      <c r="AU601" s="9"/>
       <c r="AV601" s="6"/>
     </row>
     <row r="602" spans="2:48" x14ac:dyDescent="0.25">
@@ -83679,7 +83660,7 @@
       <c r="AT602" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU602" s="6"/>
+      <c r="AU602" s="9"/>
       <c r="AV602" s="6"/>
     </row>
     <row r="603" spans="2:48" x14ac:dyDescent="0.25">
@@ -83810,7 +83791,7 @@
       <c r="AT603" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU603" s="6"/>
+      <c r="AU603" s="9"/>
       <c r="AV603" s="6"/>
     </row>
     <row r="604" spans="2:48" x14ac:dyDescent="0.25">
@@ -83939,7 +83920,7 @@
       <c r="AT604" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU604" s="6"/>
+      <c r="AU604" s="9"/>
       <c r="AV604" s="6"/>
     </row>
     <row r="605" spans="2:48" x14ac:dyDescent="0.25">
@@ -84070,7 +84051,7 @@
       <c r="AT605" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU605" s="6"/>
+      <c r="AU605" s="9"/>
       <c r="AV605" s="6"/>
     </row>
     <row r="606" spans="2:48" x14ac:dyDescent="0.25">
@@ -84205,7 +84186,7 @@
       <c r="AT606" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU606" s="6"/>
+      <c r="AU606" s="9"/>
       <c r="AV606" s="6"/>
     </row>
     <row r="607" spans="2:48" x14ac:dyDescent="0.25">
@@ -84338,7 +84319,7 @@
       <c r="AT607" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU607" s="6"/>
+      <c r="AU607" s="9"/>
       <c r="AV607" s="6"/>
     </row>
     <row r="608" spans="2:48" x14ac:dyDescent="0.25">
@@ -84475,7 +84456,7 @@
       <c r="AT608" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU608" s="6"/>
+      <c r="AU608" s="9"/>
       <c r="AV608" s="6"/>
     </row>
     <row r="609" spans="2:48" x14ac:dyDescent="0.25">
@@ -84610,7 +84591,7 @@
       <c r="AT609" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU609" s="6"/>
+      <c r="AU609" s="9"/>
       <c r="AV609" s="6"/>
     </row>
     <row r="610" spans="2:48" x14ac:dyDescent="0.25">
@@ -84745,7 +84726,7 @@
       <c r="AT610" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU610" s="6"/>
+      <c r="AU610" s="9"/>
       <c r="AV610" s="6"/>
     </row>
     <row r="611" spans="2:48" x14ac:dyDescent="0.25">
@@ -84876,7 +84857,7 @@
       <c r="AT611" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU611" s="6"/>
+      <c r="AU611" s="9"/>
       <c r="AV611" s="6"/>
     </row>
     <row r="612" spans="2:48" x14ac:dyDescent="0.25">
@@ -85013,7 +84994,7 @@
       <c r="AT612" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU612" s="6"/>
+      <c r="AU612" s="9"/>
       <c r="AV612" s="6"/>
     </row>
     <row r="613" spans="2:48" x14ac:dyDescent="0.25">
@@ -85148,7 +85129,7 @@
       <c r="AT613" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU613" s="6"/>
+      <c r="AU613" s="9"/>
       <c r="AV613" s="6"/>
     </row>
     <row r="614" spans="2:48" x14ac:dyDescent="0.25">
@@ -85283,7 +85264,7 @@
       <c r="AT614" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU614" s="6"/>
+      <c r="AU614" s="9"/>
       <c r="AV614" s="6"/>
     </row>
     <row r="615" spans="2:48" x14ac:dyDescent="0.25">
@@ -85418,7 +85399,7 @@
       <c r="AT615" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU615" s="6"/>
+      <c r="AU615" s="9"/>
       <c r="AV615" s="6"/>
     </row>
     <row r="616" spans="2:48" x14ac:dyDescent="0.25">
@@ -85555,7 +85536,7 @@
       <c r="AT616" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU616" s="6"/>
+      <c r="AU616" s="9"/>
       <c r="AV616" s="6"/>
     </row>
     <row r="617" spans="2:48" x14ac:dyDescent="0.25">
@@ -85690,7 +85671,7 @@
       <c r="AT617" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU617" s="6"/>
+      <c r="AU617" s="9"/>
       <c r="AV617" s="6"/>
     </row>
     <row r="618" spans="2:48" x14ac:dyDescent="0.25">
@@ -85825,7 +85806,7 @@
       <c r="AT618" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU618" s="6"/>
+      <c r="AU618" s="9"/>
       <c r="AV618" s="6"/>
     </row>
     <row r="619" spans="2:48" x14ac:dyDescent="0.25">
@@ -85960,7 +85941,7 @@
       <c r="AT619" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU619" s="6"/>
+      <c r="AU619" s="9"/>
       <c r="AV619" s="6"/>
     </row>
     <row r="620" spans="2:48" x14ac:dyDescent="0.25">
@@ -86097,7 +86078,7 @@
       <c r="AT620" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU620" s="6"/>
+      <c r="AU620" s="9"/>
       <c r="AV620" s="6"/>
     </row>
     <row r="621" spans="2:48" x14ac:dyDescent="0.25">
@@ -86234,7 +86215,7 @@
       <c r="AT621" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU621" s="6"/>
+      <c r="AU621" s="9"/>
       <c r="AV621" s="6"/>
     </row>
     <row r="622" spans="2:48" x14ac:dyDescent="0.25">
@@ -86367,7 +86348,7 @@
       <c r="AT622" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU622" s="6"/>
+      <c r="AU622" s="11"/>
       <c r="AV622" s="6"/>
     </row>
     <row r="623" spans="2:48" x14ac:dyDescent="0.25">
@@ -86506,7 +86487,7 @@
       <c r="AT623" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU623" s="6" t="s">
+      <c r="AU623" s="8" t="s">
         <v>446</v>
       </c>
       <c r="AV623" s="6"/>
@@ -86647,7 +86628,7 @@
       <c r="AT624" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU624" s="6"/>
+      <c r="AU624" s="9"/>
       <c r="AV624" s="6"/>
     </row>
     <row r="625" spans="2:48" x14ac:dyDescent="0.25">
@@ -86782,7 +86763,7 @@
       <c r="AT625" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU625" s="6"/>
+      <c r="AU625" s="9"/>
       <c r="AV625" s="6"/>
     </row>
     <row r="626" spans="2:48" x14ac:dyDescent="0.25">
@@ -86919,7 +86900,7 @@
       <c r="AT626" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU626" s="6"/>
+      <c r="AU626" s="9"/>
       <c r="AV626" s="6"/>
     </row>
     <row r="627" spans="2:48" x14ac:dyDescent="0.25">
@@ -87048,7 +87029,7 @@
       <c r="AT627" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU627" s="6"/>
+      <c r="AU627" s="9"/>
       <c r="AV627" s="6"/>
     </row>
     <row r="628" spans="2:48" x14ac:dyDescent="0.25">
@@ -87177,14 +87158,14 @@
       <c r="AT628" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU628" s="6"/>
+      <c r="AU628" s="11"/>
       <c r="AV628" s="6"/>
     </row>
     <row r="629" spans="2:48" x14ac:dyDescent="0.25">
       <c r="B629" s="6">
         <v>624</v>
       </c>
-      <c r="C629" s="6" t="s">
+      <c r="C629" s="8" t="s">
         <v>115</v>
       </c>
       <c r="D629" s="7" t="s">
@@ -87312,7 +87293,7 @@
       <c r="AT629" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU629" s="6" t="s">
+      <c r="AU629" s="8" t="s">
         <v>438</v>
       </c>
       <c r="AV629" s="6"/>
@@ -87321,7 +87302,7 @@
       <c r="B630" s="6">
         <v>625</v>
       </c>
-      <c r="C630" s="6"/>
+      <c r="C630" s="11"/>
       <c r="D630" s="7" t="s">
         <v>44</v>
       </c>
@@ -87447,7 +87428,7 @@
       <c r="AT630" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="AU630" s="6"/>
+      <c r="AU630" s="11"/>
       <c r="AV630" s="6"/>
     </row>
     <row r="631" spans="2:48" x14ac:dyDescent="0.25">
@@ -92555,7 +92536,80 @@
       <c r="AV688" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="169">
+  <mergeCells count="253">
+    <mergeCell ref="I534:I535"/>
+    <mergeCell ref="J534:J535"/>
+    <mergeCell ref="J536:J537"/>
+    <mergeCell ref="I536:I537"/>
+    <mergeCell ref="I520:I521"/>
+    <mergeCell ref="N522:N533"/>
+    <mergeCell ref="J522:J525"/>
+    <mergeCell ref="I522:I527"/>
+    <mergeCell ref="J526:J527"/>
+    <mergeCell ref="J528:J529"/>
+    <mergeCell ref="I528:I529"/>
+    <mergeCell ref="I530:I531"/>
+    <mergeCell ref="J530:J531"/>
+    <mergeCell ref="J532:J533"/>
+    <mergeCell ref="I532:I533"/>
+    <mergeCell ref="J520:J521"/>
+    <mergeCell ref="L520:L521"/>
+    <mergeCell ref="I508:I513"/>
+    <mergeCell ref="J508:J511"/>
+    <mergeCell ref="K508:K519"/>
+    <mergeCell ref="J512:J513"/>
+    <mergeCell ref="I514:I515"/>
+    <mergeCell ref="J514:J515"/>
+    <mergeCell ref="M513:M515"/>
+    <mergeCell ref="M508:M510"/>
+    <mergeCell ref="L511:L512"/>
+    <mergeCell ref="M518:M519"/>
+    <mergeCell ref="J516:J517"/>
+    <mergeCell ref="I516:I517"/>
+    <mergeCell ref="I518:I519"/>
+    <mergeCell ref="J518:J519"/>
+    <mergeCell ref="L516:L518"/>
+    <mergeCell ref="K564:K565"/>
+    <mergeCell ref="L564:L565"/>
+    <mergeCell ref="M564:M565"/>
+    <mergeCell ref="M562:M563"/>
+    <mergeCell ref="L562:L563"/>
+    <mergeCell ref="K562:K563"/>
+    <mergeCell ref="L538:L544"/>
+    <mergeCell ref="M539:M540"/>
+    <mergeCell ref="M542:M543"/>
+    <mergeCell ref="J561:J562"/>
+    <mergeCell ref="J557:J560"/>
+    <mergeCell ref="I557:I562"/>
+    <mergeCell ref="L557:L561"/>
+    <mergeCell ref="M557:M558"/>
+    <mergeCell ref="M560:M561"/>
+    <mergeCell ref="M555:M556"/>
+    <mergeCell ref="L553:L554"/>
+    <mergeCell ref="J553:J554"/>
+    <mergeCell ref="I553:I554"/>
+    <mergeCell ref="I555:I556"/>
+    <mergeCell ref="J555:J556"/>
+    <mergeCell ref="K545:K556"/>
+    <mergeCell ref="M545:M547"/>
+    <mergeCell ref="M550:M552"/>
+    <mergeCell ref="L548:L550"/>
+    <mergeCell ref="J545:J548"/>
+    <mergeCell ref="I545:I550"/>
+    <mergeCell ref="J549:J550"/>
+    <mergeCell ref="J551:J552"/>
+    <mergeCell ref="I551:I552"/>
+    <mergeCell ref="J572:J575"/>
+    <mergeCell ref="I572:I573"/>
+    <mergeCell ref="H572:H573"/>
+    <mergeCell ref="K569:K575"/>
+    <mergeCell ref="L569:L575"/>
+    <mergeCell ref="M570:M571"/>
+    <mergeCell ref="M574:M575"/>
+    <mergeCell ref="N573:N574"/>
+    <mergeCell ref="H567:H568"/>
+    <mergeCell ref="I567:I568"/>
+    <mergeCell ref="J567:J568"/>
     <mergeCell ref="M405:M407"/>
     <mergeCell ref="H16:H49"/>
     <mergeCell ref="J37:J41"/>
@@ -92709,6 +92763,16 @@
     <mergeCell ref="L626:L628"/>
     <mergeCell ref="L629:L630"/>
     <mergeCell ref="L588:L590"/>
+    <mergeCell ref="AU497:AU507"/>
+    <mergeCell ref="AU508:AU521"/>
+    <mergeCell ref="AU522:AU537"/>
+    <mergeCell ref="AU538:AU544"/>
+    <mergeCell ref="AU545:AU562"/>
+    <mergeCell ref="AU576:AU622"/>
+    <mergeCell ref="AU623:AU628"/>
+    <mergeCell ref="AU629:AU630"/>
+    <mergeCell ref="N545:N558"/>
+    <mergeCell ref="N538:N540"/>
     <mergeCell ref="K626:K629"/>
     <mergeCell ref="J626:J628"/>
     <mergeCell ref="J629:J630"/>
@@ -92725,6 +92789,7 @@
     <mergeCell ref="K596:K600"/>
     <mergeCell ref="J610:J611"/>
     <mergeCell ref="I609:I611"/>
+    <mergeCell ref="C629:C630"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Begun Work on Follows test cases
</commit_message>
<xml_diff>
--- a/AutoTester/Tests/System/System Testing Template.xlsx
+++ b/AutoTester/Tests/System/System Testing Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27414" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27417" uniqueCount="507">
   <si>
     <t>such that</t>
   </si>
@@ -1540,6 +1540,12 @@
   <si>
     <t>pl.stmt#=2</t>
   </si>
+  <si>
+    <t>Follows Invalid Case -1</t>
+  </si>
+  <si>
+    <t>Follows Invalid Case 0</t>
+  </si>
 </sst>
 </file>
 
@@ -2157,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1C4663-D304-44C8-B0BF-D228A95395FB}">
   <dimension ref="B3:AY688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B482" workbookViewId="0">
-      <selection activeCell="H684" sqref="H684"/>
+    <sheetView tabSelected="1" topLeftCell="K15" workbookViewId="0">
+      <selection activeCell="AU20" sqref="AU20:AU30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4169,7 +4175,7 @@
       <c r="AT16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU16" s="29" t="s">
+      <c r="AU16" s="18" t="s">
         <v>47</v>
       </c>
       <c r="AV16" s="23"/>
@@ -4306,7 +4312,7 @@
       <c r="AT17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU17" s="29"/>
+      <c r="AU17" s="19"/>
       <c r="AV17" s="23"/>
     </row>
     <row r="18" spans="2:50" ht="15.75" x14ac:dyDescent="0.25">
@@ -4441,7 +4447,9 @@
       <c r="AT18" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU18" s="29"/>
+      <c r="AU18" s="17" t="s">
+        <v>505</v>
+      </c>
       <c r="AV18" s="23"/>
       <c r="AX18" s="6"/>
     </row>
@@ -4577,7 +4585,9 @@
       <c r="AT19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU19" s="29"/>
+      <c r="AU19" s="17" t="s">
+        <v>506</v>
+      </c>
       <c r="AV19" s="23"/>
       <c r="AX19" s="6"/>
     </row>
@@ -4713,7 +4723,9 @@
       <c r="AT20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU20" s="29"/>
+      <c r="AU20" s="18" t="s">
+        <v>47</v>
+      </c>
       <c r="AV20" s="23"/>
       <c r="AX20" s="6"/>
     </row>
@@ -4849,7 +4861,7 @@
       <c r="AT21" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU21" s="29"/>
+      <c r="AU21" s="23"/>
       <c r="AV21" s="23"/>
       <c r="AX21" s="6"/>
     </row>
@@ -4985,7 +4997,7 @@
       <c r="AT22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU22" s="29"/>
+      <c r="AU22" s="23"/>
       <c r="AV22" s="23"/>
       <c r="AX22" s="6"/>
     </row>
@@ -5121,7 +5133,7 @@
       <c r="AT23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU23" s="29"/>
+      <c r="AU23" s="23"/>
       <c r="AV23" s="23"/>
       <c r="AX23" s="6"/>
     </row>
@@ -5259,7 +5271,7 @@
       <c r="AT24" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU24" s="29"/>
+      <c r="AU24" s="23"/>
       <c r="AV24" s="23"/>
       <c r="AX24" s="6"/>
     </row>
@@ -5395,7 +5407,7 @@
       <c r="AT25" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU25" s="29"/>
+      <c r="AU25" s="23"/>
       <c r="AV25" s="23"/>
       <c r="AX25" s="6"/>
     </row>
@@ -5531,7 +5543,7 @@
       <c r="AT26" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU26" s="29"/>
+      <c r="AU26" s="23"/>
       <c r="AV26" s="23"/>
       <c r="AX26" s="6"/>
     </row>
@@ -5667,7 +5679,7 @@
       <c r="AT27" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU27" s="29"/>
+      <c r="AU27" s="23"/>
       <c r="AV27" s="23"/>
       <c r="AX27" s="6"/>
     </row>
@@ -5803,7 +5815,7 @@
       <c r="AT28" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU28" s="29"/>
+      <c r="AU28" s="23"/>
       <c r="AV28" s="23"/>
       <c r="AX28" s="6"/>
     </row>
@@ -5939,7 +5951,7 @@
       <c r="AT29" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU29" s="29"/>
+      <c r="AU29" s="23"/>
       <c r="AV29" s="23"/>
       <c r="AX29" s="6"/>
     </row>
@@ -6075,7 +6087,7 @@
       <c r="AT30" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="AU30" s="29"/>
+      <c r="AU30" s="19"/>
       <c r="AV30" s="23"/>
       <c r="AX30" s="6"/>
     </row>
@@ -92192,7 +92204,7 @@
       <c r="AV688" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="255">
+  <mergeCells count="256">
     <mergeCell ref="N522:N533"/>
     <mergeCell ref="J522:J525"/>
     <mergeCell ref="I522:I527"/>
@@ -92342,7 +92354,6 @@
     <mergeCell ref="V3:V4"/>
     <mergeCell ref="AD3:AD4"/>
     <mergeCell ref="O3:O4"/>
-    <mergeCell ref="AU16:AU30"/>
     <mergeCell ref="AU50:AU64"/>
     <mergeCell ref="AU84:AU96"/>
     <mergeCell ref="J16:J23"/>
@@ -92354,6 +92365,8 @@
     <mergeCell ref="I32:I36"/>
     <mergeCell ref="I66:I70"/>
     <mergeCell ref="J71:J75"/>
+    <mergeCell ref="AU16:AU17"/>
+    <mergeCell ref="AU20:AU30"/>
     <mergeCell ref="L670:L672"/>
     <mergeCell ref="J676:J680"/>
     <mergeCell ref="AV3:AV4"/>

</xml_diff>

<commit_message>
Finished Follows/* Test Cases
</commit_message>
<xml_diff>
--- a/AutoTester/Tests/System/System Testing Template.xlsx
+++ b/AutoTester/Tests/System/System Testing Template.xlsx
@@ -2163,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1C4663-D304-44C8-B0BF-D228A95395FB}">
   <dimension ref="B3:AY688"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K15" workbookViewId="0">
-      <selection activeCell="AU20" sqref="AU20:AU30"/>
+    <sheetView tabSelected="1" topLeftCell="E21" workbookViewId="0">
+      <selection activeCell="J48" sqref="J47:AS48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>